<commit_message>
Refine rise event logic to handle 3 consecutive dips effectively
Updated the logic for handling rise events with 3 consecutive dips, ensuring accurate identification and shifting of rise events to fall when necessary.

- Modified `generate_stock_detailed_analysis.py` to implement the new approach for 3 consecutive dips.
- Adjusted backtest scripts to incorporate the updated rise event logic.
- Updated `blne_rise_volatility_analysis.json` with corrected rise event data.
- Refined data in multiple output files, including `grov_rise_events.xlsx` and `insider_conviction_all_stocks_results.json`.
- Removed outdated temporary file `~$bsfc_rise_events.xlsx`.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -517,15 +517,15 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>7.04</v>
+        <v>35.14</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>62/116</t>
+          <t>25/116</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>7.04</v>
+        <v>35.14</v>
       </c>
       <c r="H2" s="2" t="n"/>
     </row>
@@ -549,15 +549,15 @@
         <v>66</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>-46.3</v>
+        <v>-42</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>10/115</t>
+          <t>14/115</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>-39.26</v>
+        <v>-6.86</v>
       </c>
       <c r="H3" s="3" t="n"/>
     </row>
@@ -581,15 +581,15 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.48</v>
+        <v>17.24</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>112/116</t>
+          <t>49/116</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>-38.78</v>
+        <v>10.38</v>
       </c>
       <c r="H4" s="2" t="n"/>
     </row>
@@ -613,15 +613,15 @@
         <v>22</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>17.8</v>
+        <v>-17.65</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>39/115</t>
+          <t>59/115</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-20.97</v>
+        <v>-7.27</v>
       </c>
       <c r="H5" s="3" t="n"/>
     </row>
@@ -645,15 +645,15 @@
         <v>10</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>27.27</v>
+        <v>30.38</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>20/116</t>
+          <t>28/116</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>6.29</v>
+        <v>23.11</v>
       </c>
       <c r="H6" s="2" t="n"/>
     </row>
@@ -677,15 +677,15 @@
         <v>29</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>3.44</v>
+        <v>-35.28</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>102/115</t>
+          <t>22/115</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>9.74</v>
+        <v>-12.17</v>
       </c>
       <c r="H7" s="3" t="n"/>
     </row>
@@ -709,15 +709,15 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>49.33</v>
+        <v>58.75</v>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>10/116</t>
+          <t>12/116</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>59.07</v>
+        <v>46.58</v>
       </c>
       <c r="H8" s="2" t="n"/>
     </row>
@@ -741,15 +741,15 @@
         <v>9</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>-0.62</v>
+        <v>-8.66</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>111/115</t>
+          <t>95/115</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>58.45</v>
+        <v>37.92</v>
       </c>
       <c r="H9" s="3" t="n"/>
     </row>
@@ -773,15 +773,15 @@
         <v>35</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-26.3</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>21/116</t>
+          <t>68/116</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>32.15</v>
+        <v>49.92</v>
       </c>
       <c r="H10" s="2" t="n"/>
     </row>
@@ -805,15 +805,15 @@
         <v>13</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>-37.7</v>
+        <v>-42.71</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>15/115</t>
+          <t>12/115</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-5.55</v>
+        <v>7.21</v>
       </c>
       <c r="H11" s="3" t="n"/>
     </row>
@@ -837,15 +837,15 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-3.09</v>
+        <v>4.86</v>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>91/116</t>
+          <t>103/116</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>-8.630000000000001</v>
+        <v>12.07</v>
       </c>
       <c r="H12" s="2" t="n"/>
     </row>
@@ -869,15 +869,15 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-11.66</v>
+        <v>-11.95</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>63/115</t>
+          <t>82/115</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
-        <v>-20.3</v>
+        <v>0.12</v>
       </c>
       <c r="H13" s="3" t="n"/>
     </row>
@@ -901,15 +901,15 @@
         <v>11</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>8.779999999999999</v>
+        <v>12.19</v>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>56/116</t>
+          <t>67/116</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>-11.52</v>
+        <v>12.31</v>
       </c>
       <c r="H14" s="2" t="n"/>
     </row>
@@ -933,15 +933,15 @@
         <v>17</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-1.09</v>
+        <v>-5.93</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>108/115</t>
+          <t>106/115</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
-        <v>-12.61</v>
+        <v>6.38</v>
       </c>
       <c r="H15" s="3" t="n"/>
     </row>
@@ -965,7 +965,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-0.4</v>
+        <v>2.78</v>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
@@ -973,7 +973,7 @@
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>-13.02</v>
+        <v>9.16</v>
       </c>
       <c r="H16" s="2" t="n"/>
     </row>
@@ -997,15 +997,15 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>-0.15</v>
+        <v>-3.19</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>114/115</t>
+          <t>112/115</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
-        <v>-13.17</v>
+        <v>5.97</v>
       </c>
       <c r="H17" s="3" t="n"/>
     </row>
@@ -1029,15 +1029,15 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>22.07</v>
+        <v>44.42</v>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>25/116</t>
+          <t>20/116</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>8.9</v>
+        <v>50.38</v>
       </c>
       <c r="H18" s="2" t="n"/>
     </row>
@@ -1061,15 +1061,15 @@
         <v>13</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>-24.29</v>
+        <v>-23.9</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>29/115</t>
+          <t>38/115</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
-        <v>-15.38</v>
+        <v>26.48</v>
       </c>
       <c r="H19" s="3" t="n"/>
     </row>
@@ -1093,15 +1093,15 @@
         <v>11</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>-9.91</v>
+        <v>4.85</v>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>51/116</t>
+          <t>104/116</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>-25.29</v>
+        <v>31.33</v>
       </c>
       <c r="H20" s="2" t="n"/>
     </row>
@@ -1125,15 +1125,15 @@
         <v>13</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>-10.63</v>
+        <v>-14.76</v>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>67/115</t>
+          <t>71/115</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
-        <v>-35.92</v>
+        <v>16.58</v>
       </c>
       <c r="H21" s="3" t="n"/>
     </row>
@@ -1157,15 +1157,15 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>7.9</v>
+        <v>11.45</v>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>60/116</t>
+          <t>69/116</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>-28.03</v>
+        <v>28.03</v>
       </c>
       <c r="H22" s="2" t="n"/>
     </row>
@@ -1189,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>-1.06</v>
+        <v>-3.89</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="G23" s="3" t="n">
-        <v>-29.08</v>
+        <v>24.14</v>
       </c>
       <c r="H23" s="3" t="n"/>
     </row>
@@ -1221,15 +1221,15 @@
         <v>10</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>20.74</v>
+        <v>26.19</v>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>27/116</t>
+          <t>32/116</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>-8.35</v>
+        <v>50.33</v>
       </c>
       <c r="H24" s="2" t="n"/>
     </row>
@@ -1253,15 +1253,15 @@
         <v>17</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>-0.12</v>
+        <v>-6.6</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>115/115</t>
+          <t>101/115</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
-        <v>-8.470000000000001</v>
+        <v>43.72</v>
       </c>
       <c r="H25" s="3" t="n"/>
     </row>
@@ -1285,15 +1285,15 @@
         <v>18</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44.24</v>
+        <v>56.57</v>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>12/116</t>
+          <t>13/116</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>35.78</v>
+        <v>100.29</v>
       </c>
       <c r="H26" s="2" t="n"/>
     </row>
@@ -1317,15 +1317,15 @@
         <v>3</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-4.47</v>
+        <v>-5.94</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>98/115</t>
+          <t>105/115</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>31.31</v>
+        <v>94.34999999999999</v>
       </c>
       <c r="H27" s="3" t="n"/>
     </row>
@@ -1349,15 +1349,15 @@
         <v>14</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-4.63</v>
+        <v>1.92</v>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>78/116</t>
+          <t>115/116</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>26.68</v>
+        <v>96.27</v>
       </c>
       <c r="H28" s="2" t="n"/>
     </row>
@@ -1381,15 +1381,15 @@
         <v>12</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-4.92</v>
+        <v>-11.17</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>94/115</t>
+          <t>86/115</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
-        <v>21.76</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="H29" s="3" t="n"/>
     </row>
@@ -1413,15 +1413,15 @@
         <v>12</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>2.32</v>
+        <v>5.59</v>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>98/116</t>
+          <t>100/116</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>24.09</v>
+        <v>90.69</v>
       </c>
       <c r="H30" s="2" t="n"/>
     </row>
@@ -1445,15 +1445,15 @@
         <v>8</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-1.1</v>
+        <v>-3.19</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>107/115</t>
+          <t>113/115</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
-        <v>22.98</v>
+        <v>87.5</v>
       </c>
       <c r="H31" s="3" t="n"/>
     </row>
@@ -1477,15 +1477,15 @@
         <v>5</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>1.29</v>
+        <v>7.9</v>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>101/116</t>
+          <t>91/116</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>24.28</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="H32" s="2" t="n"/>
     </row>
@@ -1509,15 +1509,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>-7.93</v>
+        <v>-9.73</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>78/115</t>
+          <t>91/115</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
-        <v>16.35</v>
+        <v>85.67</v>
       </c>
       <c r="H33" s="3" t="n"/>
     </row>
@@ -1541,15 +1541,15 @@
         <v>45</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>19.37</v>
+        <v>36.63</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>29/116</t>
+          <t>23/116</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>35.71</v>
+        <v>122.3</v>
       </c>
       <c r="H34" s="2" t="n"/>
     </row>
@@ -1573,15 +1573,15 @@
         <v>7</v>
       </c>
       <c r="E35" s="3" t="n">
-        <v>-11.72</v>
+        <v>-15.14</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>62/115</t>
+          <t>67/115</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>23.99</v>
+        <v>107.16</v>
       </c>
       <c r="H35" s="3" t="n"/>
     </row>
@@ -1605,15 +1605,15 @@
         <v>17</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>-9.31</v>
+        <v>6.37</v>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>53/116</t>
+          <t>97/116</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>14.68</v>
+        <v>113.53</v>
       </c>
       <c r="H36" s="2" t="n"/>
     </row>
@@ -1637,15 +1637,15 @@
         <v>4</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>-14.27</v>
+        <v>-14.97</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>56/115</t>
+          <t>69/115</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>0.42</v>
+        <v>98.56</v>
       </c>
       <c r="H37" s="3" t="n"/>
     </row>
@@ -1669,15 +1669,15 @@
         <v>59</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>8.300000000000001</v>
+        <v>20.99</v>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>59/116</t>
+          <t>43/116</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>8.720000000000001</v>
+        <v>119.55</v>
       </c>
       <c r="H38" s="2" t="n"/>
     </row>
@@ -1701,15 +1701,15 @@
         <v>3</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>-9.01</v>
+        <v>-11.64</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>73/115</t>
+          <t>83/115</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>-0.29</v>
+        <v>107.91</v>
       </c>
       <c r="H39" s="3" t="n"/>
     </row>
@@ -1733,15 +1733,15 @@
         <v>5</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>6.25</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>67/116</t>
+          <t>88/116</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>5.96</v>
+        <v>115.94</v>
       </c>
       <c r="H40" s="2" t="n"/>
     </row>
@@ -1765,15 +1765,15 @@
         <v>13</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>-4.87</v>
+        <v>-6.71</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>95/115</t>
+          <t>100/115</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>1.09</v>
+        <v>109.24</v>
       </c>
       <c r="H41" s="3" t="n"/>
     </row>
@@ -1797,15 +1797,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>2.06</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>99/116</t>
+          <t>78/116</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>3.15</v>
+        <v>118.85</v>
       </c>
       <c r="H42" s="2" t="n"/>
     </row>
@@ -1829,15 +1829,15 @@
         <v>13</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>-25.46</v>
+        <v>-28.32</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>27/115</t>
+          <t>30/115</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>-22.31</v>
+        <v>90.53</v>
       </c>
       <c r="H43" s="3" t="n"/>
     </row>
@@ -1861,15 +1861,15 @@
         <v>10</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>4.4</v>
+        <v>6.45</v>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>80/116</t>
+          <t>96/116</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>-17.91</v>
+        <v>96.98</v>
       </c>
       <c r="H44" s="2" t="n"/>
     </row>
@@ -1893,15 +1893,15 @@
         <v>9</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>-4.55</v>
+        <v>-4.81</v>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>97/115</t>
+          <t>109/115</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>-22.46</v>
+        <v>92.16</v>
       </c>
       <c r="H45" s="3" t="n"/>
     </row>
@@ -1925,15 +1925,15 @@
         <v>40</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>-1</v>
+        <v>4.57</v>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>104/116</t>
+          <t>107/116</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>-23.46</v>
+        <v>96.73</v>
       </c>
       <c r="H46" s="2" t="n"/>
     </row>
@@ -1957,15 +1957,15 @@
         <v>43</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>-10.69</v>
+        <v>-12.32</v>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>66/115</t>
+          <t>79/115</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>-34.15</v>
+        <v>84.41</v>
       </c>
       <c r="H47" s="3" t="n"/>
     </row>
@@ -1989,15 +1989,15 @@
         <v>14</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>4.45</v>
+        <v>9.07</v>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>79/116</t>
+          <t>81/116</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>-29.69</v>
+        <v>93.48</v>
       </c>
       <c r="H48" s="2" t="n"/>
     </row>
@@ -2021,15 +2021,15 @@
         <v>5</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>-4.57</v>
+        <v>-5.38</v>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>96/115</t>
+          <t>108/115</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>-34.26</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="H49" s="3" t="n"/>
     </row>
@@ -2053,15 +2053,15 @@
         <v>14</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>2.59</v>
+        <v>6.03</v>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>96/116</t>
+          <t>99/116</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>-31.67</v>
+        <v>94.13</v>
       </c>
       <c r="H50" s="2" t="n"/>
     </row>
@@ -2085,15 +2085,15 @@
         <v>12</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-3.19</v>
+        <v>-6.02</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>103/115</t>
+          <t>104/115</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>-34.85</v>
+        <v>88.12</v>
       </c>
       <c r="H51" s="3" t="n"/>
     </row>
@@ -2117,15 +2117,15 @@
         <v>8</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>-0.9399999999999999</v>
+        <v>4.67</v>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>106/116</t>
+          <t>105/116</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>-35.79</v>
+        <v>92.79000000000001</v>
       </c>
       <c r="H52" s="2" t="n"/>
     </row>
@@ -2149,15 +2149,15 @@
         <v>6</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>-5.69</v>
+        <v>-6.78</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>90/115</t>
+          <t>99/115</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>-41.49</v>
+        <v>86.01000000000001</v>
       </c>
       <c r="H53" s="3" t="n"/>
     </row>
@@ -2181,15 +2181,15 @@
         <v>2</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>-10.94</v>
+        <v>3.72</v>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>44/116</t>
+          <t>111/116</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>-52.43</v>
+        <v>89.73</v>
       </c>
       <c r="H54" s="2" t="n"/>
     </row>
@@ -2213,15 +2213,15 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>-16.4</v>
+        <v>-16.92</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>47/115</t>
+          <t>62/115</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>-68.83</v>
+        <v>72.81</v>
       </c>
       <c r="H55" s="3" t="n"/>
     </row>
@@ -2245,15 +2245,15 @@
         <v>2</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>-6.15</v>
+        <v>2.88</v>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>70/116</t>
+          <t>113/116</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>-74.98</v>
+        <v>75.69</v>
       </c>
       <c r="H56" s="2" t="n"/>
     </row>
@@ -2277,15 +2277,15 @@
         <v>7</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>-7.9</v>
+        <v>-9</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>79/115</t>
+          <t>93/115</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>-82.88</v>
+        <v>66.69</v>
       </c>
       <c r="H57" s="3" t="n"/>
     </row>
@@ -2309,15 +2309,15 @@
         <v>6</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>-0.8</v>
+        <v>5.49</v>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>110/116</t>
+          <t>101/116</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>-83.68000000000001</v>
+        <v>72.19</v>
       </c>
       <c r="H58" s="2" t="n"/>
     </row>
@@ -2341,15 +2341,15 @@
         <v>11</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>-9.960000000000001</v>
+        <v>-12.92</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>70/115</t>
+          <t>76/115</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>-93.64</v>
+        <v>59.27</v>
       </c>
       <c r="H59" s="3" t="n"/>
     </row>
@@ -2373,15 +2373,15 @@
         <v>4</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>0.96</v>
+        <v>8.85</v>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>105/116</t>
+          <t>83/116</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>-92.68000000000001</v>
+        <v>68.12</v>
       </c>
       <c r="H60" s="2" t="n"/>
     </row>
@@ -2405,15 +2405,15 @@
         <v>2</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>-3.64</v>
+        <v>-7.69</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>101/115</t>
+          <t>97/115</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>-96.31999999999999</v>
+        <v>60.43</v>
       </c>
       <c r="H61" s="3" t="n"/>
     </row>
@@ -2437,15 +2437,15 @@
         <v>5</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>6.18</v>
+        <v>8.33</v>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>69/116</t>
+          <t>86/116</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>-90.15000000000001</v>
+        <v>68.76000000000001</v>
       </c>
       <c r="H62" s="2" t="n"/>
     </row>
@@ -2469,15 +2469,15 @@
         <v>22</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>-6.86</v>
+        <v>-19.12</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>82/115</t>
+          <t>51/115</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>-97.01000000000001</v>
+        <v>49.64</v>
       </c>
       <c r="H63" s="3" t="n"/>
     </row>
@@ -2501,15 +2501,15 @@
         <v>13</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>2.76</v>
+        <v>8.859999999999999</v>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>95/116</t>
+          <t>82/116</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>-94.25</v>
+        <v>58.5</v>
       </c>
       <c r="H64" s="2" t="n"/>
     </row>
@@ -2533,15 +2533,15 @@
         <v>7</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>-6.79</v>
+        <v>-6.98</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>84/115</t>
+          <t>98/115</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>-101.04</v>
+        <v>51.52</v>
       </c>
       <c r="H65" s="3" t="n"/>
     </row>
@@ -2565,7 +2565,7 @@
         <v>30</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>21.81</v>
+        <v>32.25</v>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
@@ -2573,7 +2573,7 @@
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>-79.22</v>
+        <v>83.77</v>
       </c>
       <c r="H66" s="2" t="n"/>
     </row>
@@ -2597,15 +2597,15 @@
         <v>16</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>-12.51</v>
+        <v>-12.48</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>58/115</t>
+          <t>78/115</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>-91.73999999999999</v>
+        <v>71.3</v>
       </c>
       <c r="H67" s="3" t="n"/>
     </row>
@@ -2629,15 +2629,15 @@
         <v>19</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>7</v>
+        <v>7.99</v>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>64/116</t>
+          <t>89/116</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>-84.73</v>
+        <v>79.29000000000001</v>
       </c>
       <c r="H68" s="2" t="n"/>
     </row>
@@ -2661,15 +2661,15 @@
         <v>34</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>-38.66</v>
+        <v>-42.4</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>14/115</t>
+          <t>13/115</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>-123.39</v>
+        <v>36.89</v>
       </c>
       <c r="H69" s="3" t="n"/>
     </row>
@@ -2693,15 +2693,15 @@
         <v>14</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>-12.16</v>
+        <v>3.15</v>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>38/116</t>
+          <t>112/116</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>-135.56</v>
+        <v>40.04</v>
       </c>
       <c r="H70" s="2" t="n"/>
     </row>
@@ -2725,15 +2725,15 @@
         <v>6</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>-16.56</v>
+        <v>-20.18</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>46/115</t>
+          <t>49/115</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>-152.12</v>
+        <v>19.86</v>
       </c>
       <c r="H71" s="3" t="n"/>
     </row>
@@ -2757,15 +2757,15 @@
         <v>4</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>15.36</v>
+        <v>26.05</v>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>32/116</t>
+          <t>34/116</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>-136.76</v>
+        <v>45.91</v>
       </c>
       <c r="H72" s="2" t="n"/>
     </row>
@@ -2789,15 +2789,15 @@
         <v>8</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>-5.25</v>
+        <v>-10.33</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>93/115</t>
+          <t>89/115</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>-142.01</v>
+        <v>35.58</v>
       </c>
       <c r="H73" s="3" t="n"/>
     </row>
@@ -2821,15 +2821,15 @@
         <v>6</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>8.44</v>
+        <v>15.59</v>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>57/116</t>
+          <t>60/116</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>-133.57</v>
+        <v>51.17</v>
       </c>
       <c r="H74" s="2" t="n"/>
     </row>
@@ -2853,15 +2853,15 @@
         <v>14</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>2.37</v>
+        <v>-10.85</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>105/115</t>
+          <t>87/115</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>-131.21</v>
+        <v>40.32</v>
       </c>
       <c r="H75" s="3" t="n"/>
     </row>
@@ -2885,15 +2885,15 @@
         <v>9</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>15.1</v>
+        <v>21.36</v>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>33/116</t>
+          <t>41/116</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>-116.11</v>
+        <v>61.68</v>
       </c>
       <c r="H76" s="2" t="n"/>
     </row>
@@ -2917,15 +2917,15 @@
         <v>5</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>-3.91</v>
+        <v>-5.6</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>100/115</t>
+          <t>107/115</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>-120.01</v>
+        <v>56.08</v>
       </c>
       <c r="H77" s="3" t="n"/>
     </row>
@@ -2949,15 +2949,15 @@
         <v>7</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>1.23</v>
+        <v>4.52</v>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>102/116</t>
+          <t>108/116</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>-118.78</v>
+        <v>60.6</v>
       </c>
       <c r="H78" s="2" t="n"/>
     </row>
@@ -2981,15 +2981,15 @@
         <v>49</v>
       </c>
       <c r="E79" s="3" t="n">
-        <v>-117.85</v>
+        <v>-72.97</v>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>1/115</t>
+          <t>2/115</t>
         </is>
       </c>
       <c r="G79" s="3" t="n">
-        <v>-236.63</v>
+        <v>-12.37</v>
       </c>
       <c r="H79" s="3" t="n"/>
     </row>
@@ -3013,15 +3013,15 @@
         <v>27</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>65.98</v>
+        <v>100</v>
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>6/116</t>
+          <t>5/116</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
-        <v>-170.65</v>
+        <v>87.63</v>
       </c>
       <c r="H80" s="2" t="n"/>
     </row>
@@ -3045,15 +3045,15 @@
         <v>5</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>-5.63</v>
+        <v>-9.5</v>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>91/115</t>
+          <t>92/115</t>
         </is>
       </c>
       <c r="G81" s="3" t="n">
-        <v>-176.28</v>
+        <v>78.13</v>
       </c>
       <c r="H81" s="3" t="n"/>
     </row>
@@ -3077,15 +3077,15 @@
         <v>9</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>-1.16</v>
+        <v>6.63</v>
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>103/116</t>
+          <t>95/116</t>
         </is>
       </c>
       <c r="G82" s="2" t="n">
-        <v>-177.44</v>
+        <v>84.76000000000001</v>
       </c>
       <c r="H82" s="2" t="n"/>
     </row>
@@ -3109,15 +3109,15 @@
         <v>18</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>-26.03</v>
+        <v>-27.46</v>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>25/115</t>
+          <t>31/115</t>
         </is>
       </c>
       <c r="G83" s="3" t="n">
-        <v>-203.46</v>
+        <v>57.3</v>
       </c>
       <c r="H83" s="3" t="n"/>
     </row>
@@ -3141,15 +3141,15 @@
         <v>7</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>-0.18</v>
+        <v>23.57</v>
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>115/116</t>
+          <t>39/116</t>
         </is>
       </c>
       <c r="G84" s="2" t="n">
-        <v>-203.64</v>
+        <v>80.87</v>
       </c>
       <c r="H84" s="2" t="n"/>
     </row>
@@ -3173,7 +3173,7 @@
         <v>8</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>-16.98</v>
+        <v>-21.39</v>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
@@ -3181,7 +3181,7 @@
         </is>
       </c>
       <c r="G85" s="3" t="n">
-        <v>-220.61</v>
+        <v>59.48</v>
       </c>
       <c r="H85" s="3" t="n"/>
     </row>
@@ -3205,15 +3205,15 @@
         <v>6</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>3.57</v>
+        <v>12.87</v>
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>86/116</t>
+          <t>65/116</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
-        <v>-217.04</v>
+        <v>72.34999999999999</v>
       </c>
       <c r="H86" s="2" t="n"/>
     </row>
@@ -3237,15 +3237,15 @@
         <v>7</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>-18.71</v>
+        <v>-18.57</v>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>36/115</t>
+          <t>54/115</t>
         </is>
       </c>
       <c r="G87" s="3" t="n">
-        <v>-235.75</v>
+        <v>53.78</v>
       </c>
       <c r="H87" s="3" t="n"/>
     </row>
@@ -3269,15 +3269,15 @@
         <v>13</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>-5.89</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>72/116</t>
+          <t>84/116</t>
         </is>
       </c>
       <c r="G88" s="2" t="n">
-        <v>-241.64</v>
+        <v>62.58</v>
       </c>
       <c r="H88" s="2" t="n"/>
     </row>
@@ -3301,15 +3301,15 @@
         <v>6</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>-14.12</v>
+        <v>-20.59</v>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>57/115</t>
+          <t>46/115</t>
         </is>
       </c>
       <c r="G89" s="3" t="n">
-        <v>-255.76</v>
+        <v>41.99</v>
       </c>
       <c r="H89" s="3" t="n"/>
     </row>
@@ -3333,15 +3333,15 @@
         <v>8</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>6.23</v>
+        <v>17.12</v>
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>68/116</t>
+          <t>51/116</t>
         </is>
       </c>
       <c r="G90" s="2" t="n">
-        <v>-249.54</v>
+        <v>59.11</v>
       </c>
       <c r="H90" s="2" t="n"/>
     </row>
@@ -3365,15 +3365,15 @@
         <v>5</v>
       </c>
       <c r="E91" s="3" t="n">
-        <v>-9.91</v>
+        <v>-10.77</v>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>71/115</t>
+          <t>88/115</t>
         </is>
       </c>
       <c r="G91" s="3" t="n">
-        <v>-259.45</v>
+        <v>48.34</v>
       </c>
       <c r="H91" s="3" t="n"/>
     </row>
@@ -3397,15 +3397,15 @@
         <v>13</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>26.29</v>
+        <v>53.45</v>
       </c>
       <c r="F92" s="2" t="inlineStr">
         <is>
-          <t>22/116</t>
+          <t>15/116</t>
         </is>
       </c>
       <c r="G92" s="2" t="n">
-        <v>-233.15</v>
+        <v>101.79</v>
       </c>
       <c r="H92" s="2" t="n"/>
     </row>
@@ -3429,15 +3429,15 @@
         <v>36</v>
       </c>
       <c r="E93" s="3" t="n">
-        <v>-43.99</v>
+        <v>-39.89</v>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>12/115</t>
+          <t>18/115</t>
         </is>
       </c>
       <c r="G93" s="3" t="n">
-        <v>-277.14</v>
+        <v>61.9</v>
       </c>
       <c r="H93" s="3" t="n"/>
     </row>
@@ -3461,15 +3461,15 @@
         <v>13</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>9.1</v>
+        <v>14.02</v>
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>54/116</t>
+          <t>62/116</t>
         </is>
       </c>
       <c r="G94" s="2" t="n">
-        <v>-268.04</v>
+        <v>75.92</v>
       </c>
       <c r="H94" s="2" t="n"/>
     </row>
@@ -3493,15 +3493,15 @@
         <v>5</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>0.36</v>
+        <v>-6.56</v>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>113/115</t>
+          <t>102/115</t>
         </is>
       </c>
       <c r="G95" s="3" t="n">
-        <v>-267.68</v>
+        <v>69.36</v>
       </c>
       <c r="H95" s="3" t="n"/>
     </row>
@@ -3525,15 +3525,15 @@
         <v>2</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>11.01</v>
+        <v>15.79</v>
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>42/116</t>
+          <t>58/116</t>
         </is>
       </c>
       <c r="G96" s="2" t="n">
-        <v>-256.67</v>
+        <v>85.15000000000001</v>
       </c>
       <c r="H96" s="2" t="n"/>
     </row>
@@ -3557,15 +3557,15 @@
         <v>12</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.5600000000000001</v>
+        <v>-6.06</v>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>112/115</t>
+          <t>103/115</t>
         </is>
       </c>
       <c r="G97" s="3" t="n">
-        <v>-256.11</v>
+        <v>79.09</v>
       </c>
       <c r="H97" s="3" t="n"/>
     </row>
@@ -3589,7 +3589,7 @@
         <v>14</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>36.43</v>
+        <v>53.23</v>
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="G98" s="2" t="n">
-        <v>-219.68</v>
+        <v>132.32</v>
       </c>
       <c r="H98" s="2" t="n"/>
     </row>
@@ -3621,15 +3621,15 @@
         <v>8</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>-17.41</v>
+        <v>-20.53</v>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>40/115</t>
+          <t>47/115</t>
         </is>
       </c>
       <c r="G99" s="3" t="n">
-        <v>-237.09</v>
+        <v>111.79</v>
       </c>
       <c r="H99" s="3" t="n"/>
     </row>
@@ -3653,15 +3653,15 @@
         <v>7</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>-6.89</v>
+        <v>8.44</v>
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>65/116</t>
+          <t>85/116</t>
         </is>
       </c>
       <c r="G100" s="2" t="n">
-        <v>-243.98</v>
+        <v>120.23</v>
       </c>
       <c r="H100" s="2" t="n"/>
     </row>
@@ -3685,15 +3685,15 @@
         <v>23</v>
       </c>
       <c r="E101" s="3" t="n">
-        <v>-27.45</v>
+        <v>-25.75</v>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>22/115</t>
+          <t>34/115</t>
         </is>
       </c>
       <c r="G101" s="3" t="n">
-        <v>-271.43</v>
+        <v>94.48999999999999</v>
       </c>
       <c r="H101" s="3" t="n"/>
     </row>
@@ -3717,15 +3717,15 @@
         <v>56</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>71.09</v>
+        <v>120.16</v>
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>4/116</t>
+          <t>3/116</t>
         </is>
       </c>
       <c r="G102" s="2" t="n">
-        <v>-200.34</v>
+        <v>214.65</v>
       </c>
       <c r="H102" s="2" t="n"/>
     </row>
@@ -3749,15 +3749,15 @@
         <v>8</v>
       </c>
       <c r="E103" s="3" t="n">
-        <v>-34.22</v>
+        <v>-32.6</v>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>16/115</t>
+          <t>25/115</t>
         </is>
       </c>
       <c r="G103" s="3" t="n">
-        <v>-234.56</v>
+        <v>182.05</v>
       </c>
       <c r="H103" s="3" t="n"/>
     </row>
@@ -3781,15 +3781,15 @@
         <v>17</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>5.98</v>
+        <v>11.41</v>
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>71/116</t>
+          <t>70/116</t>
         </is>
       </c>
       <c r="G104" s="2" t="n">
-        <v>-228.58</v>
+        <v>193.46</v>
       </c>
       <c r="H104" s="2" t="n"/>
     </row>
@@ -3813,15 +3813,15 @@
         <v>8</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>-12.39</v>
+        <v>-13.66</v>
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>59/115</t>
+          <t>73/115</t>
         </is>
       </c>
       <c r="G105" s="3" t="n">
-        <v>-240.97</v>
+        <v>179.8</v>
       </c>
       <c r="H105" s="3" t="n"/>
     </row>
@@ -3845,15 +3845,15 @@
         <v>13</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>-4.3</v>
+        <v>15.82</v>
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>81/116</t>
+          <t>57/116</t>
         </is>
       </c>
       <c r="G106" s="2" t="n">
-        <v>-245.27</v>
+        <v>195.62</v>
       </c>
       <c r="H106" s="2" t="n"/>
     </row>
@@ -3877,15 +3877,15 @@
         <v>13</v>
       </c>
       <c r="E107" s="3" t="n">
-        <v>-15.7</v>
+        <v>-22.93</v>
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>51/115</t>
+          <t>40/115</t>
         </is>
       </c>
       <c r="G107" s="3" t="n">
-        <v>-260.97</v>
+        <v>172.69</v>
       </c>
       <c r="H107" s="3" t="n"/>
     </row>
@@ -3909,15 +3909,15 @@
         <v>3</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>11.44</v>
+        <v>15.82</v>
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>40/116</t>
+          <t>56/116</t>
         </is>
       </c>
       <c r="G108" s="2" t="n">
-        <v>-249.53</v>
+        <v>188.52</v>
       </c>
       <c r="H108" s="2" t="n"/>
     </row>
@@ -3941,15 +3941,15 @@
         <v>10</v>
       </c>
       <c r="E109" s="3" t="n">
-        <v>-5.79</v>
+        <v>-8.74</v>
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>89/115</t>
+          <t>94/115</t>
         </is>
       </c>
       <c r="G109" s="3" t="n">
-        <v>-255.32</v>
+        <v>179.77</v>
       </c>
       <c r="H109" s="3" t="n"/>
     </row>
@@ -3973,15 +3973,15 @@
         <v>32</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>62.57</v>
+        <v>91.62</v>
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>7/116</t>
+          <t>6/116</t>
         </is>
       </c>
       <c r="G110" s="2" t="n">
-        <v>-192.75</v>
+        <v>271.39</v>
       </c>
       <c r="H110" s="2" t="n"/>
     </row>
@@ -4005,15 +4005,15 @@
         <v>14</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>-5.55</v>
+        <v>-12.19</v>
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>92/115</t>
+          <t>81/115</t>
         </is>
       </c>
       <c r="G111" s="3" t="n">
-        <v>-198.3</v>
+        <v>259.2</v>
       </c>
       <c r="H111" s="3" t="n"/>
     </row>
@@ -4037,15 +4037,15 @@
         <v>2</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>3.88</v>
+        <v>7.75</v>
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>82/116</t>
+          <t>92/116</t>
         </is>
       </c>
       <c r="G112" s="2" t="n">
-        <v>-194.42</v>
+        <v>266.95</v>
       </c>
       <c r="H112" s="2" t="n"/>
     </row>
@@ -4069,15 +4069,15 @@
         <v>5</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>-7.65</v>
+        <v>-7.84</v>
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>80/115</t>
+          <t>96/115</t>
         </is>
       </c>
       <c r="G113" s="3" t="n">
-        <v>-202.06</v>
+        <v>259.1</v>
       </c>
       <c r="H113" s="3" t="n"/>
     </row>
@@ -4101,15 +4101,15 @@
         <v>13</v>
       </c>
       <c r="E114" s="2" t="n">
-        <v>24.47</v>
+        <v>30.14</v>
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>23/116</t>
+          <t>29/116</t>
         </is>
       </c>
       <c r="G114" s="2" t="n">
-        <v>-177.6</v>
+        <v>289.25</v>
       </c>
       <c r="H114" s="2" t="n"/>
     </row>
@@ -4133,15 +4133,15 @@
         <v>2</v>
       </c>
       <c r="E115" s="3" t="n">
-        <v>6.06</v>
+        <v>-3.54</v>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>88/115</t>
+          <t>111/115</t>
         </is>
       </c>
       <c r="G115" s="3" t="n">
-        <v>-171.53</v>
+        <v>285.7</v>
       </c>
       <c r="H115" s="3" t="n"/>
     </row>
@@ -4165,15 +4165,15 @@
         <v>13</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>11.72</v>
+        <v>31.92</v>
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t>39/116</t>
+          <t>27/116</t>
         </is>
       </c>
       <c r="G116" s="2" t="n">
-        <v>-159.81</v>
+        <v>317.63</v>
       </c>
       <c r="H116" s="2" t="n"/>
     </row>
@@ -4197,15 +4197,15 @@
         <v>4</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>-16</v>
+        <v>-18.63</v>
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>49/115</t>
+          <t>53/115</t>
         </is>
       </c>
       <c r="G117" s="3" t="n">
-        <v>-175.81</v>
+        <v>299</v>
       </c>
       <c r="H117" s="3" t="n"/>
     </row>
@@ -4229,15 +4229,15 @@
         <v>6</v>
       </c>
       <c r="E118" s="2" t="n">
-        <v>-9.06</v>
+        <v>4.21</v>
       </c>
       <c r="F118" s="2" t="inlineStr">
         <is>
-          <t>55/116</t>
+          <t>109/116</t>
         </is>
       </c>
       <c r="G118" s="2" t="n">
-        <v>-184.87</v>
+        <v>303.21</v>
       </c>
       <c r="H118" s="2" t="n"/>
     </row>
@@ -4261,7 +4261,7 @@
         <v>13</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>-21.62</v>
+        <v>-27.02</v>
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
@@ -4269,7 +4269,7 @@
         </is>
       </c>
       <c r="G119" s="3" t="n">
-        <v>-206.49</v>
+        <v>276.19</v>
       </c>
       <c r="H119" s="3" t="n"/>
     </row>
@@ -4293,15 +4293,15 @@
         <v>32</v>
       </c>
       <c r="E120" s="2" t="n">
-        <v>-12.33</v>
+        <v>9.34</v>
       </c>
       <c r="F120" s="2" t="inlineStr">
         <is>
-          <t>37/116</t>
+          <t>79/116</t>
         </is>
       </c>
       <c r="G120" s="2" t="n">
-        <v>-218.82</v>
+        <v>285.53</v>
       </c>
       <c r="H120" s="2" t="n"/>
     </row>
@@ -4325,15 +4325,15 @@
         <v>9</v>
       </c>
       <c r="E121" s="3" t="n">
-        <v>-17.29</v>
+        <v>-20.89</v>
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>41/115</t>
+          <t>44/115</t>
         </is>
       </c>
       <c r="G121" s="3" t="n">
-        <v>-236.11</v>
+        <v>264.64</v>
       </c>
       <c r="H121" s="3" t="n"/>
     </row>
@@ -4357,15 +4357,15 @@
         <v>20</v>
       </c>
       <c r="E122" s="2" t="n">
-        <v>8.31</v>
+        <v>16.4</v>
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>58/116</t>
+          <t>53/116</t>
         </is>
       </c>
       <c r="G122" s="2" t="n">
-        <v>-227.8</v>
+        <v>281.04</v>
       </c>
       <c r="H122" s="2" t="n"/>
     </row>
@@ -4389,15 +4389,15 @@
         <v>9</v>
       </c>
       <c r="E123" s="3" t="n">
-        <v>-6.37</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>87/115</t>
+          <t>90/115</t>
         </is>
       </c>
       <c r="G123" s="3" t="n">
-        <v>-234.17</v>
+        <v>271.08</v>
       </c>
       <c r="H123" s="3" t="n"/>
     </row>
@@ -4421,15 +4421,15 @@
         <v>7</v>
       </c>
       <c r="E124" s="2" t="n">
-        <v>-28.42</v>
+        <v>9.92</v>
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>18/116</t>
+          <t>74/116</t>
         </is>
       </c>
       <c r="G124" s="2" t="n">
-        <v>-262.6</v>
+        <v>281</v>
       </c>
       <c r="H124" s="2" t="n"/>
     </row>
@@ -4453,15 +4453,15 @@
         <v>7</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>-29.49</v>
+        <v>-33.68</v>
       </c>
       <c r="F125" s="3" t="inlineStr">
         <is>
-          <t>19/115</t>
+          <t>24/115</t>
         </is>
       </c>
       <c r="G125" s="3" t="n">
-        <v>-292.09</v>
+        <v>247.32</v>
       </c>
       <c r="H125" s="3" t="n"/>
     </row>
@@ -4485,15 +4485,15 @@
         <v>3</v>
       </c>
       <c r="E126" s="2" t="n">
-        <v>-10.33</v>
+        <v>6.28</v>
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>48/116</t>
+          <t>98/116</t>
         </is>
       </c>
       <c r="G126" s="2" t="n">
-        <v>-302.42</v>
+        <v>253.6</v>
       </c>
       <c r="H126" s="2" t="n"/>
     </row>
@@ -4517,15 +4517,15 @@
         <v>7</v>
       </c>
       <c r="E127" s="3" t="n">
-        <v>-10.5</v>
+        <v>-15.76</v>
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>68/115</t>
+          <t>65/115</t>
         </is>
       </c>
       <c r="G127" s="3" t="n">
-        <v>-312.92</v>
+        <v>237.84</v>
       </c>
       <c r="H127" s="3" t="n"/>
     </row>
@@ -4549,15 +4549,15 @@
         <v>21</v>
       </c>
       <c r="E128" s="2" t="n">
-        <v>12.81</v>
+        <v>20.47</v>
       </c>
       <c r="F128" s="2" t="inlineStr">
         <is>
-          <t>36/116</t>
+          <t>44/116</t>
         </is>
       </c>
       <c r="G128" s="2" t="n">
-        <v>-300.11</v>
+        <v>258.31</v>
       </c>
       <c r="H128" s="2" t="n"/>
     </row>
@@ -4581,15 +4581,15 @@
         <v>32</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>-48.66</v>
+        <v>-51.46</v>
       </c>
       <c r="F129" s="3" t="inlineStr">
         <is>
-          <t>8/115</t>
+          <t>6/115</t>
         </is>
       </c>
       <c r="G129" s="3" t="n">
-        <v>-348.77</v>
+        <v>206.85</v>
       </c>
       <c r="H129" s="3" t="n"/>
     </row>
@@ -4613,15 +4613,15 @@
         <v>19</v>
       </c>
       <c r="E130" s="2" t="n">
-        <v>3.04</v>
+        <v>21</v>
       </c>
       <c r="F130" s="2" t="inlineStr">
         <is>
-          <t>92/116</t>
+          <t>42/116</t>
         </is>
       </c>
       <c r="G130" s="2" t="n">
-        <v>-345.73</v>
+        <v>227.85</v>
       </c>
       <c r="H130" s="2" t="n"/>
     </row>
@@ -4645,15 +4645,15 @@
         <v>7</v>
       </c>
       <c r="E131" s="3" t="n">
-        <v>-12.02</v>
+        <v>-20.66</v>
       </c>
       <c r="F131" s="3" t="inlineStr">
         <is>
-          <t>60/115</t>
+          <t>45/115</t>
         </is>
       </c>
       <c r="G131" s="3" t="n">
-        <v>-357.75</v>
+        <v>207.19</v>
       </c>
       <c r="H131" s="3" t="n"/>
     </row>
@@ -4677,15 +4677,15 @@
         <v>4</v>
       </c>
       <c r="E132" s="2" t="n">
-        <v>-2.35</v>
+        <v>13.54</v>
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>97/116</t>
+          <t>63/116</t>
         </is>
       </c>
       <c r="G132" s="2" t="n">
-        <v>-360.09</v>
+        <v>220.73</v>
       </c>
       <c r="H132" s="2" t="n"/>
     </row>
@@ -4709,15 +4709,15 @@
         <v>15</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>-15.12</v>
+        <v>-18.35</v>
       </c>
       <c r="F133" s="3" t="inlineStr">
         <is>
-          <t>52/115</t>
+          <t>56/115</t>
         </is>
       </c>
       <c r="G133" s="3" t="n">
-        <v>-375.21</v>
+        <v>202.38</v>
       </c>
       <c r="H133" s="3" t="n"/>
     </row>
@@ -4741,15 +4741,15 @@
         <v>23</v>
       </c>
       <c r="E134" s="2" t="n">
-        <v>16.91</v>
+        <v>51.69</v>
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>30/116</t>
+          <t>18/116</t>
         </is>
       </c>
       <c r="G134" s="2" t="n">
-        <v>-358.31</v>
+        <v>254.07</v>
       </c>
       <c r="H134" s="2" t="inlineStr">
         <is>
@@ -4777,15 +4777,15 @@
         <v>17</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>-31.63</v>
+        <v>-35.56</v>
       </c>
       <c r="F135" s="3" t="inlineStr">
         <is>
-          <t>18/115</t>
+          <t>21/115</t>
         </is>
       </c>
       <c r="G135" s="3" t="n">
-        <v>-389.94</v>
+        <v>218.51</v>
       </c>
       <c r="H135" s="3" t="n"/>
     </row>
@@ -4809,15 +4809,15 @@
         <v>4</v>
       </c>
       <c r="E136" s="2" t="n">
-        <v>-14.72</v>
+        <v>5.13</v>
       </c>
       <c r="F136" s="2" t="inlineStr">
         <is>
-          <t>34/116</t>
+          <t>102/116</t>
         </is>
       </c>
       <c r="G136" s="2" t="n">
-        <v>-404.66</v>
+        <v>223.64</v>
       </c>
       <c r="H136" s="2" t="n"/>
     </row>
@@ -4841,15 +4841,15 @@
         <v>28</v>
       </c>
       <c r="E137" s="3" t="n">
-        <v>-29.08</v>
+        <v>-31.46</v>
       </c>
       <c r="F137" s="3" t="inlineStr">
         <is>
-          <t>20/115</t>
+          <t>27/115</t>
         </is>
       </c>
       <c r="G137" s="3" t="n">
-        <v>-433.74</v>
+        <v>192.18</v>
       </c>
       <c r="H137" s="3" t="n"/>
     </row>
@@ -4873,15 +4873,15 @@
         <v>9</v>
       </c>
       <c r="E138" s="2" t="n">
-        <v>-10.42</v>
+        <v>7.35</v>
       </c>
       <c r="F138" s="2" t="inlineStr">
         <is>
-          <t>47/116</t>
+          <t>93/116</t>
         </is>
       </c>
       <c r="G138" s="2" t="n">
-        <v>-444.16</v>
+        <v>199.53</v>
       </c>
       <c r="H138" s="2" t="n"/>
     </row>
@@ -4905,15 +4905,15 @@
         <v>11</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>-8.43</v>
+        <v>-17.81</v>
       </c>
       <c r="F139" s="3" t="inlineStr">
         <is>
-          <t>76/115</t>
+          <t>58/115</t>
         </is>
       </c>
       <c r="G139" s="3" t="n">
-        <v>-452.59</v>
+        <v>181.72</v>
       </c>
       <c r="H139" s="3" t="n"/>
     </row>
@@ -4937,15 +4937,15 @@
         <v>3</v>
       </c>
       <c r="E140" s="2" t="n">
-        <v>5.14</v>
+        <v>19.16</v>
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>75/116</t>
+          <t>45/116</t>
         </is>
       </c>
       <c r="G140" s="2" t="n">
-        <v>-447.45</v>
+        <v>200.89</v>
       </c>
       <c r="H140" s="2" t="n"/>
     </row>
@@ -4969,15 +4969,15 @@
         <v>9</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>-15.02</v>
+        <v>-16.35</v>
       </c>
       <c r="F141" s="3" t="inlineStr">
         <is>
-          <t>53/115</t>
+          <t>64/115</t>
         </is>
       </c>
       <c r="G141" s="3" t="n">
-        <v>-462.47</v>
+        <v>184.54</v>
       </c>
       <c r="H141" s="3" t="n"/>
     </row>
@@ -5001,15 +5001,15 @@
         <v>14</v>
       </c>
       <c r="E142" s="2" t="n">
-        <v>10.18</v>
+        <v>13.09</v>
       </c>
       <c r="F142" s="2" t="inlineStr">
         <is>
-          <t>50/116</t>
+          <t>64/116</t>
         </is>
       </c>
       <c r="G142" s="2" t="n">
-        <v>-452.28</v>
+        <v>197.62</v>
       </c>
       <c r="H142" s="2" t="n"/>
     </row>
@@ -5033,15 +5033,15 @@
         <v>13</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>-6.82</v>
+        <v>-12.86</v>
       </c>
       <c r="F143" s="3" t="inlineStr">
         <is>
-          <t>83/115</t>
+          <t>77/115</t>
         </is>
       </c>
       <c r="G143" s="3" t="n">
-        <v>-459.11</v>
+        <v>184.76</v>
       </c>
       <c r="H143" s="3" t="n"/>
     </row>
@@ -5065,15 +5065,15 @@
         <v>2</v>
       </c>
       <c r="E144" s="2" t="n">
-        <v>6.29</v>
+        <v>18.03</v>
       </c>
       <c r="F144" s="2" t="inlineStr">
         <is>
-          <t>66/116</t>
+          <t>47/116</t>
         </is>
       </c>
       <c r="G144" s="2" t="n">
-        <v>-452.82</v>
+        <v>202.8</v>
       </c>
       <c r="H144" s="2" t="n"/>
     </row>
@@ -5097,15 +5097,15 @@
         <v>35</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>-57.82</v>
+        <v>-47.64</v>
       </c>
       <c r="F145" s="3" t="inlineStr">
         <is>
-          <t>5/115</t>
+          <t>8/115</t>
         </is>
       </c>
       <c r="G145" s="3" t="n">
-        <v>-510.64</v>
+        <v>155.16</v>
       </c>
       <c r="H145" s="3" t="n"/>
     </row>
@@ -5129,15 +5129,15 @@
         <v>3</v>
       </c>
       <c r="E146" s="2" t="n">
-        <v>-27.44</v>
+        <v>16.88</v>
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>19/116</t>
+          <t>52/116</t>
         </is>
       </c>
       <c r="G146" s="2" t="n">
-        <v>-538.09</v>
+        <v>172.04</v>
       </c>
       <c r="H146" s="2" t="n"/>
     </row>
@@ -5161,15 +5161,15 @@
         <v>18</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>-16.02</v>
+        <v>-40.89</v>
       </c>
       <c r="F147" s="3" t="inlineStr">
         <is>
-          <t>48/115</t>
+          <t>16/115</t>
         </is>
       </c>
       <c r="G147" s="3" t="n">
-        <v>-554.1</v>
+        <v>131.15</v>
       </c>
       <c r="H147" s="3" t="n"/>
     </row>
@@ -5193,15 +5193,15 @@
         <v>2</v>
       </c>
       <c r="E148" s="2" t="n">
-        <v>0.42</v>
+        <v>17.18</v>
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>113/116</t>
+          <t>50/116</t>
         </is>
       </c>
       <c r="G148" s="2" t="n">
-        <v>-553.6799999999999</v>
+        <v>148.33</v>
       </c>
       <c r="H148" s="2" t="n"/>
     </row>
@@ -5225,15 +5225,15 @@
         <v>21</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>-8.369999999999999</v>
+        <v>-14.96</v>
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>77/115</t>
+          <t>70/115</t>
         </is>
       </c>
       <c r="G149" s="3" t="n">
-        <v>-562.05</v>
+        <v>133.38</v>
       </c>
       <c r="H149" s="3" t="n"/>
     </row>
@@ -5257,15 +5257,15 @@
         <v>14</v>
       </c>
       <c r="E150" s="2" t="n">
-        <v>-10.96</v>
+        <v>3.96</v>
       </c>
       <c r="F150" s="2" t="inlineStr">
         <is>
-          <t>43/116</t>
+          <t>110/116</t>
         </is>
       </c>
       <c r="G150" s="2" t="n">
-        <v>-573.01</v>
+        <v>137.34</v>
       </c>
       <c r="H150" s="2" t="n"/>
     </row>
@@ -5289,15 +5289,15 @@
         <v>45</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>-26.65</v>
+        <v>-28.57</v>
       </c>
       <c r="F151" s="3" t="inlineStr">
         <is>
-          <t>23/115</t>
+          <t>29/115</t>
         </is>
       </c>
       <c r="G151" s="3" t="n">
-        <v>-599.66</v>
+        <v>108.77</v>
       </c>
       <c r="H151" s="3" t="n"/>
     </row>
@@ -5321,15 +5321,15 @@
         <v>13</v>
       </c>
       <c r="E152" s="2" t="n">
-        <v>19.73</v>
+        <v>26.67</v>
       </c>
       <c r="F152" s="2" t="inlineStr">
         <is>
-          <t>28/116</t>
+          <t>31/116</t>
         </is>
       </c>
       <c r="G152" s="2" t="n">
-        <v>-579.9299999999999</v>
+        <v>135.43</v>
       </c>
       <c r="H152" s="2" t="n"/>
     </row>
@@ -5353,15 +5353,15 @@
         <v>15</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>-8.82</v>
+        <v>-11.23</v>
       </c>
       <c r="F153" s="3" t="inlineStr">
         <is>
-          <t>74/115</t>
+          <t>85/115</t>
         </is>
       </c>
       <c r="G153" s="3" t="n">
-        <v>-588.75</v>
+        <v>124.21</v>
       </c>
       <c r="H153" s="3" t="n"/>
     </row>
@@ -5385,15 +5385,15 @@
         <v>7</v>
       </c>
       <c r="E154" s="2" t="n">
-        <v>24.07</v>
+        <v>78.73999999999999</v>
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>24/116</t>
+          <t>10/116</t>
         </is>
       </c>
       <c r="G154" s="2" t="n">
-        <v>-564.6799999999999</v>
+        <v>202.95</v>
       </c>
       <c r="H154" s="2" t="n"/>
     </row>
@@ -5417,15 +5417,15 @@
         <v>7</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>-22.5</v>
+        <v>-35.9</v>
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>31/115</t>
+          <t>20/115</t>
         </is>
       </c>
       <c r="G155" s="3" t="n">
-        <v>-587.1799999999999</v>
+        <v>167.04</v>
       </c>
       <c r="H155" s="3" t="n"/>
     </row>
@@ -5449,15 +5449,15 @@
         <v>2</v>
       </c>
       <c r="E156" s="2" t="n">
-        <v>-4.92</v>
+        <v>14.78</v>
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>77/116</t>
+          <t>61/116</t>
         </is>
       </c>
       <c r="G156" s="2" t="n">
-        <v>-592.1</v>
+        <v>181.82</v>
       </c>
       <c r="H156" s="2" t="n"/>
     </row>
@@ -5481,15 +5481,15 @@
         <v>8</v>
       </c>
       <c r="E157" s="3" t="n">
-        <v>-20.24</v>
+        <v>-20.36</v>
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>33/115</t>
+          <t>48/115</t>
         </is>
       </c>
       <c r="G157" s="3" t="n">
-        <v>-612.33</v>
+        <v>161.46</v>
       </c>
       <c r="H157" s="3" t="n"/>
     </row>
@@ -5513,15 +5513,15 @@
         <v>10</v>
       </c>
       <c r="E158" s="2" t="n">
-        <v>5.44</v>
+        <v>9.77</v>
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>74/116</t>
+          <t>77/116</t>
         </is>
       </c>
       <c r="G158" s="2" t="n">
-        <v>-606.89</v>
+        <v>171.23</v>
       </c>
       <c r="H158" s="2" t="n"/>
     </row>
@@ -5545,15 +5545,15 @@
         <v>13</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>-18.38</v>
+        <v>-21.58</v>
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>37/115</t>
+          <t>42/115</t>
         </is>
       </c>
       <c r="G159" s="3" t="n">
-        <v>-625.28</v>
+        <v>149.66</v>
       </c>
       <c r="H159" s="3" t="n"/>
     </row>
@@ -5577,15 +5577,15 @@
         <v>11</v>
       </c>
       <c r="E160" s="2" t="n">
-        <v>9.42</v>
+        <v>52.84</v>
       </c>
       <c r="F160" s="2" t="inlineStr">
         <is>
-          <t>52/116</t>
+          <t>17/116</t>
         </is>
       </c>
       <c r="G160" s="2" t="n">
-        <v>-615.86</v>
+        <v>202.5</v>
       </c>
       <c r="H160" s="2" t="n"/>
     </row>
@@ -5609,7 +5609,7 @@
         <v>16</v>
       </c>
       <c r="E161" s="3" t="n">
-        <v>-46.05</v>
+        <v>-44</v>
       </c>
       <c r="F161" s="3" t="inlineStr">
         <is>
@@ -5617,7 +5617,7 @@
         </is>
       </c>
       <c r="G161" s="3" t="n">
-        <v>-661.91</v>
+        <v>158.5</v>
       </c>
       <c r="H161" s="3" t="n"/>
     </row>
@@ -5641,15 +5641,15 @@
         <v>2</v>
       </c>
       <c r="E162" s="2" t="n">
-        <v>-0.93</v>
+        <v>4.59</v>
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>107/116</t>
+          <t>106/116</t>
         </is>
       </c>
       <c r="G162" s="2" t="n">
-        <v>-662.84</v>
+        <v>163.09</v>
       </c>
       <c r="H162" s="2" t="n"/>
     </row>
@@ -5673,15 +5673,15 @@
         <v>11</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>-8.75</v>
+        <v>-15.61</v>
       </c>
       <c r="F163" s="3" t="inlineStr">
         <is>
-          <t>75/115</t>
+          <t>66/115</t>
         </is>
       </c>
       <c r="G163" s="3" t="n">
-        <v>-671.59</v>
+        <v>147.48</v>
       </c>
       <c r="H163" s="3" t="n"/>
     </row>
@@ -5705,15 +5705,15 @@
         <v>10</v>
       </c>
       <c r="E164" s="2" t="n">
-        <v>10.72</v>
+        <v>38.29</v>
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>46/116</t>
+          <t>22/116</t>
         </is>
       </c>
       <c r="G164" s="2" t="n">
-        <v>-660.87</v>
+        <v>185.77</v>
       </c>
       <c r="H164" s="2" t="n"/>
     </row>
@@ -5737,15 +5737,15 @@
         <v>2</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>-24.57</v>
+        <v>-25.43</v>
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>28/115</t>
+          <t>35/115</t>
         </is>
       </c>
       <c r="G165" s="3" t="n">
-        <v>-685.45</v>
+        <v>160.33</v>
       </c>
       <c r="H165" s="3" t="n"/>
     </row>
@@ -5769,15 +5769,15 @@
         <v>5</v>
       </c>
       <c r="E166" s="2" t="n">
-        <v>3.32</v>
+        <v>19.15</v>
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>89/116</t>
+          <t>46/116</t>
         </is>
       </c>
       <c r="G166" s="2" t="n">
-        <v>-682.13</v>
+        <v>179.48</v>
       </c>
       <c r="H166" s="2" t="n"/>
     </row>
@@ -5801,15 +5801,15 @@
         <v>15</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>-23.19</v>
+        <v>-26.51</v>
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>30/115</t>
+          <t>33/115</t>
         </is>
       </c>
       <c r="G167" s="3" t="n">
-        <v>-705.3200000000001</v>
+        <v>152.97</v>
       </c>
       <c r="H167" s="3" t="n"/>
     </row>
@@ -5833,15 +5833,15 @@
         <v>5</v>
       </c>
       <c r="E168" s="2" t="n">
-        <v>38.95</v>
+        <v>87.65000000000001</v>
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>14/116</t>
+          <t>7/116</t>
         </is>
       </c>
       <c r="G168" s="2" t="n">
-        <v>-666.37</v>
+        <v>240.62</v>
       </c>
       <c r="H168" s="2" t="n"/>
     </row>
@@ -5865,15 +5865,15 @@
         <v>13</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>-53.96</v>
+        <v>-50.4</v>
       </c>
       <c r="F169" s="3" t="inlineStr">
         <is>
-          <t>6/115</t>
+          <t>7/115</t>
         </is>
       </c>
       <c r="G169" s="3" t="n">
-        <v>-720.34</v>
+        <v>190.22</v>
       </c>
       <c r="H169" s="3" t="n"/>
     </row>
@@ -5897,15 +5897,15 @@
         <v>22</v>
       </c>
       <c r="E170" s="2" t="n">
-        <v>7.01</v>
+        <v>9.9</v>
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>63/116</t>
+          <t>75/116</t>
         </is>
       </c>
       <c r="G170" s="2" t="n">
-        <v>-713.33</v>
+        <v>200.12</v>
       </c>
       <c r="H170" s="2" t="n"/>
     </row>
@@ -5929,15 +5929,15 @@
         <v>8</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>-11.73</v>
+        <v>-13.37</v>
       </c>
       <c r="F171" s="3" t="inlineStr">
         <is>
-          <t>61/115</t>
+          <t>75/115</t>
         </is>
       </c>
       <c r="G171" s="3" t="n">
-        <v>-725.0599999999999</v>
+        <v>186.75</v>
       </c>
       <c r="H171" s="3" t="n"/>
     </row>
@@ -5961,15 +5961,15 @@
         <v>5</v>
       </c>
       <c r="E172" s="2" t="n">
-        <v>2.86</v>
+        <v>12.75</v>
       </c>
       <c r="F172" s="2" t="inlineStr">
         <is>
-          <t>93/116</t>
+          <t>66/116</t>
         </is>
       </c>
       <c r="G172" s="2" t="n">
-        <v>-722.2</v>
+        <v>199.5</v>
       </c>
       <c r="H172" s="2" t="n"/>
     </row>
@@ -5993,15 +5993,15 @@
         <v>56</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>-82.65000000000001</v>
+        <v>-62.8</v>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>2/115</t>
+          <t>4/115</t>
         </is>
       </c>
       <c r="G173" s="3" t="n">
-        <v>-804.85</v>
+        <v>136.7</v>
       </c>
       <c r="H173" s="3" t="n"/>
     </row>
@@ -6025,15 +6025,15 @@
         <v>6</v>
       </c>
       <c r="E174" s="2" t="n">
-        <v>45.31</v>
+        <v>49.6</v>
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>11/116</t>
+          <t>19/116</t>
         </is>
       </c>
       <c r="G174" s="2" t="n">
-        <v>-759.55</v>
+        <v>186.3</v>
       </c>
       <c r="H174" s="2" t="n"/>
     </row>
@@ -6057,15 +6057,15 @@
         <v>4</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>4.42</v>
+        <v>-2.14</v>
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>99/115</t>
+          <t>114/115</t>
         </is>
       </c>
       <c r="G175" s="3" t="n">
-        <v>-755.13</v>
+        <v>184.16</v>
       </c>
       <c r="H175" s="3" t="n"/>
     </row>
@@ -6089,15 +6089,15 @@
         <v>2</v>
       </c>
       <c r="E176" s="2" t="n">
-        <v>3.35</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>88/116</t>
+          <t>87/116</t>
         </is>
       </c>
       <c r="G176" s="2" t="n">
-        <v>-751.78</v>
+        <v>192.36</v>
       </c>
       <c r="H176" s="2" t="n"/>
     </row>
@@ -6121,15 +6121,15 @@
         <v>15</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>-20.17</v>
+        <v>-34.34</v>
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>34/115</t>
+          <t>23/115</t>
         </is>
       </c>
       <c r="G177" s="3" t="n">
-        <v>-771.9400000000001</v>
+        <v>158.02</v>
       </c>
       <c r="H177" s="3" t="n"/>
     </row>
@@ -6153,15 +6153,15 @@
         <v>4</v>
       </c>
       <c r="E178" s="2" t="n">
-        <v>-5.6</v>
+        <v>15.6</v>
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>73/116</t>
+          <t>59/116</t>
         </is>
       </c>
       <c r="G178" s="2" t="n">
-        <v>-777.55</v>
+        <v>173.62</v>
       </c>
       <c r="H178" s="2" t="n"/>
     </row>
@@ -6185,15 +6185,15 @@
         <v>26</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>-47.62</v>
+        <v>-44.17</v>
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>9/115</t>
+          <t>10/115</t>
         </is>
       </c>
       <c r="G179" s="3" t="n">
-        <v>-825.17</v>
+        <v>129.45</v>
       </c>
       <c r="H179" s="3" t="n"/>
     </row>
@@ -6217,15 +6217,15 @@
         <v>43</v>
       </c>
       <c r="E180" s="2" t="n">
-        <v>30.48</v>
+        <v>36.32</v>
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>17/116</t>
+          <t>24/116</t>
         </is>
       </c>
       <c r="G180" s="2" t="n">
-        <v>-794.6900000000001</v>
+        <v>165.76</v>
       </c>
       <c r="H180" s="2" t="n"/>
     </row>
@@ -6249,15 +6249,15 @@
         <v>12</v>
       </c>
       <c r="E181" s="3" t="n">
-        <v>-17.18</v>
+        <v>-17.37</v>
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>42/115</t>
+          <t>60/115</t>
         </is>
       </c>
       <c r="G181" s="3" t="n">
-        <v>-811.87</v>
+        <v>148.39</v>
       </c>
       <c r="H181" s="3" t="n"/>
     </row>
@@ -6281,7 +6281,7 @@
         <v>3</v>
       </c>
       <c r="E182" s="2" t="n">
-        <v>0.11</v>
+        <v>1.87</v>
       </c>
       <c r="F182" s="2" t="inlineStr">
         <is>
@@ -6289,7 +6289,7 @@
         </is>
       </c>
       <c r="G182" s="2" t="n">
-        <v>-811.76</v>
+        <v>150.26</v>
       </c>
       <c r="H182" s="2" t="n"/>
     </row>
@@ -6313,15 +6313,15 @@
         <v>7</v>
       </c>
       <c r="E183" s="3" t="n">
-        <v>1.1</v>
+        <v>-1.83</v>
       </c>
       <c r="F183" s="3" t="inlineStr">
         <is>
-          <t>106/115</t>
+          <t>115/115</t>
         </is>
       </c>
       <c r="G183" s="3" t="n">
-        <v>-810.65</v>
+        <v>148.42</v>
       </c>
       <c r="H183" s="3" t="n"/>
     </row>
@@ -6345,15 +6345,15 @@
         <v>4</v>
       </c>
       <c r="E184" s="2" t="n">
-        <v>3.77</v>
+        <v>7.94</v>
       </c>
       <c r="F184" s="2" t="inlineStr">
         <is>
-          <t>83/116</t>
+          <t>90/116</t>
         </is>
       </c>
       <c r="G184" s="2" t="n">
-        <v>-806.88</v>
+        <v>156.37</v>
       </c>
       <c r="H184" s="2" t="n"/>
     </row>
@@ -6377,15 +6377,15 @@
         <v>14</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>-7.59</v>
+        <v>-13.51</v>
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>81/115</t>
+          <t>74/115</t>
         </is>
       </c>
       <c r="G185" s="3" t="n">
-        <v>-814.47</v>
+        <v>142.86</v>
       </c>
       <c r="H185" s="3" t="n"/>
     </row>
@@ -6409,15 +6409,15 @@
         <v>5</v>
       </c>
       <c r="E186" s="2" t="n">
-        <v>10.25</v>
+        <v>26.13</v>
       </c>
       <c r="F186" s="2" t="inlineStr">
         <is>
-          <t>49/116</t>
+          <t>33/116</t>
         </is>
       </c>
       <c r="G186" s="2" t="n">
-        <v>-804.22</v>
+        <v>168.99</v>
       </c>
       <c r="H186" s="2" t="n"/>
     </row>
@@ -6441,15 +6441,15 @@
         <v>9</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>-15.79</v>
+        <v>-16.67</v>
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>50/115</t>
+          <t>63/115</t>
         </is>
       </c>
       <c r="G187" s="3" t="n">
-        <v>-820.01</v>
+        <v>152.32</v>
       </c>
       <c r="H187" s="3" t="n"/>
     </row>
@@ -6473,15 +6473,15 @@
         <v>12</v>
       </c>
       <c r="E188" s="2" t="n">
-        <v>-0.92</v>
+        <v>41.63</v>
       </c>
       <c r="F188" s="2" t="inlineStr">
         <is>
-          <t>108/116</t>
+          <t>21/116</t>
         </is>
       </c>
       <c r="G188" s="2" t="n">
-        <v>-820.92</v>
+        <v>193.95</v>
       </c>
       <c r="H188" s="2" t="n"/>
     </row>
@@ -6505,15 +6505,15 @@
         <v>7</v>
       </c>
       <c r="E189" s="3" t="n">
-        <v>-32.99</v>
+        <v>-36.91</v>
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>17/115</t>
+          <t>19/115</t>
         </is>
       </c>
       <c r="G189" s="3" t="n">
-        <v>-853.91</v>
+        <v>157.04</v>
       </c>
       <c r="H189" s="3" t="n"/>
     </row>
@@ -6537,15 +6537,15 @@
         <v>9</v>
       </c>
       <c r="E190" s="2" t="n">
-        <v>-0.64</v>
+        <v>24.47</v>
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>111/116</t>
+          <t>36/116</t>
         </is>
       </c>
       <c r="G190" s="2" t="n">
-        <v>-854.55</v>
+        <v>181.51</v>
       </c>
       <c r="H190" s="2" t="n"/>
     </row>
@@ -6569,15 +6569,15 @@
         <v>8</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>-25.83</v>
+        <v>-25.3</v>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>26/115</t>
+          <t>36/115</t>
         </is>
       </c>
       <c r="G191" s="3" t="n">
-        <v>-880.38</v>
+        <v>156.21</v>
       </c>
       <c r="H191" s="3" t="n"/>
     </row>
@@ -6601,15 +6601,15 @@
         <v>13</v>
       </c>
       <c r="E192" s="2" t="n">
-        <v>11.13</v>
+        <v>24.03</v>
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>41/116</t>
+          <t>37/116</t>
         </is>
       </c>
       <c r="G192" s="2" t="n">
-        <v>-869.25</v>
+        <v>180.24</v>
       </c>
       <c r="H192" s="2" t="n"/>
     </row>
@@ -6633,15 +6633,15 @@
         <v>3</v>
       </c>
       <c r="E193" s="3" t="n">
-        <v>3.14</v>
+        <v>-11.44</v>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>104/115</t>
+          <t>84/115</t>
         </is>
       </c>
       <c r="G193" s="3" t="n">
-        <v>-866.1</v>
+        <v>168.8</v>
       </c>
       <c r="H193" s="3" t="n"/>
     </row>
@@ -6665,15 +6665,15 @@
         <v>7</v>
       </c>
       <c r="E194" s="2" t="n">
-        <v>16.46</v>
+        <v>69.79000000000001</v>
       </c>
       <c r="F194" s="2" t="inlineStr">
         <is>
-          <t>31/116</t>
+          <t>11/116</t>
         </is>
       </c>
       <c r="G194" s="2" t="n">
-        <v>-849.65</v>
+        <v>238.59</v>
       </c>
       <c r="H194" s="2" t="n"/>
     </row>
@@ -6697,15 +6697,15 @@
         <v>7</v>
       </c>
       <c r="E195" s="3" t="n">
-        <v>-39.58</v>
+        <v>-40.61</v>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>13/115</t>
+          <t>17/115</t>
         </is>
       </c>
       <c r="G195" s="3" t="n">
-        <v>-889.23</v>
+        <v>197.98</v>
       </c>
       <c r="H195" s="3" t="n"/>
     </row>
@@ -6729,15 +6729,15 @@
         <v>10</v>
       </c>
       <c r="E196" s="2" t="n">
-        <v>3.7</v>
+        <v>22.93</v>
       </c>
       <c r="F196" s="2" t="inlineStr">
         <is>
-          <t>84/116</t>
+          <t>40/116</t>
         </is>
       </c>
       <c r="G196" s="2" t="n">
-        <v>-885.53</v>
+        <v>220.91</v>
       </c>
       <c r="H196" s="2" t="n"/>
     </row>
@@ -6761,15 +6761,15 @@
         <v>4</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>-17.97</v>
+        <v>-18.49</v>
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>38/115</t>
+          <t>55/115</t>
         </is>
       </c>
       <c r="G197" s="3" t="n">
-        <v>-903.5</v>
+        <v>202.42</v>
       </c>
       <c r="H197" s="3" t="n"/>
     </row>
@@ -6793,15 +6793,15 @@
         <v>20</v>
       </c>
       <c r="E198" s="2" t="n">
-        <v>0.88</v>
+        <v>17.53</v>
       </c>
       <c r="F198" s="2" t="inlineStr">
         <is>
-          <t>109/116</t>
+          <t>48/116</t>
         </is>
       </c>
       <c r="G198" s="2" t="n">
-        <v>-902.62</v>
+        <v>219.95</v>
       </c>
       <c r="H198" s="2" t="n"/>
     </row>
@@ -6825,15 +6825,15 @@
         <v>6</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>-14.38</v>
+        <v>-15</v>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>55/115</t>
+          <t>68/115</t>
         </is>
       </c>
       <c r="G199" s="3" t="n">
-        <v>-917</v>
+        <v>204.95</v>
       </c>
       <c r="H199" s="3" t="n"/>
     </row>
@@ -6857,15 +6857,15 @@
         <v>11</v>
       </c>
       <c r="E200" s="2" t="n">
-        <v>-2.82</v>
+        <v>23.84</v>
       </c>
       <c r="F200" s="2" t="inlineStr">
         <is>
-          <t>94/116</t>
+          <t>38/116</t>
         </is>
       </c>
       <c r="G200" s="2" t="n">
-        <v>-919.8200000000001</v>
+        <v>228.79</v>
       </c>
       <c r="H200" s="2" t="n"/>
     </row>
@@ -6889,15 +6889,15 @@
         <v>7</v>
       </c>
       <c r="E201" s="3" t="n">
-        <v>-18.95</v>
+        <v>-25</v>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>35/115</t>
+          <t>37/115</t>
         </is>
       </c>
       <c r="G201" s="3" t="n">
-        <v>-938.77</v>
+        <v>203.79</v>
       </c>
       <c r="H201" s="3" t="n"/>
     </row>
@@ -6921,15 +6921,15 @@
         <v>3</v>
       </c>
       <c r="E202" s="2" t="n">
-        <v>3.53</v>
+        <v>6.78</v>
       </c>
       <c r="F202" s="2" t="inlineStr">
         <is>
-          <t>87/116</t>
+          <t>94/116</t>
         </is>
       </c>
       <c r="G202" s="2" t="n">
-        <v>-935.24</v>
+        <v>210.57</v>
       </c>
       <c r="H202" s="2" t="n"/>
     </row>
@@ -6953,15 +6953,15 @@
         <v>10</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>-16.87</v>
+        <v>-21.96</v>
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>45/115</t>
+          <t>41/115</t>
         </is>
       </c>
       <c r="G203" s="3" t="n">
-        <v>-952.11</v>
+        <v>188.61</v>
       </c>
       <c r="H203" s="3" t="n"/>
     </row>
@@ -6985,15 +6985,15 @@
         <v>2</v>
       </c>
       <c r="E204" s="2" t="n">
-        <v>-7.88</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="F204" s="2" t="inlineStr">
         <is>
-          <t>61/116</t>
+          <t>76/116</t>
         </is>
       </c>
       <c r="G204" s="2" t="n">
-        <v>-959.99</v>
+        <v>198.48</v>
       </c>
       <c r="H204" s="2" t="n"/>
     </row>
@@ -7017,15 +7017,15 @@
         <v>54</v>
       </c>
       <c r="E205" s="3" t="n">
-        <v>-1.07</v>
+        <v>-41.02</v>
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>109/115</t>
+          <t>15/115</t>
         </is>
       </c>
       <c r="G205" s="3" t="n">
-        <v>-961.0599999999999</v>
+        <v>157.46</v>
       </c>
       <c r="H205" s="3" t="n"/>
     </row>
@@ -7049,15 +7049,15 @@
         <v>3</v>
       </c>
       <c r="E206" s="2" t="n">
-        <v>10.85</v>
+        <v>16</v>
       </c>
       <c r="F206" s="2" t="inlineStr">
         <is>
-          <t>45/116</t>
+          <t>54/116</t>
         </is>
       </c>
       <c r="G206" s="2" t="n">
-        <v>-950.22</v>
+        <v>173.46</v>
       </c>
       <c r="H206" s="2" t="n"/>
     </row>
@@ -7081,15 +7081,15 @@
         <v>10</v>
       </c>
       <c r="E207" s="3" t="n">
-        <v>10.22</v>
+        <v>-13.79</v>
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>69/115</t>
+          <t>72/115</t>
         </is>
       </c>
       <c r="G207" s="3" t="n">
-        <v>-940</v>
+        <v>159.66</v>
       </c>
       <c r="H207" s="3" t="n"/>
     </row>
@@ -7113,15 +7113,15 @@
         <v>5</v>
       </c>
       <c r="E208" s="2" t="n">
-        <v>1.5</v>
+        <v>11.34</v>
       </c>
       <c r="F208" s="2" t="inlineStr">
         <is>
-          <t>100/116</t>
+          <t>71/116</t>
         </is>
       </c>
       <c r="G208" s="2" t="n">
-        <v>-938.5</v>
+        <v>171</v>
       </c>
       <c r="H208" s="2" t="n"/>
     </row>
@@ -7145,15 +7145,15 @@
         <v>13</v>
       </c>
       <c r="E209" s="3" t="n">
-        <v>-16.9</v>
+        <v>-19.44</v>
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>44/115</t>
+          <t>50/115</t>
         </is>
       </c>
       <c r="G209" s="3" t="n">
-        <v>-955.4</v>
+        <v>151.56</v>
       </c>
       <c r="H209" s="3" t="n"/>
     </row>
@@ -7177,7 +7177,7 @@
         <v>57</v>
       </c>
       <c r="E210" s="2" t="n">
-        <v>60.66</v>
+        <v>84.48</v>
       </c>
       <c r="F210" s="2" t="inlineStr">
         <is>
@@ -7185,7 +7185,7 @@
         </is>
       </c>
       <c r="G210" s="2" t="n">
-        <v>-894.74</v>
+        <v>236.04</v>
       </c>
       <c r="H210" s="2" t="inlineStr">
         <is>
@@ -7213,15 +7213,15 @@
         <v>20</v>
       </c>
       <c r="E211" s="3" t="n">
-        <v>-6.45</v>
+        <v>-23.78</v>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>86/115</t>
+          <t>39/115</t>
         </is>
       </c>
       <c r="G211" s="3" t="n">
-        <v>-901.1900000000001</v>
+        <v>212.26</v>
       </c>
       <c r="H211" s="3" t="n"/>
     </row>
@@ -7245,15 +7245,15 @@
         <v>5</v>
       </c>
       <c r="E212" s="2" t="n">
-        <v>-3.68</v>
+        <v>25</v>
       </c>
       <c r="F212" s="2" t="inlineStr">
         <is>
-          <t>85/116</t>
+          <t>35/116</t>
         </is>
       </c>
       <c r="G212" s="2" t="n">
-        <v>-904.87</v>
+        <v>237.26</v>
       </c>
       <c r="H212" s="2" t="n"/>
     </row>
@@ -7277,15 +7277,15 @@
         <v>6</v>
       </c>
       <c r="E213" s="3" t="n">
-        <v>-27.69</v>
+        <v>-29.05</v>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>21/115</t>
+          <t>28/115</t>
         </is>
       </c>
       <c r="G213" s="3" t="n">
-        <v>-932.5599999999999</v>
+        <v>208.21</v>
       </c>
       <c r="H213" s="3" t="n"/>
     </row>
@@ -7309,15 +7309,15 @@
         <v>3</v>
       </c>
       <c r="E214" s="2" t="n">
-        <v>4.99</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="F214" s="2" t="inlineStr">
         <is>
-          <t>76/116</t>
+          <t>80/116</t>
         </is>
       </c>
       <c r="G214" s="2" t="n">
-        <v>-927.5700000000001</v>
+        <v>217.41</v>
       </c>
       <c r="H214" s="2" t="n"/>
     </row>
@@ -7341,15 +7341,15 @@
         <v>7</v>
       </c>
       <c r="E215" s="3" t="n">
-        <v>-10.85</v>
+        <v>-12.23</v>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>65/115</t>
+          <t>80/115</t>
         </is>
       </c>
       <c r="G215" s="3" t="n">
-        <v>-938.4299999999999</v>
+        <v>205.18</v>
       </c>
       <c r="H215" s="3" t="n"/>
     </row>
@@ -7373,15 +7373,15 @@
         <v>40</v>
       </c>
       <c r="E216" s="2" t="n">
-        <v>-116.24</v>
+        <v>26.93</v>
       </c>
       <c r="F216" s="2" t="inlineStr">
         <is>
-          <t>1/116</t>
+          <t>30/116</t>
         </is>
       </c>
       <c r="G216" s="2" t="n">
-        <v>-1054.67</v>
+        <v>232.12</v>
       </c>
       <c r="H216" s="2" t="inlineStr">
         <is>
@@ -7409,15 +7409,15 @@
         <v>5</v>
       </c>
       <c r="E217" s="3" t="n">
-        <v>-66.63</v>
+        <v>-80.12</v>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>4/115</t>
+          <t>1/115</t>
         </is>
       </c>
       <c r="G217" s="3" t="n">
-        <v>-1121.29</v>
+        <v>151.99</v>
       </c>
       <c r="H217" s="3" t="n"/>
     </row>
@@ -7441,15 +7441,15 @@
         <v>2</v>
       </c>
       <c r="E218" s="2" t="n">
-        <v>-14.28</v>
+        <v>15.95</v>
       </c>
       <c r="F218" s="2" t="inlineStr">
         <is>
-          <t>35/116</t>
+          <t>55/116</t>
         </is>
       </c>
       <c r="G218" s="2" t="n">
-        <v>-1135.57</v>
+        <v>167.94</v>
       </c>
       <c r="H218" s="2" t="n"/>
     </row>
@@ -7473,7 +7473,7 @@
         <v>70</v>
       </c>
       <c r="E219" s="3" t="n">
-        <v>-82.38</v>
+        <v>-65.70999999999999</v>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
@@ -7481,7 +7481,7 @@
         </is>
       </c>
       <c r="G219" s="3" t="n">
-        <v>-1217.95</v>
+        <v>102.23</v>
       </c>
       <c r="H219" s="3" t="inlineStr">
         <is>
@@ -7509,15 +7509,15 @@
         <v>17</v>
       </c>
       <c r="E220" s="2" t="n">
-        <v>93.36</v>
+        <v>128.4</v>
       </c>
       <c r="F220" s="2" t="inlineStr">
         <is>
-          <t>3/116</t>
+          <t>2/116</t>
         </is>
       </c>
       <c r="G220" s="2" t="n">
-        <v>-1124.59</v>
+        <v>230.63</v>
       </c>
       <c r="H220" s="2" t="n"/>
     </row>
@@ -7541,15 +7541,15 @@
         <v>16</v>
       </c>
       <c r="E221" s="3" t="n">
-        <v>14.61</v>
+        <v>-18.92</v>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>54/115</t>
+          <t>52/115</t>
         </is>
       </c>
       <c r="G221" s="3" t="n">
-        <v>-1109.98</v>
+        <v>211.71</v>
       </c>
       <c r="H221" s="3" t="n"/>
     </row>
@@ -7573,15 +7573,15 @@
         <v>5</v>
       </c>
       <c r="E222" s="2" t="n">
-        <v>43.58</v>
+        <v>83.69</v>
       </c>
       <c r="F222" s="2" t="inlineStr">
         <is>
-          <t>13/116</t>
+          <t>9/116</t>
         </is>
       </c>
       <c r="G222" s="2" t="n">
-        <v>-1066.4</v>
+        <v>295.39</v>
       </c>
       <c r="H222" s="2" t="n"/>
     </row>
@@ -7605,15 +7605,15 @@
         <v>42</v>
       </c>
       <c r="E223" s="3" t="n">
-        <v>6.57</v>
+        <v>-45.56</v>
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>85/115</t>
+          <t>9/115</t>
         </is>
       </c>
       <c r="G223" s="3" t="n">
-        <v>-1059.83</v>
+        <v>249.83</v>
       </c>
       <c r="H223" s="3" t="inlineStr">
         <is>
@@ -7641,15 +7641,15 @@
         <v>22</v>
       </c>
       <c r="E224" s="2" t="n">
-        <v>112.25</v>
+        <v>170.19</v>
       </c>
       <c r="F224" s="2" t="inlineStr">
         <is>
-          <t>2/116</t>
+          <t>1/116</t>
         </is>
       </c>
       <c r="G224" s="2" t="n">
-        <v>-947.58</v>
+        <v>420.02</v>
       </c>
       <c r="H224" s="2" t="inlineStr">
         <is>
@@ -7677,15 +7677,15 @@
         <v>20</v>
       </c>
       <c r="E225" s="3" t="n">
-        <v>-26.6</v>
+        <v>-32.18</v>
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>24/115</t>
+          <t>26/115</t>
         </is>
       </c>
       <c r="G225" s="3" t="n">
-        <v>-974.1799999999999</v>
+        <v>387.84</v>
       </c>
       <c r="H225" s="3" t="n"/>
     </row>
@@ -7709,15 +7709,15 @@
         <v>15</v>
       </c>
       <c r="E226" s="2" t="n">
-        <v>-50.02</v>
+        <v>9.94</v>
       </c>
       <c r="F226" s="2" t="inlineStr">
         <is>
-          <t>9/116</t>
+          <t>73/116</t>
         </is>
       </c>
       <c r="G226" s="2" t="n">
-        <v>-1024.2</v>
+        <v>397.77</v>
       </c>
       <c r="H226" s="2" t="n"/>
     </row>
@@ -7741,15 +7741,15 @@
         <v>17</v>
       </c>
       <c r="E227" s="3" t="n">
-        <v>-49.34</v>
+        <v>-56.56</v>
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>7/115</t>
+          <t>5/115</t>
         </is>
       </c>
       <c r="G227" s="3" t="n">
-        <v>-1073.55</v>
+        <v>341.21</v>
       </c>
       <c r="H227" s="3" t="inlineStr">
         <is>
@@ -7777,15 +7777,15 @@
         <v>19</v>
       </c>
       <c r="E228" s="2" t="n">
-        <v>37.22</v>
+        <v>53.69</v>
       </c>
       <c r="F228" s="2" t="inlineStr">
         <is>
-          <t>15/116</t>
+          <t>14/116</t>
         </is>
       </c>
       <c r="G228" s="2" t="n">
-        <v>-1036.33</v>
+        <v>394.9</v>
       </c>
       <c r="H228" s="2" t="inlineStr">
         <is>
@@ -7813,15 +7813,15 @@
         <v>7</v>
       </c>
       <c r="E229" s="3" t="n">
-        <v>-11.19</v>
+        <v>-17.03</v>
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>64/115</t>
+          <t>61/115</t>
         </is>
       </c>
       <c r="G229" s="3" t="n">
-        <v>-1047.52</v>
+        <v>377.87</v>
       </c>
       <c r="H229" s="3" t="n"/>
     </row>
@@ -7845,15 +7845,15 @@
         <v>5</v>
       </c>
       <c r="E230" s="2" t="n">
-        <v>3.26</v>
+        <v>10.53</v>
       </c>
       <c r="F230" s="2" t="inlineStr">
         <is>
-          <t>90/116</t>
+          <t>72/116</t>
         </is>
       </c>
       <c r="G230" s="2" t="n">
-        <v>-1044.26</v>
+        <v>388.4</v>
       </c>
       <c r="H230" s="2" t="n"/>
     </row>
@@ -7877,15 +7877,15 @@
         <v>8</v>
       </c>
       <c r="E231" s="3" t="n">
-        <v>-9.720000000000001</v>
+        <v>-18.1</v>
       </c>
       <c r="F231" s="3" t="inlineStr">
         <is>
-          <t>72/115</t>
+          <t>57/115</t>
         </is>
       </c>
       <c r="G231" s="3" t="n">
-        <v>-1053.98</v>
+        <v>370.31</v>
       </c>
       <c r="H231" s="3" t="n"/>
     </row>
@@ -7909,15 +7909,15 @@
         <v>35</v>
       </c>
       <c r="E232" s="2" t="n">
-        <v>67.31999999999999</v>
+        <v>108.72</v>
       </c>
       <c r="F232" s="2" t="inlineStr">
         <is>
-          <t>5/116</t>
+          <t>4/116</t>
         </is>
       </c>
       <c r="G232" s="2" t="n">
-        <v>-986.66</v>
+        <v>479.03</v>
       </c>
       <c r="H232" s="2" t="n"/>
     </row>

</xml_diff>

<commit_message>
Improve detection logic for beginning of a rise
Refined the logic to accurately detect the start of a rise event, ensuring better alignment with peak-to-fall transitions and updated related outputs.

- Updated `trend_start_date` logic in backtest script to use `trend_peak_date`
- Modified `blne_rise_events.xlsx` with updated rise event data
- Adjusted `blne_rise_volatility_analysis.json` with new analysis timestamp and rise event details
- Updated `insider_conviction_all_stocks_results.json` with new analysis timestamp

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>23/01/2017</t>
+          <t>17/01/2017</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>-42</v>
@@ -601,7 +601,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>20/04/2017</t>
+          <t>19/04/2017</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>-17.65</v>
@@ -665,7 +665,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>23/05/2017</t>
+          <t>22/05/2017</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>-35.28</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>11/07/2017</t>
+          <t>10/07/2017</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>-8.66</v>
@@ -793,7 +793,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>25/08/2017</t>
+          <t>31/07/2017</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>-42.71</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>12/09/2017</t>
+          <t>11/09/2017</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>-11.95</v>
@@ -921,7 +921,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>09/10/2017</t>
+          <t>05/10/2017</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>-5.93</v>
@@ -985,7 +985,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>03/11/2017</t>
+          <t>30/10/2017</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>-3.19</v>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>01/12/2017</t>
+          <t>17/11/2017</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>-23.9</v>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>26/12/2017</t>
+          <t>22/12/2017</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>-14.76</v>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>23/01/2018</t>
+          <t>22/01/2018</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>-3.89</v>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>09/02/2018</t>
+          <t>01/02/2018</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>-6.6</v>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>19/03/2018</t>
+          <t>16/03/2018</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1314,7 +1314,7 @@
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>-5.94</v>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>06/04/2018</t>
+          <t>26/03/2018</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>-11.17</v>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>01/05/2018</t>
+          <t>24/04/2018</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>-3.19</v>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>15/05/2018</t>
+          <t>14/05/2018</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1506,7 +1506,7 @@
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>-9.73</v>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>09/07/2018</t>
+          <t>22/06/2018</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E35" s="3" t="n">
         <v>-15.14</v>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>03/08/2018</t>
+          <t>19/07/2018</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>-14.97</v>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>08/10/2018</t>
+          <t>24/09/2018</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="n">
         <v>-11.64</v>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>17/10/2018</t>
+          <t>16/10/2018</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>-6.71</v>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>07/11/2018</t>
+          <t>05/11/2018</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1826,7 +1826,7 @@
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>-28.32</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>03/12/2018</t>
+          <t>26/11/2018</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="D45" s="3" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>-4.81</v>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>22/01/2019</t>
+          <t>04/01/2019</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="D47" s="3" t="n">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E47" s="3" t="n">
         <v>-12.32</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>21/03/2019</t>
+          <t>18/03/2019</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
         </is>
       </c>
       <c r="D49" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="n">
         <v>-5.38</v>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>10/04/2019</t>
+          <t>09/04/2019</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E51" s="3" t="n">
         <v>-6.02</v>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>01/05/2019</t>
+          <t>29/04/2019</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="n">
         <v>-6.78</v>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>10/05/2019</t>
+          <t>09/05/2019</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E55" s="3" t="n">
         <v>-16.92</v>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>23/05/2019</t>
+          <t>22/05/2019</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="n">
         <v>-9</v>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>06/06/2019</t>
+          <t>05/06/2019</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2338,7 +2338,7 @@
         </is>
       </c>
       <c r="D59" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E59" s="3" t="n">
         <v>-12.92</v>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>24/06/2019</t>
+          <t>21/06/2019</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
@@ -2402,7 +2402,7 @@
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E61" s="3" t="n">
         <v>-7.69</v>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>02/07/2019</t>
+          <t>01/07/2019</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -2466,7 +2466,7 @@
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E63" s="3" t="n">
         <v>-19.12</v>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>07/08/2019</t>
+          <t>06/08/2019</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -2530,7 +2530,7 @@
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="n">
         <v>-6.98</v>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>16/09/2019</t>
+          <t>03/09/2019</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>-12.48</v>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>22/10/2019</t>
+          <t>16/10/2019</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
@@ -2658,7 +2658,7 @@
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E69" s="3" t="n">
         <v>-42.4</v>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>10/12/2019</t>
+          <t>27/11/2019</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E71" s="3" t="n">
         <v>-20.18</v>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>23/12/2019</t>
+          <t>19/12/2019</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -2786,7 +2786,7 @@
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E73" s="3" t="n">
         <v>-10.33</v>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>07/01/2020</t>
+          <t>06/01/2020</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -2850,7 +2850,7 @@
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E75" s="3" t="n">
         <v>-10.85</v>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>31/01/2020</t>
+          <t>30/01/2020</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E77" s="3" t="n">
         <v>-5.6</v>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>13/02/2020</t>
+          <t>07/02/2020</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="D79" s="3" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E79" s="3" t="n">
         <v>-72.97</v>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>30/04/2020</t>
+          <t>27/04/2020</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="D81" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="n">
         <v>-9.5</v>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>15/05/2020</t>
+          <t>08/05/2020</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
@@ -3106,7 +3106,7 @@
         </is>
       </c>
       <c r="D83" s="3" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E83" s="3" t="n">
         <v>-27.46</v>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>10/06/2020</t>
+          <t>09/06/2020</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
@@ -3170,7 +3170,7 @@
         </is>
       </c>
       <c r="D85" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E85" s="3" t="n">
         <v>-21.39</v>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>25/06/2020</t>
+          <t>24/06/2020</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="D87" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="n">
         <v>-18.57</v>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>16/07/2020</t>
+          <t>15/07/2020</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
@@ -3298,7 +3298,7 @@
         </is>
       </c>
       <c r="D89" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E89" s="3" t="n">
         <v>-20.59</v>
@@ -3353,7 +3353,7 @@
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>31/07/2020</t>
+          <t>27/07/2020</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="D91" s="3" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E91" s="3" t="n">
         <v>-10.77</v>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B93" s="3" t="inlineStr">
         <is>
-          <t>19/08/2020</t>
+          <t>18/08/2020</t>
         </is>
       </c>
       <c r="C93" s="3" t="inlineStr">
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="D93" s="3" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E93" s="3" t="n">
         <v>-39.89</v>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="B95" s="3" t="inlineStr">
         <is>
-          <t>08/10/2020</t>
+          <t>07/10/2020</t>
         </is>
       </c>
       <c r="C95" s="3" t="inlineStr">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="D95" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E95" s="3" t="n">
         <v>-6.56</v>
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B97" s="3" t="inlineStr">
         <is>
-          <t>16/10/2020</t>
+          <t>15/10/2020</t>
         </is>
       </c>
       <c r="C97" s="3" t="inlineStr">
@@ -3554,7 +3554,7 @@
         </is>
       </c>
       <c r="D97" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E97" s="3" t="n">
         <v>-6.06</v>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>12/11/2020</t>
+          <t>11/11/2020</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="D99" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E99" s="3" t="n">
         <v>-20.53</v>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="B101" s="3" t="inlineStr">
         <is>
-          <t>30/11/2020</t>
+          <t>27/11/2020</t>
         </is>
       </c>
       <c r="C101" s="3" t="inlineStr">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="D101" s="3" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E101" s="3" t="n">
         <v>-25.75</v>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>18/02/2021</t>
+          <t>09/02/2021</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
@@ -3746,7 +3746,7 @@
         </is>
       </c>
       <c r="D103" s="3" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E103" s="3" t="n">
         <v>-32.6</v>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="B105" s="3" t="inlineStr">
         <is>
-          <t>16/03/2021</t>
+          <t>15/03/2021</t>
         </is>
       </c>
       <c r="C105" s="3" t="inlineStr">
@@ -3810,7 +3810,7 @@
         </is>
       </c>
       <c r="D105" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E105" s="3" t="n">
         <v>-13.66</v>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="B107" s="3" t="inlineStr">
         <is>
-          <t>07/04/2021</t>
+          <t>06/04/2021</t>
         </is>
       </c>
       <c r="C107" s="3" t="inlineStr">
@@ -3874,7 +3874,7 @@
         </is>
       </c>
       <c r="D107" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E107" s="3" t="n">
         <v>-22.93</v>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="B109" s="3" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>23/04/2021</t>
         </is>
       </c>
       <c r="C109" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
         </is>
       </c>
       <c r="D109" s="3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E109" s="3" t="n">
         <v>-8.74</v>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B111" s="3" t="inlineStr">
         <is>
-          <t>08/06/2021</t>
+          <t>07/06/2021</t>
         </is>
       </c>
       <c r="C111" s="3" t="inlineStr">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="D111" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E111" s="3" t="n">
         <v>-12.19</v>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="B113" s="3" t="inlineStr">
         <is>
-          <t>25/06/2021</t>
+          <t>24/06/2021</t>
         </is>
       </c>
       <c r="C113" s="3" t="inlineStr">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D113" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E113" s="3" t="n">
         <v>-7.84</v>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="B115" s="3" t="inlineStr">
         <is>
-          <t>14/07/2021</t>
+          <t>13/07/2021</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
@@ -4130,7 +4130,7 @@
         </is>
       </c>
       <c r="D115" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E115" s="3" t="n">
         <v>-3.54</v>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="B117" s="3" t="inlineStr">
         <is>
-          <t>30/07/2021</t>
+          <t>23/07/2021</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
@@ -4194,7 +4194,7 @@
         </is>
       </c>
       <c r="D117" s="3" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E117" s="3" t="n">
         <v>-18.63</v>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="B119" s="3" t="inlineStr">
         <is>
-          <t>10/08/2021</t>
+          <t>06/08/2021</t>
         </is>
       </c>
       <c r="C119" s="3" t="inlineStr">
@@ -4258,7 +4258,7 @@
         </is>
       </c>
       <c r="D119" s="3" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E119" s="3" t="n">
         <v>-27.02</v>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="B121" s="3" t="inlineStr">
         <is>
-          <t>27/09/2021</t>
+          <t>09/09/2021</t>
         </is>
       </c>
       <c r="C121" s="3" t="inlineStr">
@@ -4322,7 +4322,7 @@
         </is>
       </c>
       <c r="D121" s="3" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E121" s="3" t="n">
         <v>-20.89</v>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="B123" s="3" t="inlineStr">
         <is>
-          <t>27/10/2021</t>
+          <t>26/10/2021</t>
         </is>
       </c>
       <c r="C123" s="3" t="inlineStr">
@@ -4386,7 +4386,7 @@
         </is>
       </c>
       <c r="D123" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E123" s="3" t="n">
         <v>-9.970000000000001</v>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="B125" s="3" t="inlineStr">
         <is>
-          <t>15/11/2021</t>
+          <t>12/11/2021</t>
         </is>
       </c>
       <c r="C125" s="3" t="inlineStr">
@@ -4450,7 +4450,7 @@
         </is>
       </c>
       <c r="D125" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E125" s="3" t="n">
         <v>-33.68</v>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="B127" s="3" t="inlineStr">
         <is>
-          <t>26/11/2021</t>
+          <t>24/11/2021</t>
         </is>
       </c>
       <c r="C127" s="3" t="inlineStr">
@@ -4514,7 +4514,7 @@
         </is>
       </c>
       <c r="D127" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E127" s="3" t="n">
         <v>-15.76</v>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="B129" s="3" t="inlineStr">
         <is>
-          <t>27/12/2021</t>
+          <t>08/12/2021</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="D129" s="3" t="n">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E129" s="3" t="n">
         <v>-51.46</v>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="B131" s="3" t="inlineStr">
         <is>
-          <t>17/02/2022</t>
+          <t>01/02/2022</t>
         </is>
       </c>
       <c r="C131" s="3" t="inlineStr">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="D131" s="3" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E131" s="3" t="n">
         <v>-20.66</v>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="B133" s="3" t="inlineStr">
         <is>
-          <t>01/03/2022</t>
+          <t>28/02/2022</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
@@ -4706,7 +4706,7 @@
         </is>
       </c>
       <c r="D133" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E133" s="3" t="n">
         <v>-18.35</v>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="B135" s="3" t="inlineStr">
         <is>
-          <t>11/04/2022</t>
+          <t>08/04/2022</t>
         </is>
       </c>
       <c r="C135" s="3" t="inlineStr">
@@ -4774,7 +4774,7 @@
         </is>
       </c>
       <c r="D135" s="3" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E135" s="3" t="n">
         <v>-35.56</v>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>03/05/2022</t>
+          <t>02/05/2022</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
@@ -4838,7 +4838,7 @@
         </is>
       </c>
       <c r="D137" s="3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E137" s="3" t="n">
         <v>-31.46</v>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>10/06/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
@@ -4902,7 +4902,7 @@
         </is>
       </c>
       <c r="D139" s="3" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E139" s="3" t="n">
         <v>-17.81</v>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>27/06/2022</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="D141" s="3" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E141" s="3" t="n">
         <v>-16.35</v>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>21/07/2022</t>
+          <t>08/07/2022</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
@@ -5030,7 +5030,7 @@
         </is>
       </c>
       <c r="D143" s="3" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E143" s="3" t="n">
         <v>-12.86</v>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>05/08/2022</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
         </is>
       </c>
       <c r="D145" s="3" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E145" s="3" t="n">
         <v>-47.64</v>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>16/09/2022</t>
+          <t>14/09/2022</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
@@ -5158,7 +5158,7 @@
         </is>
       </c>
       <c r="D147" s="3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E147" s="3" t="n">
         <v>-40.89</v>
@@ -5213,7 +5213,7 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>07/10/2022</t>
+          <t>06/10/2022</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="D149" s="3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E149" s="3" t="n">
         <v>-14.96</v>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>14/11/2022</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
@@ -5286,7 +5286,7 @@
         </is>
       </c>
       <c r="D151" s="3" t="n">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E151" s="3" t="n">
         <v>-28.57</v>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>12/01/2023</t>
+          <t>11/01/2023</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
@@ -5350,7 +5350,7 @@
         </is>
       </c>
       <c r="D153" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E153" s="3" t="n">
         <v>-11.23</v>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>06/02/2023</t>
+          <t>03/02/2023</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
@@ -5414,7 +5414,7 @@
         </is>
       </c>
       <c r="D155" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E155" s="3" t="n">
         <v>-35.9</v>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>16/02/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
@@ -5478,7 +5478,7 @@
         </is>
       </c>
       <c r="D157" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E157" s="3" t="n">
         <v>-20.36</v>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>07/03/2023</t>
+          <t>03/03/2023</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="D159" s="3" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E159" s="3" t="n">
         <v>-21.58</v>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>03/04/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
@@ -5606,7 +5606,7 @@
         </is>
       </c>
       <c r="D161" s="3" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E161" s="3" t="n">
         <v>-44</v>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>24/04/2023</t>
+          <t>21/04/2023</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
@@ -5670,7 +5670,7 @@
         </is>
       </c>
       <c r="D163" s="3" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E163" s="3" t="n">
         <v>-15.61</v>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>16/05/2023</t>
+          <t>15/05/2023</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
@@ -5734,7 +5734,7 @@
         </is>
       </c>
       <c r="D165" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E165" s="3" t="n">
         <v>-25.43</v>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>24/05/2023</t>
+          <t>23/05/2023</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
@@ -5798,7 +5798,7 @@
         </is>
       </c>
       <c r="D167" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E167" s="3" t="n">
         <v>-26.51</v>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>14/06/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
@@ -5862,7 +5862,7 @@
         </is>
       </c>
       <c r="D169" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E169" s="3" t="n">
         <v>-50.4</v>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>20/07/2023</t>
+          <t>10/07/2023</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="D171" s="3" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E171" s="3" t="n">
         <v>-13.37</v>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>03/08/2023</t>
+          <t>02/08/2023</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
@@ -5990,7 +5990,7 @@
         </is>
       </c>
       <c r="D173" s="3" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E173" s="3" t="n">
         <v>-62.8</v>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>05/10/2023</t>
+          <t>04/10/2023</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
@@ -6054,7 +6054,7 @@
         </is>
       </c>
       <c r="D175" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E175" s="3" t="n">
         <v>-2.14</v>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>12/10/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
@@ -6118,7 +6118,7 @@
         </is>
       </c>
       <c r="D177" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E177" s="3" t="n">
         <v>-34.34</v>
@@ -6173,7 +6173,7 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>01/11/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
@@ -6182,7 +6182,7 @@
         </is>
       </c>
       <c r="D179" s="3" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E179" s="3" t="n">
         <v>-44.17</v>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>28/12/2023</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
@@ -6246,7 +6246,7 @@
         </is>
       </c>
       <c r="D181" s="3" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E181" s="3" t="n">
         <v>-17.37</v>
@@ -6301,7 +6301,7 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>26/01/2024</t>
+          <t>24/01/2024</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
@@ -6310,7 +6310,7 @@
         </is>
       </c>
       <c r="D183" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E183" s="3" t="n">
         <v>-1.83</v>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>07/02/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
@@ -6374,7 +6374,7 @@
         </is>
       </c>
       <c r="D185" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E185" s="3" t="n">
         <v>-13.51</v>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>27/02/2024</t>
+          <t>26/02/2024</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
@@ -6438,7 +6438,7 @@
         </is>
       </c>
       <c r="D187" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E187" s="3" t="n">
         <v>-16.67</v>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>20/03/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
@@ -6502,7 +6502,7 @@
         </is>
       </c>
       <c r="D189" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E189" s="3" t="n">
         <v>-36.91</v>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>08/04/2024</t>
+          <t>01/04/2024</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
@@ -6566,7 +6566,7 @@
         </is>
       </c>
       <c r="D191" s="3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E191" s="3" t="n">
         <v>-25.3</v>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>30/04/2024</t>
+          <t>23/04/2024</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
@@ -6630,7 +6630,7 @@
         </is>
       </c>
       <c r="D193" s="3" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E193" s="3" t="n">
         <v>-11.44</v>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>13/05/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
@@ -6694,7 +6694,7 @@
         </is>
       </c>
       <c r="D195" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E195" s="3" t="n">
         <v>-40.61</v>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>31/05/2024</t>
+          <t>30/05/2024</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
@@ -6758,7 +6758,7 @@
         </is>
       </c>
       <c r="D197" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E197" s="3" t="n">
         <v>-18.49</v>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>25/06/2024</t>
+          <t>24/06/2024</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
@@ -6822,7 +6822,7 @@
         </is>
       </c>
       <c r="D199" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E199" s="3" t="n">
         <v>-15</v>
@@ -6877,7 +6877,7 @@
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>15/07/2024</t>
+          <t>12/07/2024</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
@@ -6886,7 +6886,7 @@
         </is>
       </c>
       <c r="D201" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E201" s="3" t="n">
         <v>-25</v>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>26/07/2024</t>
+          <t>25/07/2024</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
@@ -6950,7 +6950,7 @@
         </is>
       </c>
       <c r="D203" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E203" s="3" t="n">
         <v>-21.96</v>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>08/08/2024</t>
+          <t>07/08/2024</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
@@ -7014,7 +7014,7 @@
         </is>
       </c>
       <c r="D205" s="3" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E205" s="3" t="n">
         <v>-41.02</v>
@@ -7069,7 +7069,7 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
@@ -7078,7 +7078,7 @@
         </is>
       </c>
       <c r="D207" s="3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E207" s="3" t="n">
         <v>-13.79</v>
@@ -7133,7 +7133,7 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="D209" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E209" s="3" t="n">
         <v>-19.44</v>
@@ -7201,7 +7201,7 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>31/12/2024</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
@@ -7210,7 +7210,7 @@
         </is>
       </c>
       <c r="D211" s="3" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E211" s="3" t="n">
         <v>-23.78</v>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>28/01/2025</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
@@ -7274,7 +7274,7 @@
         </is>
       </c>
       <c r="D213" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E213" s="3" t="n">
         <v>-29.05</v>
@@ -7329,7 +7329,7 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
@@ -7338,7 +7338,7 @@
         </is>
       </c>
       <c r="D215" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E215" s="3" t="n">
         <v>-12.23</v>
@@ -7397,7 +7397,7 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>27/03/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
@@ -7406,7 +7406,7 @@
         </is>
       </c>
       <c r="D217" s="3" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E217" s="3" t="n">
         <v>-80.12</v>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>04/04/2025</t>
+          <t>03/04/2025</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
@@ -7470,7 +7470,7 @@
         </is>
       </c>
       <c r="D219" s="3" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E219" s="3" t="n">
         <v>-65.70999999999999</v>
@@ -7529,7 +7529,7 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>01/07/2025</t>
+          <t>30/06/2025</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
@@ -7538,7 +7538,7 @@
         </is>
       </c>
       <c r="D221" s="3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E221" s="3" t="n">
         <v>-18.92</v>
@@ -7593,7 +7593,7 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>23/07/2025</t>
+          <t>22/07/2025</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
@@ -7602,7 +7602,7 @@
         </is>
       </c>
       <c r="D223" s="3" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E223" s="3" t="n">
         <v>-45.56</v>
@@ -7665,7 +7665,7 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>26/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
@@ -7674,7 +7674,7 @@
         </is>
       </c>
       <c r="D225" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E225" s="3" t="n">
         <v>-32.18</v>
@@ -7729,7 +7729,7 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>03/11/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
@@ -7738,7 +7738,7 @@
         </is>
       </c>
       <c r="D227" s="3" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E227" s="3" t="n">
         <v>-56.56</v>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
@@ -7810,7 +7810,7 @@
         </is>
       </c>
       <c r="D229" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E229" s="3" t="n">
         <v>-17.03</v>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="B231" s="3" t="inlineStr">
         <is>
-          <t>23/12/2025</t>
+          <t>22/12/2025</t>
         </is>
       </c>
       <c r="C231" s="3" t="inlineStr">
@@ -7874,7 +7874,7 @@
         </is>
       </c>
       <c r="D231" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E231" s="3" t="n">
         <v>-18.1</v>

</xml_diff>

<commit_message>
Align CSV and JSON data for consistency
Updated the CSV and JSON files to ensure alignment in data structure and content. Adjusted dates and values to match across both formats, improving data accuracy and consistency.

- Modified `blne_rise_events.xlsx` to reflect updated rise and fall data.
- Adjusted `blne_rise_volatility_analysis.json` with corrected dates and values for rise events, dips, and recoveries.
- Removed redundant entries in JSON for mid rises and mid falls.
- Updated `backtest_all_stocks_insider_conviction.py` script to handle aligned data formats effectively.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>25/116</t>
+          <t>23/116</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
@@ -585,7 +585,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>49/116</t>
+          <t>48/116</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>28/116</t>
+          <t>27/116</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
@@ -766,18 +766,18 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>24/08/2017</t>
+          <t>31/07/2017</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>68/116</t>
+          <t>67/116</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>67/116</t>
+          <t>66/116</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
@@ -1022,11 +1022,11 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>30/11/2017</t>
+          <t>17/11/2017</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>44.42</v>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>69/116</t>
+          <t>68/116</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>32/116</t>
+          <t>31/116</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
@@ -1534,22 +1534,22 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>06/07/2018</t>
+          <t>07/06/2018</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>36.63</v>
+        <v>10.04</v>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>23/116</t>
+          <t>72/116</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>122.3</v>
+        <v>95.70999999999999</v>
       </c>
       <c r="H34" s="2" t="n"/>
     </row>
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="G35" s="3" t="n">
-        <v>107.16</v>
+        <v>80.58</v>
       </c>
       <c r="H35" s="3" t="n"/>
     </row>
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>113.53</v>
+        <v>86.95</v>
       </c>
       <c r="H36" s="2" t="n"/>
     </row>
@@ -1645,7 +1645,7 @@
         </is>
       </c>
       <c r="G37" s="3" t="n">
-        <v>98.56</v>
+        <v>71.97</v>
       </c>
       <c r="H37" s="3" t="n"/>
     </row>
@@ -1673,11 +1673,11 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>43/116</t>
+          <t>42/116</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>119.55</v>
+        <v>92.95999999999999</v>
       </c>
       <c r="H38" s="2" t="n"/>
     </row>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="G39" s="3" t="n">
-        <v>107.91</v>
+        <v>81.31999999999999</v>
       </c>
       <c r="H39" s="3" t="n"/>
     </row>
@@ -1741,7 +1741,7 @@
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>115.94</v>
+        <v>89.36</v>
       </c>
       <c r="H40" s="2" t="n"/>
     </row>
@@ -1773,7 +1773,7 @@
         </is>
       </c>
       <c r="G41" s="3" t="n">
-        <v>109.24</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="H41" s="3" t="n"/>
     </row>
@@ -1805,7 +1805,7 @@
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>118.85</v>
+        <v>92.26000000000001</v>
       </c>
       <c r="H42" s="2" t="n"/>
     </row>
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="G43" s="3" t="n">
-        <v>90.53</v>
+        <v>63.94</v>
       </c>
       <c r="H43" s="3" t="n"/>
     </row>
@@ -1869,7 +1869,7 @@
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>96.98</v>
+        <v>70.39</v>
       </c>
       <c r="H44" s="2" t="n"/>
     </row>
@@ -1901,7 +1901,7 @@
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>92.16</v>
+        <v>65.56999999999999</v>
       </c>
       <c r="H45" s="3" t="n"/>
     </row>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>96.73</v>
+        <v>70.14</v>
       </c>
       <c r="H46" s="2" t="n"/>
     </row>
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="G47" s="3" t="n">
-        <v>84.41</v>
+        <v>57.82</v>
       </c>
       <c r="H47" s="3" t="n"/>
     </row>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>93.48</v>
+        <v>66.89</v>
       </c>
       <c r="H48" s="2" t="n"/>
     </row>
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="G49" s="3" t="n">
-        <v>88.09999999999999</v>
+        <v>61.51</v>
       </c>
       <c r="H49" s="3" t="n"/>
     </row>
@@ -2061,7 +2061,7 @@
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>94.13</v>
+        <v>67.54000000000001</v>
       </c>
       <c r="H50" s="2" t="n"/>
     </row>
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="G51" s="3" t="n">
-        <v>88.12</v>
+        <v>61.53</v>
       </c>
       <c r="H51" s="3" t="n"/>
     </row>
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>92.79000000000001</v>
+        <v>66.2</v>
       </c>
       <c r="H52" s="2" t="n"/>
     </row>
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="G53" s="3" t="n">
-        <v>86.01000000000001</v>
+        <v>59.42</v>
       </c>
       <c r="H53" s="3" t="n"/>
     </row>
@@ -2189,7 +2189,7 @@
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>89.73</v>
+        <v>63.15</v>
       </c>
       <c r="H54" s="2" t="n"/>
     </row>
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="G55" s="3" t="n">
-        <v>72.81</v>
+        <v>46.22</v>
       </c>
       <c r="H55" s="3" t="n"/>
     </row>
@@ -2253,7 +2253,7 @@
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>75.69</v>
+        <v>49.1</v>
       </c>
       <c r="H56" s="2" t="n"/>
     </row>
@@ -2285,7 +2285,7 @@
         </is>
       </c>
       <c r="G57" s="3" t="n">
-        <v>66.69</v>
+        <v>40.1</v>
       </c>
       <c r="H57" s="3" t="n"/>
     </row>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>72.19</v>
+        <v>45.6</v>
       </c>
       <c r="H58" s="2" t="n"/>
     </row>
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="G59" s="3" t="n">
-        <v>59.27</v>
+        <v>32.68</v>
       </c>
       <c r="H59" s="3" t="n"/>
     </row>
@@ -2381,7 +2381,7 @@
         </is>
       </c>
       <c r="G60" s="2" t="n">
-        <v>68.12</v>
+        <v>41.53</v>
       </c>
       <c r="H60" s="2" t="n"/>
     </row>
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="G61" s="3" t="n">
-        <v>60.43</v>
+        <v>33.84</v>
       </c>
       <c r="H61" s="3" t="n"/>
     </row>
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="G62" s="2" t="n">
-        <v>68.76000000000001</v>
+        <v>42.17</v>
       </c>
       <c r="H62" s="2" t="n"/>
     </row>
@@ -2477,7 +2477,7 @@
         </is>
       </c>
       <c r="G63" s="3" t="n">
-        <v>49.64</v>
+        <v>23.05</v>
       </c>
       <c r="H63" s="3" t="n"/>
     </row>
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="G64" s="2" t="n">
-        <v>58.5</v>
+        <v>31.91</v>
       </c>
       <c r="H64" s="2" t="n"/>
     </row>
@@ -2541,7 +2541,7 @@
         </is>
       </c>
       <c r="G65" s="3" t="n">
-        <v>51.52</v>
+        <v>24.94</v>
       </c>
       <c r="H65" s="3" t="n"/>
     </row>
@@ -2569,11 +2569,11 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>26/116</t>
+          <t>25/116</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
-        <v>83.77</v>
+        <v>57.19</v>
       </c>
       <c r="H66" s="2" t="n"/>
     </row>
@@ -2605,7 +2605,7 @@
         </is>
       </c>
       <c r="G67" s="3" t="n">
-        <v>71.3</v>
+        <v>44.71</v>
       </c>
       <c r="H67" s="3" t="n"/>
     </row>
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="G68" s="2" t="n">
-        <v>79.29000000000001</v>
+        <v>52.7</v>
       </c>
       <c r="H68" s="2" t="n"/>
     </row>
@@ -2669,7 +2669,7 @@
         </is>
       </c>
       <c r="G69" s="3" t="n">
-        <v>36.89</v>
+        <v>10.3</v>
       </c>
       <c r="H69" s="3" t="n"/>
     </row>
@@ -2701,7 +2701,7 @@
         </is>
       </c>
       <c r="G70" s="2" t="n">
-        <v>40.04</v>
+        <v>13.46</v>
       </c>
       <c r="H70" s="2" t="n"/>
     </row>
@@ -2733,7 +2733,7 @@
         </is>
       </c>
       <c r="G71" s="3" t="n">
-        <v>19.86</v>
+        <v>-6.73</v>
       </c>
       <c r="H71" s="3" t="n"/>
     </row>
@@ -2761,11 +2761,11 @@
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>34/116</t>
+          <t>33/116</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
-        <v>45.91</v>
+        <v>19.33</v>
       </c>
       <c r="H72" s="2" t="n"/>
     </row>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="G73" s="3" t="n">
-        <v>35.58</v>
+        <v>8.99</v>
       </c>
       <c r="H73" s="3" t="n"/>
     </row>
@@ -2825,11 +2825,11 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>60/116</t>
+          <t>59/116</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
-        <v>51.17</v>
+        <v>24.58</v>
       </c>
       <c r="H74" s="2" t="n"/>
     </row>
@@ -2861,7 +2861,7 @@
         </is>
       </c>
       <c r="G75" s="3" t="n">
-        <v>40.32</v>
+        <v>13.73</v>
       </c>
       <c r="H75" s="3" t="n"/>
     </row>
@@ -2889,11 +2889,11 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>41/116</t>
+          <t>40/116</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
-        <v>61.68</v>
+        <v>35.09</v>
       </c>
       <c r="H76" s="2" t="n"/>
     </row>
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="G77" s="3" t="n">
-        <v>56.08</v>
+        <v>29.49</v>
       </c>
       <c r="H77" s="3" t="n"/>
     </row>
@@ -2957,7 +2957,7 @@
         </is>
       </c>
       <c r="G78" s="2" t="n">
-        <v>60.6</v>
+        <v>34.01</v>
       </c>
       <c r="H78" s="2" t="n"/>
     </row>
@@ -2989,7 +2989,7 @@
         </is>
       </c>
       <c r="G79" s="3" t="n">
-        <v>-12.37</v>
+        <v>-38.96</v>
       </c>
       <c r="H79" s="3" t="n"/>
     </row>
@@ -3021,7 +3021,7 @@
         </is>
       </c>
       <c r="G80" s="2" t="n">
-        <v>87.63</v>
+        <v>61.04</v>
       </c>
       <c r="H80" s="2" t="n"/>
     </row>
@@ -3053,7 +3053,7 @@
         </is>
       </c>
       <c r="G81" s="3" t="n">
-        <v>78.13</v>
+        <v>51.54</v>
       </c>
       <c r="H81" s="3" t="n"/>
     </row>
@@ -3085,7 +3085,7 @@
         </is>
       </c>
       <c r="G82" s="2" t="n">
-        <v>84.76000000000001</v>
+        <v>58.17</v>
       </c>
       <c r="H82" s="2" t="n"/>
     </row>
@@ -3117,7 +3117,7 @@
         </is>
       </c>
       <c r="G83" s="3" t="n">
-        <v>57.3</v>
+        <v>30.71</v>
       </c>
       <c r="H83" s="3" t="n"/>
     </row>
@@ -3145,11 +3145,11 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>39/116</t>
+          <t>38/116</t>
         </is>
       </c>
       <c r="G84" s="2" t="n">
-        <v>80.87</v>
+        <v>54.28</v>
       </c>
       <c r="H84" s="2" t="n"/>
     </row>
@@ -3181,7 +3181,7 @@
         </is>
       </c>
       <c r="G85" s="3" t="n">
-        <v>59.48</v>
+        <v>32.89</v>
       </c>
       <c r="H85" s="3" t="n"/>
     </row>
@@ -3209,11 +3209,11 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>65/116</t>
+          <t>64/116</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
-        <v>72.34999999999999</v>
+        <v>45.76</v>
       </c>
       <c r="H86" s="2" t="n"/>
     </row>
@@ -3245,7 +3245,7 @@
         </is>
       </c>
       <c r="G87" s="3" t="n">
-        <v>53.78</v>
+        <v>27.19</v>
       </c>
       <c r="H87" s="3" t="n"/>
     </row>
@@ -3277,7 +3277,7 @@
         </is>
       </c>
       <c r="G88" s="2" t="n">
-        <v>62.58</v>
+        <v>35.99</v>
       </c>
       <c r="H88" s="2" t="n"/>
     </row>
@@ -3309,7 +3309,7 @@
         </is>
       </c>
       <c r="G89" s="3" t="n">
-        <v>41.99</v>
+        <v>15.41</v>
       </c>
       <c r="H89" s="3" t="n"/>
     </row>
@@ -3337,11 +3337,11 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>51/116</t>
+          <t>50/116</t>
         </is>
       </c>
       <c r="G90" s="2" t="n">
-        <v>59.11</v>
+        <v>32.52</v>
       </c>
       <c r="H90" s="2" t="n"/>
     </row>
@@ -3373,7 +3373,7 @@
         </is>
       </c>
       <c r="G91" s="3" t="n">
-        <v>48.34</v>
+        <v>21.75</v>
       </c>
       <c r="H91" s="3" t="n"/>
     </row>
@@ -3405,7 +3405,7 @@
         </is>
       </c>
       <c r="G92" s="2" t="n">
-        <v>101.79</v>
+        <v>75.2</v>
       </c>
       <c r="H92" s="2" t="n"/>
     </row>
@@ -3437,7 +3437,7 @@
         </is>
       </c>
       <c r="G93" s="3" t="n">
-        <v>61.9</v>
+        <v>35.31</v>
       </c>
       <c r="H93" s="3" t="n"/>
     </row>
@@ -3465,11 +3465,11 @@
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>62/116</t>
+          <t>61/116</t>
         </is>
       </c>
       <c r="G94" s="2" t="n">
-        <v>75.92</v>
+        <v>49.33</v>
       </c>
       <c r="H94" s="2" t="n"/>
     </row>
@@ -3501,7 +3501,7 @@
         </is>
       </c>
       <c r="G95" s="3" t="n">
-        <v>69.36</v>
+        <v>42.78</v>
       </c>
       <c r="H95" s="3" t="n"/>
     </row>
@@ -3529,11 +3529,11 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>58/116</t>
+          <t>57/116</t>
         </is>
       </c>
       <c r="G96" s="2" t="n">
-        <v>85.15000000000001</v>
+        <v>58.57</v>
       </c>
       <c r="H96" s="2" t="n"/>
     </row>
@@ -3565,7 +3565,7 @@
         </is>
       </c>
       <c r="G97" s="3" t="n">
-        <v>79.09</v>
+        <v>52.5</v>
       </c>
       <c r="H97" s="3" t="n"/>
     </row>
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="G98" s="2" t="n">
-        <v>132.32</v>
+        <v>105.73</v>
       </c>
       <c r="H98" s="2" t="n"/>
     </row>
@@ -3629,7 +3629,7 @@
         </is>
       </c>
       <c r="G99" s="3" t="n">
-        <v>111.79</v>
+        <v>85.2</v>
       </c>
       <c r="H99" s="3" t="n"/>
     </row>
@@ -3661,7 +3661,7 @@
         </is>
       </c>
       <c r="G100" s="2" t="n">
-        <v>120.23</v>
+        <v>93.65000000000001</v>
       </c>
       <c r="H100" s="2" t="n"/>
     </row>
@@ -3693,7 +3693,7 @@
         </is>
       </c>
       <c r="G101" s="3" t="n">
-        <v>94.48999999999999</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="H101" s="3" t="n"/>
     </row>
@@ -3725,7 +3725,7 @@
         </is>
       </c>
       <c r="G102" s="2" t="n">
-        <v>214.65</v>
+        <v>188.06</v>
       </c>
       <c r="H102" s="2" t="n"/>
     </row>
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="G103" s="3" t="n">
-        <v>182.05</v>
+        <v>155.46</v>
       </c>
       <c r="H103" s="3" t="n"/>
     </row>
@@ -3785,11 +3785,11 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>70/116</t>
+          <t>69/116</t>
         </is>
       </c>
       <c r="G104" s="2" t="n">
-        <v>193.46</v>
+        <v>166.87</v>
       </c>
       <c r="H104" s="2" t="n"/>
     </row>
@@ -3821,7 +3821,7 @@
         </is>
       </c>
       <c r="G105" s="3" t="n">
-        <v>179.8</v>
+        <v>153.21</v>
       </c>
       <c r="H105" s="3" t="n"/>
     </row>
@@ -3849,11 +3849,11 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>57/116</t>
+          <t>56/116</t>
         </is>
       </c>
       <c r="G106" s="2" t="n">
-        <v>195.62</v>
+        <v>169.03</v>
       </c>
       <c r="H106" s="2" t="n"/>
     </row>
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="G107" s="3" t="n">
-        <v>172.69</v>
+        <v>146.1</v>
       </c>
       <c r="H107" s="3" t="n"/>
     </row>
@@ -3913,11 +3913,11 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>56/116</t>
+          <t>55/116</t>
         </is>
       </c>
       <c r="G108" s="2" t="n">
-        <v>188.52</v>
+        <v>161.93</v>
       </c>
       <c r="H108" s="2" t="n"/>
     </row>
@@ -3949,7 +3949,7 @@
         </is>
       </c>
       <c r="G109" s="3" t="n">
-        <v>179.77</v>
+        <v>153.18</v>
       </c>
       <c r="H109" s="3" t="n"/>
     </row>
@@ -3981,7 +3981,7 @@
         </is>
       </c>
       <c r="G110" s="2" t="n">
-        <v>271.39</v>
+        <v>244.8</v>
       </c>
       <c r="H110" s="2" t="n"/>
     </row>
@@ -4013,7 +4013,7 @@
         </is>
       </c>
       <c r="G111" s="3" t="n">
-        <v>259.2</v>
+        <v>232.61</v>
       </c>
       <c r="H111" s="3" t="n"/>
     </row>
@@ -4045,7 +4045,7 @@
         </is>
       </c>
       <c r="G112" s="2" t="n">
-        <v>266.95</v>
+        <v>240.36</v>
       </c>
       <c r="H112" s="2" t="n"/>
     </row>
@@ -4077,7 +4077,7 @@
         </is>
       </c>
       <c r="G113" s="3" t="n">
-        <v>259.1</v>
+        <v>232.52</v>
       </c>
       <c r="H113" s="3" t="n"/>
     </row>
@@ -4105,11 +4105,11 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>29/116</t>
+          <t>28/116</t>
         </is>
       </c>
       <c r="G114" s="2" t="n">
-        <v>289.25</v>
+        <v>262.66</v>
       </c>
       <c r="H114" s="2" t="n"/>
     </row>
@@ -4141,7 +4141,7 @@
         </is>
       </c>
       <c r="G115" s="3" t="n">
-        <v>285.7</v>
+        <v>259.12</v>
       </c>
       <c r="H115" s="3" t="n"/>
     </row>
@@ -4169,11 +4169,11 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t>27/116</t>
+          <t>26/116</t>
         </is>
       </c>
       <c r="G116" s="2" t="n">
-        <v>317.63</v>
+        <v>291.04</v>
       </c>
       <c r="H116" s="2" t="n"/>
     </row>
@@ -4205,7 +4205,7 @@
         </is>
       </c>
       <c r="G117" s="3" t="n">
-        <v>299</v>
+        <v>272.41</v>
       </c>
       <c r="H117" s="3" t="n"/>
     </row>
@@ -4237,7 +4237,7 @@
         </is>
       </c>
       <c r="G118" s="2" t="n">
-        <v>303.21</v>
+        <v>276.62</v>
       </c>
       <c r="H118" s="2" t="n"/>
     </row>
@@ -4269,7 +4269,7 @@
         </is>
       </c>
       <c r="G119" s="3" t="n">
-        <v>276.19</v>
+        <v>249.6</v>
       </c>
       <c r="H119" s="3" t="n"/>
     </row>
@@ -4301,7 +4301,7 @@
         </is>
       </c>
       <c r="G120" s="2" t="n">
-        <v>285.53</v>
+        <v>258.94</v>
       </c>
       <c r="H120" s="2" t="n"/>
     </row>
@@ -4333,7 +4333,7 @@
         </is>
       </c>
       <c r="G121" s="3" t="n">
-        <v>264.64</v>
+        <v>238.05</v>
       </c>
       <c r="H121" s="3" t="n"/>
     </row>
@@ -4361,11 +4361,11 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>53/116</t>
+          <t>52/116</t>
         </is>
       </c>
       <c r="G122" s="2" t="n">
-        <v>281.04</v>
+        <v>254.45</v>
       </c>
       <c r="H122" s="2" t="n"/>
     </row>
@@ -4397,7 +4397,7 @@
         </is>
       </c>
       <c r="G123" s="3" t="n">
-        <v>271.08</v>
+        <v>244.49</v>
       </c>
       <c r="H123" s="3" t="n"/>
     </row>
@@ -4429,7 +4429,7 @@
         </is>
       </c>
       <c r="G124" s="2" t="n">
-        <v>281</v>
+        <v>254.41</v>
       </c>
       <c r="H124" s="2" t="n"/>
     </row>
@@ -4461,7 +4461,7 @@
         </is>
       </c>
       <c r="G125" s="3" t="n">
-        <v>247.32</v>
+        <v>220.73</v>
       </c>
       <c r="H125" s="3" t="n"/>
     </row>
@@ -4493,7 +4493,7 @@
         </is>
       </c>
       <c r="G126" s="2" t="n">
-        <v>253.6</v>
+        <v>227.01</v>
       </c>
       <c r="H126" s="2" t="n"/>
     </row>
@@ -4525,7 +4525,7 @@
         </is>
       </c>
       <c r="G127" s="3" t="n">
-        <v>237.84</v>
+        <v>211.25</v>
       </c>
       <c r="H127" s="3" t="n"/>
     </row>
@@ -4553,11 +4553,11 @@
       </c>
       <c r="F128" s="2" t="inlineStr">
         <is>
-          <t>44/116</t>
+          <t>43/116</t>
         </is>
       </c>
       <c r="G128" s="2" t="n">
-        <v>258.31</v>
+        <v>231.72</v>
       </c>
       <c r="H128" s="2" t="n"/>
     </row>
@@ -4589,7 +4589,7 @@
         </is>
       </c>
       <c r="G129" s="3" t="n">
-        <v>206.85</v>
+        <v>180.26</v>
       </c>
       <c r="H129" s="3" t="n"/>
     </row>
@@ -4617,11 +4617,11 @@
       </c>
       <c r="F130" s="2" t="inlineStr">
         <is>
-          <t>42/116</t>
+          <t>41/116</t>
         </is>
       </c>
       <c r="G130" s="2" t="n">
-        <v>227.85</v>
+        <v>201.26</v>
       </c>
       <c r="H130" s="2" t="n"/>
     </row>
@@ -4653,7 +4653,7 @@
         </is>
       </c>
       <c r="G131" s="3" t="n">
-        <v>207.19</v>
+        <v>180.6</v>
       </c>
       <c r="H131" s="3" t="n"/>
     </row>
@@ -4681,11 +4681,11 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>63/116</t>
+          <t>62/116</t>
         </is>
       </c>
       <c r="G132" s="2" t="n">
-        <v>220.73</v>
+        <v>194.14</v>
       </c>
       <c r="H132" s="2" t="n"/>
     </row>
@@ -4717,7 +4717,7 @@
         </is>
       </c>
       <c r="G133" s="3" t="n">
-        <v>202.38</v>
+        <v>175.79</v>
       </c>
       <c r="H133" s="3" t="n"/>
     </row>
@@ -4749,7 +4749,7 @@
         </is>
       </c>
       <c r="G134" s="2" t="n">
-        <v>254.07</v>
+        <v>227.48</v>
       </c>
       <c r="H134" s="2" t="inlineStr">
         <is>
@@ -4785,7 +4785,7 @@
         </is>
       </c>
       <c r="G135" s="3" t="n">
-        <v>218.51</v>
+        <v>191.92</v>
       </c>
       <c r="H135" s="3" t="n"/>
     </row>
@@ -4817,7 +4817,7 @@
         </is>
       </c>
       <c r="G136" s="2" t="n">
-        <v>223.64</v>
+        <v>197.06</v>
       </c>
       <c r="H136" s="2" t="n"/>
     </row>
@@ -4849,7 +4849,7 @@
         </is>
       </c>
       <c r="G137" s="3" t="n">
-        <v>192.18</v>
+        <v>165.59</v>
       </c>
       <c r="H137" s="3" t="n"/>
     </row>
@@ -4881,7 +4881,7 @@
         </is>
       </c>
       <c r="G138" s="2" t="n">
-        <v>199.53</v>
+        <v>172.94</v>
       </c>
       <c r="H138" s="2" t="n"/>
     </row>
@@ -4913,7 +4913,7 @@
         </is>
       </c>
       <c r="G139" s="3" t="n">
-        <v>181.72</v>
+        <v>155.14</v>
       </c>
       <c r="H139" s="3" t="n"/>
     </row>
@@ -4941,11 +4941,11 @@
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>45/116</t>
+          <t>44/116</t>
         </is>
       </c>
       <c r="G140" s="2" t="n">
-        <v>200.89</v>
+        <v>174.3</v>
       </c>
       <c r="H140" s="2" t="n"/>
     </row>
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="G141" s="3" t="n">
-        <v>184.54</v>
+        <v>157.95</v>
       </c>
       <c r="H141" s="3" t="n"/>
     </row>
@@ -5005,11 +5005,11 @@
       </c>
       <c r="F142" s="2" t="inlineStr">
         <is>
-          <t>64/116</t>
+          <t>63/116</t>
         </is>
       </c>
       <c r="G142" s="2" t="n">
-        <v>197.62</v>
+        <v>171.03</v>
       </c>
       <c r="H142" s="2" t="n"/>
     </row>
@@ -5041,7 +5041,7 @@
         </is>
       </c>
       <c r="G143" s="3" t="n">
-        <v>184.76</v>
+        <v>158.18</v>
       </c>
       <c r="H143" s="3" t="n"/>
     </row>
@@ -5069,11 +5069,11 @@
       </c>
       <c r="F144" s="2" t="inlineStr">
         <is>
-          <t>47/116</t>
+          <t>46/116</t>
         </is>
       </c>
       <c r="G144" s="2" t="n">
-        <v>202.8</v>
+        <v>176.21</v>
       </c>
       <c r="H144" s="2" t="n"/>
     </row>
@@ -5105,7 +5105,7 @@
         </is>
       </c>
       <c r="G145" s="3" t="n">
-        <v>155.16</v>
+        <v>128.57</v>
       </c>
       <c r="H145" s="3" t="n"/>
     </row>
@@ -5133,11 +5133,11 @@
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>52/116</t>
+          <t>51/116</t>
         </is>
       </c>
       <c r="G146" s="2" t="n">
-        <v>172.04</v>
+        <v>145.45</v>
       </c>
       <c r="H146" s="2" t="n"/>
     </row>
@@ -5169,7 +5169,7 @@
         </is>
       </c>
       <c r="G147" s="3" t="n">
-        <v>131.15</v>
+        <v>104.56</v>
       </c>
       <c r="H147" s="3" t="n"/>
     </row>
@@ -5197,11 +5197,11 @@
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>50/116</t>
+          <t>49/116</t>
         </is>
       </c>
       <c r="G148" s="2" t="n">
-        <v>148.33</v>
+        <v>121.75</v>
       </c>
       <c r="H148" s="2" t="n"/>
     </row>
@@ -5233,7 +5233,7 @@
         </is>
       </c>
       <c r="G149" s="3" t="n">
-        <v>133.38</v>
+        <v>106.79</v>
       </c>
       <c r="H149" s="3" t="n"/>
     </row>
@@ -5250,11 +5250,11 @@
       </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>11/11/2022</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="D150" s="2" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E150" s="2" t="n">
         <v>3.96</v>
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="G150" s="2" t="n">
-        <v>137.34</v>
+        <v>110.75</v>
       </c>
       <c r="H150" s="2" t="n"/>
     </row>
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="G151" s="3" t="n">
-        <v>108.77</v>
+        <v>82.18000000000001</v>
       </c>
       <c r="H151" s="3" t="n"/>
     </row>
@@ -5325,11 +5325,11 @@
       </c>
       <c r="F152" s="2" t="inlineStr">
         <is>
-          <t>31/116</t>
+          <t>30/116</t>
         </is>
       </c>
       <c r="G152" s="2" t="n">
-        <v>135.43</v>
+        <v>108.85</v>
       </c>
       <c r="H152" s="2" t="n"/>
     </row>
@@ -5361,7 +5361,7 @@
         </is>
       </c>
       <c r="G153" s="3" t="n">
-        <v>124.21</v>
+        <v>97.62</v>
       </c>
       <c r="H153" s="3" t="n"/>
     </row>
@@ -5393,7 +5393,7 @@
         </is>
       </c>
       <c r="G154" s="2" t="n">
-        <v>202.95</v>
+        <v>176.36</v>
       </c>
       <c r="H154" s="2" t="n"/>
     </row>
@@ -5425,7 +5425,7 @@
         </is>
       </c>
       <c r="G155" s="3" t="n">
-        <v>167.04</v>
+        <v>140.45</v>
       </c>
       <c r="H155" s="3" t="n"/>
     </row>
@@ -5453,11 +5453,11 @@
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>61/116</t>
+          <t>60/116</t>
         </is>
       </c>
       <c r="G156" s="2" t="n">
-        <v>181.82</v>
+        <v>155.23</v>
       </c>
       <c r="H156" s="2" t="n"/>
     </row>
@@ -5489,7 +5489,7 @@
         </is>
       </c>
       <c r="G157" s="3" t="n">
-        <v>161.46</v>
+        <v>134.87</v>
       </c>
       <c r="H157" s="3" t="n"/>
     </row>
@@ -5521,7 +5521,7 @@
         </is>
       </c>
       <c r="G158" s="2" t="n">
-        <v>171.23</v>
+        <v>144.65</v>
       </c>
       <c r="H158" s="2" t="n"/>
     </row>
@@ -5553,7 +5553,7 @@
         </is>
       </c>
       <c r="G159" s="3" t="n">
-        <v>149.66</v>
+        <v>123.07</v>
       </c>
       <c r="H159" s="3" t="n"/>
     </row>
@@ -5585,7 +5585,7 @@
         </is>
       </c>
       <c r="G160" s="2" t="n">
-        <v>202.5</v>
+        <v>175.91</v>
       </c>
       <c r="H160" s="2" t="n"/>
     </row>
@@ -5617,7 +5617,7 @@
         </is>
       </c>
       <c r="G161" s="3" t="n">
-        <v>158.5</v>
+        <v>131.91</v>
       </c>
       <c r="H161" s="3" t="n"/>
     </row>
@@ -5649,7 +5649,7 @@
         </is>
       </c>
       <c r="G162" s="2" t="n">
-        <v>163.09</v>
+        <v>136.5</v>
       </c>
       <c r="H162" s="2" t="n"/>
     </row>
@@ -5681,7 +5681,7 @@
         </is>
       </c>
       <c r="G163" s="3" t="n">
-        <v>147.48</v>
+        <v>120.89</v>
       </c>
       <c r="H163" s="3" t="n"/>
     </row>
@@ -5713,7 +5713,7 @@
         </is>
       </c>
       <c r="G164" s="2" t="n">
-        <v>185.77</v>
+        <v>159.18</v>
       </c>
       <c r="H164" s="2" t="n"/>
     </row>
@@ -5745,7 +5745,7 @@
         </is>
       </c>
       <c r="G165" s="3" t="n">
-        <v>160.33</v>
+        <v>133.74</v>
       </c>
       <c r="H165" s="3" t="n"/>
     </row>
@@ -5773,11 +5773,11 @@
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>46/116</t>
+          <t>45/116</t>
         </is>
       </c>
       <c r="G166" s="2" t="n">
-        <v>179.48</v>
+        <v>152.89</v>
       </c>
       <c r="H166" s="2" t="n"/>
     </row>
@@ -5809,7 +5809,7 @@
         </is>
       </c>
       <c r="G167" s="3" t="n">
-        <v>152.97</v>
+        <v>126.38</v>
       </c>
       <c r="H167" s="3" t="n"/>
     </row>
@@ -5841,7 +5841,7 @@
         </is>
       </c>
       <c r="G168" s="2" t="n">
-        <v>240.62</v>
+        <v>214.03</v>
       </c>
       <c r="H168" s="2" t="n"/>
     </row>
@@ -5873,7 +5873,7 @@
         </is>
       </c>
       <c r="G169" s="3" t="n">
-        <v>190.22</v>
+        <v>163.63</v>
       </c>
       <c r="H169" s="3" t="n"/>
     </row>
@@ -5905,7 +5905,7 @@
         </is>
       </c>
       <c r="G170" s="2" t="n">
-        <v>200.12</v>
+        <v>173.53</v>
       </c>
       <c r="H170" s="2" t="n"/>
     </row>
@@ -5937,7 +5937,7 @@
         </is>
       </c>
       <c r="G171" s="3" t="n">
-        <v>186.75</v>
+        <v>160.16</v>
       </c>
       <c r="H171" s="3" t="n"/>
     </row>
@@ -5965,11 +5965,11 @@
       </c>
       <c r="F172" s="2" t="inlineStr">
         <is>
-          <t>66/116</t>
+          <t>65/116</t>
         </is>
       </c>
       <c r="G172" s="2" t="n">
-        <v>199.5</v>
+        <v>172.91</v>
       </c>
       <c r="H172" s="2" t="n"/>
     </row>
@@ -6001,7 +6001,7 @@
         </is>
       </c>
       <c r="G173" s="3" t="n">
-        <v>136.7</v>
+        <v>110.11</v>
       </c>
       <c r="H173" s="3" t="n"/>
     </row>
@@ -6033,7 +6033,7 @@
         </is>
       </c>
       <c r="G174" s="2" t="n">
-        <v>186.3</v>
+        <v>159.71</v>
       </c>
       <c r="H174" s="2" t="n"/>
     </row>
@@ -6065,7 +6065,7 @@
         </is>
       </c>
       <c r="G175" s="3" t="n">
-        <v>184.16</v>
+        <v>157.57</v>
       </c>
       <c r="H175" s="3" t="n"/>
     </row>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="G176" s="2" t="n">
-        <v>192.36</v>
+        <v>165.77</v>
       </c>
       <c r="H176" s="2" t="n"/>
     </row>
@@ -6129,7 +6129,7 @@
         </is>
       </c>
       <c r="G177" s="3" t="n">
-        <v>158.02</v>
+        <v>131.43</v>
       </c>
       <c r="H177" s="3" t="n"/>
     </row>
@@ -6157,11 +6157,11 @@
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>59/116</t>
+          <t>58/116</t>
         </is>
       </c>
       <c r="G178" s="2" t="n">
-        <v>173.62</v>
+        <v>147.03</v>
       </c>
       <c r="H178" s="2" t="n"/>
     </row>
@@ -6193,7 +6193,7 @@
         </is>
       </c>
       <c r="G179" s="3" t="n">
-        <v>129.45</v>
+        <v>102.86</v>
       </c>
       <c r="H179" s="3" t="n"/>
     </row>
@@ -6210,14 +6210,14 @@
       </c>
       <c r="C180" s="2" t="inlineStr">
         <is>
-          <t>09/01/2024</t>
+          <t>30/11/2023</t>
         </is>
       </c>
       <c r="D180" s="2" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="E180" s="2" t="n">
-        <v>36.32</v>
+        <v>34.74</v>
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
@@ -6225,7 +6225,7 @@
         </is>
       </c>
       <c r="G180" s="2" t="n">
-        <v>165.76</v>
+        <v>137.6</v>
       </c>
       <c r="H180" s="2" t="n"/>
     </row>
@@ -6257,7 +6257,7 @@
         </is>
       </c>
       <c r="G181" s="3" t="n">
-        <v>148.39</v>
+        <v>120.22</v>
       </c>
       <c r="H181" s="3" t="n"/>
     </row>
@@ -6289,7 +6289,7 @@
         </is>
       </c>
       <c r="G182" s="2" t="n">
-        <v>150.26</v>
+        <v>122.09</v>
       </c>
       <c r="H182" s="2" t="n"/>
     </row>
@@ -6321,7 +6321,7 @@
         </is>
       </c>
       <c r="G183" s="3" t="n">
-        <v>148.42</v>
+        <v>120.26</v>
       </c>
       <c r="H183" s="3" t="n"/>
     </row>
@@ -6353,7 +6353,7 @@
         </is>
       </c>
       <c r="G184" s="2" t="n">
-        <v>156.37</v>
+        <v>128.2</v>
       </c>
       <c r="H184" s="2" t="n"/>
     </row>
@@ -6385,7 +6385,7 @@
         </is>
       </c>
       <c r="G185" s="3" t="n">
-        <v>142.86</v>
+        <v>114.69</v>
       </c>
       <c r="H185" s="3" t="n"/>
     </row>
@@ -6413,11 +6413,11 @@
       </c>
       <c r="F186" s="2" t="inlineStr">
         <is>
-          <t>33/116</t>
+          <t>32/116</t>
         </is>
       </c>
       <c r="G186" s="2" t="n">
-        <v>168.99</v>
+        <v>140.82</v>
       </c>
       <c r="H186" s="2" t="n"/>
     </row>
@@ -6449,7 +6449,7 @@
         </is>
       </c>
       <c r="G187" s="3" t="n">
-        <v>152.32</v>
+        <v>124.15</v>
       </c>
       <c r="H187" s="3" t="n"/>
     </row>
@@ -6481,7 +6481,7 @@
         </is>
       </c>
       <c r="G188" s="2" t="n">
-        <v>193.95</v>
+        <v>165.79</v>
       </c>
       <c r="H188" s="2" t="n"/>
     </row>
@@ -6513,7 +6513,7 @@
         </is>
       </c>
       <c r="G189" s="3" t="n">
-        <v>157.04</v>
+        <v>128.88</v>
       </c>
       <c r="H189" s="3" t="n"/>
     </row>
@@ -6541,11 +6541,11 @@
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>36/116</t>
+          <t>35/116</t>
         </is>
       </c>
       <c r="G190" s="2" t="n">
-        <v>181.51</v>
+        <v>153.34</v>
       </c>
       <c r="H190" s="2" t="n"/>
     </row>
@@ -6577,7 +6577,7 @@
         </is>
       </c>
       <c r="G191" s="3" t="n">
-        <v>156.21</v>
+        <v>128.04</v>
       </c>
       <c r="H191" s="3" t="n"/>
     </row>
@@ -6605,11 +6605,11 @@
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>37/116</t>
+          <t>36/116</t>
         </is>
       </c>
       <c r="G192" s="2" t="n">
-        <v>180.24</v>
+        <v>152.07</v>
       </c>
       <c r="H192" s="2" t="n"/>
     </row>
@@ -6641,7 +6641,7 @@
         </is>
       </c>
       <c r="G193" s="3" t="n">
-        <v>168.8</v>
+        <v>140.63</v>
       </c>
       <c r="H193" s="3" t="n"/>
     </row>
@@ -6673,7 +6673,7 @@
         </is>
       </c>
       <c r="G194" s="2" t="n">
-        <v>238.59</v>
+        <v>210.42</v>
       </c>
       <c r="H194" s="2" t="n"/>
     </row>
@@ -6705,7 +6705,7 @@
         </is>
       </c>
       <c r="G195" s="3" t="n">
-        <v>197.98</v>
+        <v>169.81</v>
       </c>
       <c r="H195" s="3" t="n"/>
     </row>
@@ -6733,11 +6733,11 @@
       </c>
       <c r="F196" s="2" t="inlineStr">
         <is>
-          <t>40/116</t>
+          <t>39/116</t>
         </is>
       </c>
       <c r="G196" s="2" t="n">
-        <v>220.91</v>
+        <v>192.74</v>
       </c>
       <c r="H196" s="2" t="n"/>
     </row>
@@ -6769,7 +6769,7 @@
         </is>
       </c>
       <c r="G197" s="3" t="n">
-        <v>202.42</v>
+        <v>174.26</v>
       </c>
       <c r="H197" s="3" t="n"/>
     </row>
@@ -6797,11 +6797,11 @@
       </c>
       <c r="F198" s="2" t="inlineStr">
         <is>
-          <t>48/116</t>
+          <t>47/116</t>
         </is>
       </c>
       <c r="G198" s="2" t="n">
-        <v>219.95</v>
+        <v>191.78</v>
       </c>
       <c r="H198" s="2" t="n"/>
     </row>
@@ -6833,7 +6833,7 @@
         </is>
       </c>
       <c r="G199" s="3" t="n">
-        <v>204.95</v>
+        <v>176.78</v>
       </c>
       <c r="H199" s="3" t="n"/>
     </row>
@@ -6861,11 +6861,11 @@
       </c>
       <c r="F200" s="2" t="inlineStr">
         <is>
-          <t>38/116</t>
+          <t>37/116</t>
         </is>
       </c>
       <c r="G200" s="2" t="n">
-        <v>228.79</v>
+        <v>200.62</v>
       </c>
       <c r="H200" s="2" t="n"/>
     </row>
@@ -6897,7 +6897,7 @@
         </is>
       </c>
       <c r="G201" s="3" t="n">
-        <v>203.79</v>
+        <v>175.62</v>
       </c>
       <c r="H201" s="3" t="n"/>
     </row>
@@ -6929,7 +6929,7 @@
         </is>
       </c>
       <c r="G202" s="2" t="n">
-        <v>210.57</v>
+        <v>182.4</v>
       </c>
       <c r="H202" s="2" t="n"/>
     </row>
@@ -6961,7 +6961,7 @@
         </is>
       </c>
       <c r="G203" s="3" t="n">
-        <v>188.61</v>
+        <v>160.44</v>
       </c>
       <c r="H203" s="3" t="n"/>
     </row>
@@ -6993,7 +6993,7 @@
         </is>
       </c>
       <c r="G204" s="2" t="n">
-        <v>198.48</v>
+        <v>170.31</v>
       </c>
       <c r="H204" s="2" t="n"/>
     </row>
@@ -7025,7 +7025,7 @@
         </is>
       </c>
       <c r="G205" s="3" t="n">
-        <v>157.46</v>
+        <v>129.29</v>
       </c>
       <c r="H205" s="3" t="n"/>
     </row>
@@ -7053,11 +7053,11 @@
       </c>
       <c r="F206" s="2" t="inlineStr">
         <is>
-          <t>54/116</t>
+          <t>53/116</t>
         </is>
       </c>
       <c r="G206" s="2" t="n">
-        <v>173.46</v>
+        <v>145.29</v>
       </c>
       <c r="H206" s="2" t="n"/>
     </row>
@@ -7089,7 +7089,7 @@
         </is>
       </c>
       <c r="G207" s="3" t="n">
-        <v>159.66</v>
+        <v>131.5</v>
       </c>
       <c r="H207" s="3" t="n"/>
     </row>
@@ -7117,11 +7117,11 @@
       </c>
       <c r="F208" s="2" t="inlineStr">
         <is>
-          <t>71/116</t>
+          <t>70/116</t>
         </is>
       </c>
       <c r="G208" s="2" t="n">
-        <v>171</v>
+        <v>142.84</v>
       </c>
       <c r="H208" s="2" t="n"/>
     </row>
@@ -7153,7 +7153,7 @@
         </is>
       </c>
       <c r="G209" s="3" t="n">
-        <v>151.56</v>
+        <v>123.39</v>
       </c>
       <c r="H209" s="3" t="n"/>
     </row>
@@ -7185,7 +7185,7 @@
         </is>
       </c>
       <c r="G210" s="2" t="n">
-        <v>236.04</v>
+        <v>207.88</v>
       </c>
       <c r="H210" s="2" t="inlineStr">
         <is>
@@ -7221,7 +7221,7 @@
         </is>
       </c>
       <c r="G211" s="3" t="n">
-        <v>212.26</v>
+        <v>184.1</v>
       </c>
       <c r="H211" s="3" t="n"/>
     </row>
@@ -7249,11 +7249,11 @@
       </c>
       <c r="F212" s="2" t="inlineStr">
         <is>
-          <t>35/116</t>
+          <t>34/116</t>
         </is>
       </c>
       <c r="G212" s="2" t="n">
-        <v>237.26</v>
+        <v>209.1</v>
       </c>
       <c r="H212" s="2" t="n"/>
     </row>
@@ -7285,7 +7285,7 @@
         </is>
       </c>
       <c r="G213" s="3" t="n">
-        <v>208.21</v>
+        <v>180.04</v>
       </c>
       <c r="H213" s="3" t="n"/>
     </row>
@@ -7317,7 +7317,7 @@
         </is>
       </c>
       <c r="G214" s="2" t="n">
-        <v>217.41</v>
+        <v>189.24</v>
       </c>
       <c r="H214" s="2" t="n"/>
     </row>
@@ -7349,7 +7349,7 @@
         </is>
       </c>
       <c r="G215" s="3" t="n">
-        <v>205.18</v>
+        <v>177.01</v>
       </c>
       <c r="H215" s="3" t="n"/>
     </row>
@@ -7366,22 +7366,22 @@
       </c>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>26/03/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="D216" s="2" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E216" s="2" t="n">
         <v>26.93</v>
       </c>
       <c r="F216" s="2" t="inlineStr">
         <is>
-          <t>30/116</t>
+          <t>29/116</t>
         </is>
       </c>
       <c r="G216" s="2" t="n">
-        <v>232.12</v>
+        <v>203.95</v>
       </c>
       <c r="H216" s="2" t="inlineStr">
         <is>
@@ -7417,7 +7417,7 @@
         </is>
       </c>
       <c r="G217" s="3" t="n">
-        <v>151.99</v>
+        <v>123.83</v>
       </c>
       <c r="H217" s="3" t="n"/>
     </row>
@@ -7445,11 +7445,11 @@
       </c>
       <c r="F218" s="2" t="inlineStr">
         <is>
-          <t>55/116</t>
+          <t>54/116</t>
         </is>
       </c>
       <c r="G218" s="2" t="n">
-        <v>167.94</v>
+        <v>139.78</v>
       </c>
       <c r="H218" s="2" t="n"/>
     </row>
@@ -7481,7 +7481,7 @@
         </is>
       </c>
       <c r="G219" s="3" t="n">
-        <v>102.23</v>
+        <v>74.06</v>
       </c>
       <c r="H219" s="3" t="inlineStr">
         <is>
@@ -7517,7 +7517,7 @@
         </is>
       </c>
       <c r="G220" s="2" t="n">
-        <v>230.63</v>
+        <v>202.46</v>
       </c>
       <c r="H220" s="2" t="n"/>
     </row>
@@ -7549,7 +7549,7 @@
         </is>
       </c>
       <c r="G221" s="3" t="n">
-        <v>211.71</v>
+        <v>183.54</v>
       </c>
       <c r="H221" s="3" t="n"/>
     </row>
@@ -7581,7 +7581,7 @@
         </is>
       </c>
       <c r="G222" s="2" t="n">
-        <v>295.39</v>
+        <v>267.23</v>
       </c>
       <c r="H222" s="2" t="n"/>
     </row>
@@ -7613,7 +7613,7 @@
         </is>
       </c>
       <c r="G223" s="3" t="n">
-        <v>249.83</v>
+        <v>221.67</v>
       </c>
       <c r="H223" s="3" t="inlineStr">
         <is>
@@ -7649,7 +7649,7 @@
         </is>
       </c>
       <c r="G224" s="2" t="n">
-        <v>420.02</v>
+        <v>391.85</v>
       </c>
       <c r="H224" s="2" t="inlineStr">
         <is>
@@ -7685,7 +7685,7 @@
         </is>
       </c>
       <c r="G225" s="3" t="n">
-        <v>387.84</v>
+        <v>359.67</v>
       </c>
       <c r="H225" s="3" t="n"/>
     </row>
@@ -7717,7 +7717,7 @@
         </is>
       </c>
       <c r="G226" s="2" t="n">
-        <v>397.77</v>
+        <v>369.61</v>
       </c>
       <c r="H226" s="2" t="n"/>
     </row>
@@ -7749,7 +7749,7 @@
         </is>
       </c>
       <c r="G227" s="3" t="n">
-        <v>341.21</v>
+        <v>313.05</v>
       </c>
       <c r="H227" s="3" t="inlineStr">
         <is>
@@ -7785,7 +7785,7 @@
         </is>
       </c>
       <c r="G228" s="2" t="n">
-        <v>394.9</v>
+        <v>366.74</v>
       </c>
       <c r="H228" s="2" t="inlineStr">
         <is>
@@ -7821,7 +7821,7 @@
         </is>
       </c>
       <c r="G229" s="3" t="n">
-        <v>377.87</v>
+        <v>349.71</v>
       </c>
       <c r="H229" s="3" t="n"/>
     </row>
@@ -7849,11 +7849,11 @@
       </c>
       <c r="F230" s="2" t="inlineStr">
         <is>
-          <t>72/116</t>
+          <t>71/116</t>
         </is>
       </c>
       <c r="G230" s="2" t="n">
-        <v>388.4</v>
+        <v>360.23</v>
       </c>
       <c r="H230" s="2" t="n"/>
     </row>
@@ -7885,7 +7885,7 @@
         </is>
       </c>
       <c r="G231" s="3" t="n">
-        <v>370.31</v>
+        <v>342.14</v>
       </c>
       <c r="H231" s="3" t="n"/>
     </row>
@@ -7917,7 +7917,7 @@
         </is>
       </c>
       <c r="G232" s="2" t="n">
-        <v>479.03</v>
+        <v>450.86</v>
       </c>
       <c r="H232" s="2" t="n"/>
     </row>

</xml_diff>

<commit_message>
Fix insider events display issue in CSV output
Resolved a problem where insider events were not correctly displayed in the CSV output. Adjustments were made to ensure accurate representation of data.

- Updated `blne_rise_events.xlsx` with corrected data.
- Modified `blne_rise_volatility_analysis.json` to handle empty insider events.
- Adjusted `insider_conviction_all_stocks_results.json` with updated analysis date.
- Refined logic in `backtest_all_stocks_insider_conviction.py` to correct rise event handling.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -7383,11 +7383,7 @@
       <c r="G216" s="2" t="n">
         <v>203.95</v>
       </c>
-      <c r="H216" s="2" t="inlineStr">
-        <is>
-          <t>18/03/2025, 19/03/2025, 20/03/2025</t>
-        </is>
-      </c>
+      <c r="H216" s="2" t="n"/>
     </row>
     <row r="217">
       <c r="A217" s="3" t="inlineStr">
@@ -7419,7 +7415,11 @@
       <c r="G217" s="3" t="n">
         <v>123.83</v>
       </c>
-      <c r="H217" s="3" t="n"/>
+      <c r="H217" s="3" t="inlineStr">
+        <is>
+          <t>18/03/2025, 19/03/2025, 20/03/2025</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Remove 2-day rise event after fall with insider buying
Updated the data and logic to reflect changes in rise event detection.

- Modified `blne_rise_events.xlsx` to remove the 2-day rise event with insider buying.
- Adjusted `blne_rise_volatility_analysis.json` to reflect updated rise event counts and details.
- Updated `insider_conviction_all_stocks_results.json` with revised analysis results.
- Added new files `sezl_rise_events.xlsx` and `sezl_rise_volatility_analysis.json` for SEZL stock analysis.
- Refined `backtest_all_stocks_insider_conviction.py` to align with updated rise event logic.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H232"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>23/116</t>
+          <t>23/115</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>14/115</t>
+          <t>13/114</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
@@ -585,7 +585,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>48/116</t>
+          <t>49/115</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
@@ -617,7 +617,7 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>59/115</t>
+          <t>57/114</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>27/116</t>
+          <t>27/115</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
@@ -681,7 +681,7 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>22/115</t>
+          <t>21/114</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
@@ -713,7 +713,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>12/116</t>
+          <t>12/115</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
@@ -745,7 +745,7 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>95/115</t>
+          <t>93/114</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
@@ -777,7 +777,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>67/116</t>
+          <t>67/115</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
@@ -809,7 +809,7 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>12/115</t>
+          <t>11/114</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>103/116</t>
+          <t>102/115</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
@@ -873,7 +873,7 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>82/115</t>
+          <t>79/114</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>66/116</t>
+          <t>66/115</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
@@ -937,7 +937,7 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>106/115</t>
+          <t>105/114</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>114/116</t>
+          <t>113/115</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>112/115</t>
+          <t>111/114</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>20/116</t>
+          <t>20/115</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>38/115</t>
+          <t>37/114</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>104/116</t>
+          <t>103/115</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>71/115</t>
+          <t>69/114</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>68/116</t>
+          <t>69/115</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>110/115</t>
+          <t>109/114</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>31/116</t>
+          <t>31/115</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>101/115</t>
+          <t>99/114</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>13/116</t>
+          <t>13/115</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>105/115</t>
+          <t>104/114</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>115/116</t>
+          <t>114/115</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>86/115</t>
+          <t>84/114</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>100/116</t>
+          <t>100/115</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>113/115</t>
+          <t>112/114</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>91/116</t>
+          <t>92/115</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>91/115</t>
+          <t>89/114</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>72/116</t>
+          <t>74/115</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>67/115</t>
+          <t>65/114</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>97/116</t>
+          <t>97/115</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>69/115</t>
+          <t>67/114</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>42/116</t>
+          <t>42/115</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>83/115</t>
+          <t>80/114</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>88/116</t>
+          <t>89/115</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>100/115</t>
+          <t>98/114</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>78/116</t>
+          <t>79/115</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>30/115</t>
+          <t>28/114</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>96/116</t>
+          <t>96/115</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>109/115</t>
+          <t>108/114</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>107/116</t>
+          <t>106/115</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>79/115</t>
+          <t>76/114</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>81/116</t>
+          <t>82/115</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>108/115</t>
+          <t>107/114</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>99/116</t>
+          <t>99/115</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>104/115</t>
+          <t>103/114</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>105/116</t>
+          <t>104/115</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>99/115</t>
+          <t>97/114</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>111/116</t>
+          <t>110/115</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>62/115</t>
+          <t>60/114</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>113/116</t>
+          <t>112/115</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>93/115</t>
+          <t>91/114</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>101/116</t>
+          <t>101/115</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>76/115</t>
+          <t>74/114</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>83/116</t>
+          <t>84/115</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>97/115</t>
+          <t>95/114</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>86/116</t>
+          <t>87/115</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>51/115</t>
+          <t>50/114</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>82/116</t>
+          <t>83/115</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>98/115</t>
+          <t>96/114</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>25/116</t>
+          <t>25/115</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>78/115</t>
+          <t>75/114</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>89/116</t>
+          <t>90/115</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>13/115</t>
+          <t>12/114</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>112/116</t>
+          <t>111/115</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>49/115</t>
+          <t>48/114</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>33/116</t>
+          <t>33/115</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>89/115</t>
+          <t>87/114</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>59/116</t>
+          <t>59/115</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>87/115</t>
+          <t>85/114</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>40/116</t>
+          <t>40/115</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>107/115</t>
+          <t>106/114</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>108/116</t>
+          <t>107/115</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>2/115</t>
+          <t>2/114</t>
         </is>
       </c>
       <c r="G79" s="3" t="n">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>5/116</t>
+          <t>5/115</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>92/115</t>
+          <t>90/114</t>
         </is>
       </c>
       <c r="G81" s="3" t="n">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>95/116</t>
+          <t>95/115</t>
         </is>
       </c>
       <c r="G82" s="2" t="n">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>31/115</t>
+          <t>29/114</t>
         </is>
       </c>
       <c r="G83" s="3" t="n">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>38/116</t>
+          <t>38/115</t>
         </is>
       </c>
       <c r="G84" s="2" t="n">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>43/115</t>
+          <t>42/114</t>
         </is>
       </c>
       <c r="G85" s="3" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>64/116</t>
+          <t>64/115</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>54/115</t>
+          <t>53/114</t>
         </is>
       </c>
       <c r="G87" s="3" t="n">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>84/116</t>
+          <t>85/115</t>
         </is>
       </c>
       <c r="G88" s="2" t="n">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>46/115</t>
+          <t>45/114</t>
         </is>
       </c>
       <c r="G89" s="3" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>50/116</t>
+          <t>51/115</t>
         </is>
       </c>
       <c r="G90" s="2" t="n">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>88/115</t>
+          <t>86/114</t>
         </is>
       </c>
       <c r="G91" s="3" t="n">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="F92" s="2" t="inlineStr">
         <is>
-          <t>15/116</t>
+          <t>15/115</t>
         </is>
       </c>
       <c r="G92" s="2" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>18/115</t>
+          <t>17/114</t>
         </is>
       </c>
       <c r="G93" s="3" t="n">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>61/116</t>
+          <t>62/115</t>
         </is>
       </c>
       <c r="G94" s="2" t="n">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>102/115</t>
+          <t>100/114</t>
         </is>
       </c>
       <c r="G95" s="3" t="n">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>57/116</t>
+          <t>57/115</t>
         </is>
       </c>
       <c r="G96" s="2" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>103/115</t>
+          <t>102/114</t>
         </is>
       </c>
       <c r="G97" s="3" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>16/116</t>
+          <t>16/115</t>
         </is>
       </c>
       <c r="G98" s="2" t="n">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>47/115</t>
+          <t>46/114</t>
         </is>
       </c>
       <c r="G99" s="3" t="n">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>85/116</t>
+          <t>86/115</t>
         </is>
       </c>
       <c r="G100" s="2" t="n">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>34/115</t>
+          <t>33/114</t>
         </is>
       </c>
       <c r="G101" s="3" t="n">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>3/116</t>
+          <t>3/115</t>
         </is>
       </c>
       <c r="G102" s="2" t="n">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>25/115</t>
+          <t>24/114</t>
         </is>
       </c>
       <c r="G103" s="3" t="n">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>69/116</t>
+          <t>70/115</t>
         </is>
       </c>
       <c r="G104" s="2" t="n">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>73/115</t>
+          <t>71/114</t>
         </is>
       </c>
       <c r="G105" s="3" t="n">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>56/116</t>
+          <t>56/115</t>
         </is>
       </c>
       <c r="G106" s="2" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>40/115</t>
+          <t>39/114</t>
         </is>
       </c>
       <c r="G107" s="3" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>55/116</t>
+          <t>55/115</t>
         </is>
       </c>
       <c r="G108" s="2" t="n">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>94/115</t>
+          <t>92/114</t>
         </is>
       </c>
       <c r="G109" s="3" t="n">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>6/116</t>
+          <t>7/115</t>
         </is>
       </c>
       <c r="G110" s="2" t="n">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>81/115</t>
+          <t>78/114</t>
         </is>
       </c>
       <c r="G111" s="3" t="n">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>92/116</t>
+          <t>93/115</t>
         </is>
       </c>
       <c r="G112" s="2" t="n">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>96/115</t>
+          <t>94/114</t>
         </is>
       </c>
       <c r="G113" s="3" t="n">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>28/116</t>
+          <t>28/115</t>
         </is>
       </c>
       <c r="G114" s="2" t="n">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>111/115</t>
+          <t>110/114</t>
         </is>
       </c>
       <c r="G115" s="3" t="n">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t>26/116</t>
+          <t>26/115</t>
         </is>
       </c>
       <c r="G116" s="2" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>53/115</t>
+          <t>52/114</t>
         </is>
       </c>
       <c r="G117" s="3" t="n">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="F118" s="2" t="inlineStr">
         <is>
-          <t>109/116</t>
+          <t>108/115</t>
         </is>
       </c>
       <c r="G118" s="2" t="n">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>32/115</t>
+          <t>30/114</t>
         </is>
       </c>
       <c r="G119" s="3" t="n">
@@ -4297,7 +4297,7 @@
       </c>
       <c r="F120" s="2" t="inlineStr">
         <is>
-          <t>79/116</t>
+          <t>80/115</t>
         </is>
       </c>
       <c r="G120" s="2" t="n">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>44/115</t>
+          <t>43/114</t>
         </is>
       </c>
       <c r="G121" s="3" t="n">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>52/116</t>
+          <t>53/115</t>
         </is>
       </c>
       <c r="G122" s="2" t="n">
@@ -4393,7 +4393,7 @@
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>90/115</t>
+          <t>88/114</t>
         </is>
       </c>
       <c r="G123" s="3" t="n">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>74/116</t>
+          <t>75/115</t>
         </is>
       </c>
       <c r="G124" s="2" t="n">
@@ -4457,7 +4457,7 @@
       </c>
       <c r="F125" s="3" t="inlineStr">
         <is>
-          <t>24/115</t>
+          <t>23/114</t>
         </is>
       </c>
       <c r="G125" s="3" t="n">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>98/116</t>
+          <t>98/115</t>
         </is>
       </c>
       <c r="G126" s="2" t="n">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>65/115</t>
+          <t>63/114</t>
         </is>
       </c>
       <c r="G127" s="3" t="n">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="F128" s="2" t="inlineStr">
         <is>
-          <t>43/116</t>
+          <t>43/115</t>
         </is>
       </c>
       <c r="G128" s="2" t="n">
@@ -4585,7 +4585,7 @@
       </c>
       <c r="F129" s="3" t="inlineStr">
         <is>
-          <t>6/115</t>
+          <t>6/114</t>
         </is>
       </c>
       <c r="G129" s="3" t="n">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="F130" s="2" t="inlineStr">
         <is>
-          <t>41/116</t>
+          <t>41/115</t>
         </is>
       </c>
       <c r="G130" s="2" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="F131" s="3" t="inlineStr">
         <is>
-          <t>45/115</t>
+          <t>44/114</t>
         </is>
       </c>
       <c r="G131" s="3" t="n">
@@ -4681,7 +4681,7 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>62/116</t>
+          <t>63/115</t>
         </is>
       </c>
       <c r="G132" s="2" t="n">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="F133" s="3" t="inlineStr">
         <is>
-          <t>56/115</t>
+          <t>55/114</t>
         </is>
       </c>
       <c r="G133" s="3" t="n">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>18/116</t>
+          <t>18/115</t>
         </is>
       </c>
       <c r="G134" s="2" t="n">
@@ -4770,22 +4770,22 @@
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>28/04/2022</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="D135" s="3" t="n">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>-35.56</v>
+        <v>-55.56</v>
       </c>
       <c r="F135" s="3" t="inlineStr">
         <is>
-          <t>21/115</t>
+          <t>5/114</t>
         </is>
       </c>
       <c r="G135" s="3" t="n">
-        <v>191.92</v>
+        <v>171.92</v>
       </c>
       <c r="H135" s="3" t="n"/>
     </row>
@@ -4797,27 +4797,27 @@
       </c>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>28/04/2022</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>02/05/2022</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="D136" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E136" s="2" t="n">
-        <v>5.13</v>
+        <v>19.16</v>
       </c>
       <c r="F136" s="2" t="inlineStr">
         <is>
-          <t>102/116</t>
+          <t>44/115</t>
         </is>
       </c>
       <c r="G136" s="2" t="n">
-        <v>197.06</v>
+        <v>191.09</v>
       </c>
       <c r="H136" s="2" t="n"/>
     </row>
@@ -4829,27 +4829,27 @@
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>02/05/2022</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>31/05/2022</t>
+          <t>13/07/2022</t>
         </is>
       </c>
       <c r="D137" s="3" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E137" s="3" t="n">
-        <v>-31.46</v>
+        <v>-16.49</v>
       </c>
       <c r="F137" s="3" t="inlineStr">
         <is>
-          <t>27/115</t>
+          <t>62/114</t>
         </is>
       </c>
       <c r="G137" s="3" t="n">
-        <v>165.59</v>
+        <v>174.6</v>
       </c>
       <c r="H137" s="3" t="n"/>
     </row>
@@ -4861,27 +4861,27 @@
       </c>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>31/05/2022</t>
+          <t>13/07/2022</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr">
         <is>
-          <t>09/06/2022</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="D138" s="2" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E138" s="2" t="n">
-        <v>7.35</v>
+        <v>11.65</v>
       </c>
       <c r="F138" s="2" t="inlineStr">
         <is>
-          <t>93/116</t>
+          <t>68/115</t>
         </is>
       </c>
       <c r="G138" s="2" t="n">
-        <v>172.94</v>
+        <v>186.25</v>
       </c>
       <c r="H138" s="2" t="n"/>
     </row>
@@ -4893,27 +4893,27 @@
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>06/06/2022</t>
+          <t>28/07/2022</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>21/06/2022</t>
+          <t>03/08/2022</t>
         </is>
       </c>
       <c r="D139" s="3" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>-17.81</v>
+        <v>-11.59</v>
       </c>
       <c r="F139" s="3" t="inlineStr">
         <is>
-          <t>58/115</t>
+          <t>81/114</t>
         </is>
       </c>
       <c r="G139" s="3" t="n">
-        <v>155.14</v>
+        <v>174.66</v>
       </c>
       <c r="H139" s="3" t="n"/>
     </row>
@@ -4925,27 +4925,27 @@
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>21/06/2022</t>
+          <t>03/08/2022</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr">
         <is>
-          <t>24/06/2022</t>
+          <t>05/08/2022</t>
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E140" s="2" t="n">
-        <v>19.16</v>
+        <v>18.03</v>
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>44/116</t>
+          <t>46/115</t>
         </is>
       </c>
       <c r="G140" s="2" t="n">
-        <v>174.3</v>
+        <v>192.69</v>
       </c>
       <c r="H140" s="2" t="n"/>
     </row>
@@ -4957,27 +4957,27 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>24/06/2022</t>
+          <t>05/08/2022</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>06/07/2022</t>
+          <t>12/09/2022</t>
         </is>
       </c>
       <c r="D141" s="3" t="n">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>-16.35</v>
+        <v>-47.64</v>
       </c>
       <c r="F141" s="3" t="inlineStr">
         <is>
-          <t>64/115</t>
+          <t>8/114</t>
         </is>
       </c>
       <c r="G141" s="3" t="n">
-        <v>157.95</v>
+        <v>145.05</v>
       </c>
       <c r="H141" s="3" t="n"/>
     </row>
@@ -4989,27 +4989,27 @@
       </c>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>06/07/2022</t>
+          <t>12/09/2022</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>20/07/2022</t>
+          <t>15/09/2022</t>
         </is>
       </c>
       <c r="D142" s="2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E142" s="2" t="n">
-        <v>13.09</v>
+        <v>16.88</v>
       </c>
       <c r="F142" s="2" t="inlineStr">
         <is>
-          <t>63/116</t>
+          <t>52/115</t>
         </is>
       </c>
       <c r="G142" s="2" t="n">
-        <v>171.03</v>
+        <v>161.93</v>
       </c>
       <c r="H142" s="2" t="n"/>
     </row>
@@ -5021,27 +5021,27 @@
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>08/07/2022</t>
+          <t>14/09/2022</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>03/08/2022</t>
+          <t>04/10/2022</t>
         </is>
       </c>
       <c r="D143" s="3" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>-12.86</v>
+        <v>-40.89</v>
       </c>
       <c r="F143" s="3" t="inlineStr">
         <is>
-          <t>77/115</t>
+          <t>15/114</t>
         </is>
       </c>
       <c r="G143" s="3" t="n">
-        <v>158.18</v>
+        <v>121.05</v>
       </c>
       <c r="H143" s="3" t="n"/>
     </row>
@@ -5053,27 +5053,27 @@
       </c>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>03/08/2022</t>
+          <t>04/10/2022</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr">
         <is>
-          <t>05/08/2022</t>
+          <t>06/10/2022</t>
         </is>
       </c>
       <c r="D144" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E144" s="2" t="n">
-        <v>18.03</v>
+        <v>17.18</v>
       </c>
       <c r="F144" s="2" t="inlineStr">
         <is>
-          <t>46/116</t>
+          <t>50/115</t>
         </is>
       </c>
       <c r="G144" s="2" t="n">
-        <v>176.21</v>
+        <v>138.23</v>
       </c>
       <c r="H144" s="2" t="n"/>
     </row>
@@ -5085,27 +5085,27 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>05/08/2022</t>
+          <t>06/10/2022</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>12/09/2022</t>
+          <t>28/10/2022</t>
         </is>
       </c>
       <c r="D145" s="3" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>-47.64</v>
+        <v>-14.96</v>
       </c>
       <c r="F145" s="3" t="inlineStr">
         <is>
-          <t>8/115</t>
+          <t>68/114</t>
         </is>
       </c>
       <c r="G145" s="3" t="n">
-        <v>128.57</v>
+        <v>123.27</v>
       </c>
       <c r="H145" s="3" t="n"/>
     </row>
@@ -5117,27 +5117,27 @@
       </c>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>12/09/2022</t>
+          <t>28/10/2022</t>
         </is>
       </c>
       <c r="C146" s="2" t="inlineStr">
         <is>
-          <t>15/09/2022</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="D146" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E146" s="2" t="n">
-        <v>16.88</v>
+        <v>3.96</v>
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>51/116</t>
+          <t>109/115</t>
         </is>
       </c>
       <c r="G146" s="2" t="n">
-        <v>145.45</v>
+        <v>127.23</v>
       </c>
       <c r="H146" s="2" t="n"/>
     </row>
@@ -5149,27 +5149,27 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>14/09/2022</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>04/10/2022</t>
+          <t>29/12/2022</t>
         </is>
       </c>
       <c r="D147" s="3" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>-40.89</v>
+        <v>-28.57</v>
       </c>
       <c r="F147" s="3" t="inlineStr">
         <is>
-          <t>16/115</t>
+          <t>27/114</t>
         </is>
       </c>
       <c r="G147" s="3" t="n">
-        <v>104.56</v>
+        <v>98.66</v>
       </c>
       <c r="H147" s="3" t="n"/>
     </row>
@@ -5181,27 +5181,27 @@
       </c>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>04/10/2022</t>
+          <t>29/12/2022</t>
         </is>
       </c>
       <c r="C148" s="2" t="inlineStr">
         <is>
-          <t>06/10/2022</t>
+          <t>11/01/2023</t>
         </is>
       </c>
       <c r="D148" s="2" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E148" s="2" t="n">
-        <v>17.18</v>
+        <v>26.67</v>
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>49/116</t>
+          <t>30/115</t>
         </is>
       </c>
       <c r="G148" s="2" t="n">
-        <v>121.75</v>
+        <v>125.33</v>
       </c>
       <c r="H148" s="2" t="n"/>
     </row>
@@ -5213,27 +5213,27 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>06/10/2022</t>
+          <t>11/01/2023</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>28/10/2022</t>
+          <t>27/01/2023</t>
         </is>
       </c>
       <c r="D149" s="3" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>-14.96</v>
+        <v>-11.23</v>
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>70/115</t>
+          <t>83/114</t>
         </is>
       </c>
       <c r="G149" s="3" t="n">
-        <v>106.79</v>
+        <v>114.1</v>
       </c>
       <c r="H149" s="3" t="n"/>
     </row>
@@ -5245,27 +5245,27 @@
       </c>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>28/10/2022</t>
+          <t>27/01/2023</t>
         </is>
       </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>01/11/2022</t>
+          <t>03/02/2023</t>
         </is>
       </c>
       <c r="D150" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E150" s="2" t="n">
-        <v>3.96</v>
+        <v>78.73999999999999</v>
       </c>
       <c r="F150" s="2" t="inlineStr">
         <is>
-          <t>110/116</t>
+          <t>10/115</t>
         </is>
       </c>
       <c r="G150" s="2" t="n">
-        <v>110.75</v>
+        <v>192.84</v>
       </c>
       <c r="H150" s="2" t="n"/>
     </row>
@@ -5277,27 +5277,27 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>01/11/2022</t>
+          <t>03/02/2023</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>29/12/2022</t>
+          <t>13/02/2023</t>
         </is>
       </c>
       <c r="D151" s="3" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>-28.57</v>
+        <v>-35.9</v>
       </c>
       <c r="F151" s="3" t="inlineStr">
         <is>
-          <t>29/115</t>
+          <t>20/114</t>
         </is>
       </c>
       <c r="G151" s="3" t="n">
-        <v>82.18000000000001</v>
+        <v>156.94</v>
       </c>
       <c r="H151" s="3" t="n"/>
     </row>
@@ -5309,27 +5309,27 @@
       </c>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>29/12/2022</t>
+          <t>13/02/2023</t>
         </is>
       </c>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>11/01/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="D152" s="2" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E152" s="2" t="n">
-        <v>26.67</v>
+        <v>14.78</v>
       </c>
       <c r="F152" s="2" t="inlineStr">
         <is>
-          <t>30/116</t>
+          <t>60/115</t>
         </is>
       </c>
       <c r="G152" s="2" t="n">
-        <v>108.85</v>
+        <v>171.71</v>
       </c>
       <c r="H152" s="2" t="n"/>
     </row>
@@ -5341,27 +5341,27 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>11/01/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>27/01/2023</t>
+          <t>24/02/2023</t>
         </is>
       </c>
       <c r="D153" s="3" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>-11.23</v>
+        <v>-20.36</v>
       </c>
       <c r="F153" s="3" t="inlineStr">
         <is>
-          <t>85/115</t>
+          <t>47/114</t>
         </is>
       </c>
       <c r="G153" s="3" t="n">
-        <v>97.62</v>
+        <v>151.35</v>
       </c>
       <c r="H153" s="3" t="n"/>
     </row>
@@ -5373,27 +5373,27 @@
       </c>
       <c r="B154" s="2" t="inlineStr">
         <is>
-          <t>27/01/2023</t>
+          <t>24/02/2023</t>
         </is>
       </c>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>03/02/2023</t>
+          <t>06/03/2023</t>
         </is>
       </c>
       <c r="D154" s="2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E154" s="2" t="n">
-        <v>78.73999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>10/116</t>
+          <t>78/115</t>
         </is>
       </c>
       <c r="G154" s="2" t="n">
-        <v>176.36</v>
+        <v>161.13</v>
       </c>
       <c r="H154" s="2" t="n"/>
     </row>
@@ -5405,27 +5405,27 @@
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>03/02/2023</t>
+          <t>03/03/2023</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>13/02/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="D155" s="3" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>-35.9</v>
+        <v>-21.58</v>
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>20/115</t>
+          <t>41/114</t>
         </is>
       </c>
       <c r="G155" s="3" t="n">
-        <v>140.45</v>
+        <v>139.55</v>
       </c>
       <c r="H155" s="3" t="n"/>
     </row>
@@ -5437,27 +5437,27 @@
       </c>
       <c r="B156" s="2" t="inlineStr">
         <is>
-          <t>13/02/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>15/02/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="D156" s="2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E156" s="2" t="n">
-        <v>14.78</v>
+        <v>52.84</v>
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>60/116</t>
+          <t>17/115</t>
         </is>
       </c>
       <c r="G156" s="2" t="n">
-        <v>155.23</v>
+        <v>192.39</v>
       </c>
       <c r="H156" s="2" t="n"/>
     </row>
@@ -5469,27 +5469,27 @@
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>15/02/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>24/02/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="D157" s="3" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E157" s="3" t="n">
-        <v>-20.36</v>
+        <v>-44</v>
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>48/115</t>
+          <t>10/114</t>
         </is>
       </c>
       <c r="G157" s="3" t="n">
-        <v>134.87</v>
+        <v>148.39</v>
       </c>
       <c r="H157" s="3" t="n"/>
     </row>
@@ -5501,27 +5501,27 @@
       </c>
       <c r="B158" s="2" t="inlineStr">
         <is>
-          <t>24/02/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>06/03/2023</t>
+          <t>21/04/2023</t>
         </is>
       </c>
       <c r="D158" s="2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E158" s="2" t="n">
-        <v>9.77</v>
+        <v>4.59</v>
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>77/116</t>
+          <t>105/115</t>
         </is>
       </c>
       <c r="G158" s="2" t="n">
-        <v>144.65</v>
+        <v>152.98</v>
       </c>
       <c r="H158" s="2" t="n"/>
     </row>
@@ -5533,27 +5533,27 @@
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>03/03/2023</t>
+          <t>21/04/2023</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>05/05/2023</t>
         </is>
       </c>
       <c r="D159" s="3" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>-21.58</v>
+        <v>-15.61</v>
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>42/115</t>
+          <t>64/114</t>
         </is>
       </c>
       <c r="G159" s="3" t="n">
-        <v>123.07</v>
+        <v>137.37</v>
       </c>
       <c r="H159" s="3" t="n"/>
     </row>
@@ -5565,27 +5565,27 @@
       </c>
       <c r="B160" s="2" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>05/05/2023</t>
         </is>
       </c>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>31/03/2023</t>
+          <t>15/05/2023</t>
         </is>
       </c>
       <c r="D160" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E160" s="2" t="n">
-        <v>52.84</v>
+        <v>38.29</v>
       </c>
       <c r="F160" s="2" t="inlineStr">
         <is>
-          <t>17/116</t>
+          <t>22/115</t>
         </is>
       </c>
       <c r="G160" s="2" t="n">
-        <v>175.91</v>
+        <v>175.66</v>
       </c>
       <c r="H160" s="2" t="n"/>
     </row>
@@ -5597,27 +5597,27 @@
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>31/03/2023</t>
+          <t>15/05/2023</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>19/04/2023</t>
+          <t>18/05/2023</t>
         </is>
       </c>
       <c r="D161" s="3" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E161" s="3" t="n">
-        <v>-44</v>
+        <v>-25.43</v>
       </c>
       <c r="F161" s="3" t="inlineStr">
         <is>
-          <t>11/115</t>
+          <t>34/114</t>
         </is>
       </c>
       <c r="G161" s="3" t="n">
-        <v>131.91</v>
+        <v>150.22</v>
       </c>
       <c r="H161" s="3" t="n"/>
     </row>
@@ -5629,27 +5629,27 @@
       </c>
       <c r="B162" s="2" t="inlineStr">
         <is>
-          <t>19/04/2023</t>
+          <t>18/05/2023</t>
         </is>
       </c>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>21/04/2023</t>
+          <t>23/05/2023</t>
         </is>
       </c>
       <c r="D162" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E162" s="2" t="n">
-        <v>4.59</v>
+        <v>19.15</v>
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>106/116</t>
+          <t>45/115</t>
         </is>
       </c>
       <c r="G162" s="2" t="n">
-        <v>136.5</v>
+        <v>169.37</v>
       </c>
       <c r="H162" s="2" t="n"/>
     </row>
@@ -5661,27 +5661,27 @@
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>21/04/2023</t>
+          <t>23/05/2023</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>05/05/2023</t>
+          <t>08/06/2023</t>
         </is>
       </c>
       <c r="D163" s="3" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>-15.61</v>
+        <v>-26.51</v>
       </c>
       <c r="F163" s="3" t="inlineStr">
         <is>
-          <t>66/115</t>
+          <t>31/114</t>
         </is>
       </c>
       <c r="G163" s="3" t="n">
-        <v>120.89</v>
+        <v>142.86</v>
       </c>
       <c r="H163" s="3" t="n"/>
     </row>
@@ -5693,27 +5693,27 @@
       </c>
       <c r="B164" s="2" t="inlineStr">
         <is>
-          <t>05/05/2023</t>
+          <t>08/06/2023</t>
         </is>
       </c>
       <c r="C164" s="2" t="inlineStr">
         <is>
-          <t>15/05/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="D164" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E164" s="2" t="n">
-        <v>38.29</v>
+        <v>87.65000000000001</v>
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>22/116</t>
+          <t>8/115</t>
         </is>
       </c>
       <c r="G164" s="2" t="n">
-        <v>159.18</v>
+        <v>230.51</v>
       </c>
       <c r="H164" s="2" t="n"/>
     </row>
@@ -5725,27 +5725,27 @@
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>15/05/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>18/05/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="D165" s="3" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>-25.43</v>
+        <v>-50.4</v>
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>35/115</t>
+          <t>7/114</t>
         </is>
       </c>
       <c r="G165" s="3" t="n">
-        <v>133.74</v>
+        <v>180.11</v>
       </c>
       <c r="H165" s="3" t="n"/>
     </row>
@@ -5757,27 +5757,27 @@
       </c>
       <c r="B166" s="2" t="inlineStr">
         <is>
-          <t>18/05/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="C166" s="2" t="inlineStr">
         <is>
-          <t>23/05/2023</t>
+          <t>19/07/2023</t>
         </is>
       </c>
       <c r="D166" s="2" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E166" s="2" t="n">
-        <v>19.15</v>
+        <v>9.9</v>
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>45/116</t>
+          <t>76/115</t>
         </is>
       </c>
       <c r="G166" s="2" t="n">
-        <v>152.89</v>
+        <v>190.01</v>
       </c>
       <c r="H166" s="2" t="n"/>
     </row>
@@ -5789,27 +5789,27 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>23/05/2023</t>
+          <t>10/07/2023</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>08/06/2023</t>
+          <t>28/07/2023</t>
         </is>
       </c>
       <c r="D167" s="3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>-26.51</v>
+        <v>-13.37</v>
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>33/115</t>
+          <t>73/114</t>
         </is>
       </c>
       <c r="G167" s="3" t="n">
-        <v>126.38</v>
+        <v>176.64</v>
       </c>
       <c r="H167" s="3" t="n"/>
     </row>
@@ -5821,27 +5821,27 @@
       </c>
       <c r="B168" s="2" t="inlineStr">
         <is>
-          <t>08/06/2023</t>
+          <t>28/07/2023</t>
         </is>
       </c>
       <c r="C168" s="2" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>02/08/2023</t>
         </is>
       </c>
       <c r="D168" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E168" s="2" t="n">
-        <v>87.65000000000001</v>
+        <v>12.75</v>
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>7/116</t>
+          <t>65/115</t>
         </is>
       </c>
       <c r="G168" s="2" t="n">
-        <v>214.03</v>
+        <v>189.39</v>
       </c>
       <c r="H168" s="2" t="n"/>
     </row>
@@ -5853,27 +5853,27 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>02/08/2023</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="D169" s="3" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>-50.4</v>
+        <v>-62.8</v>
       </c>
       <c r="F169" s="3" t="inlineStr">
         <is>
-          <t>7/115</t>
+          <t>3/114</t>
         </is>
       </c>
       <c r="G169" s="3" t="n">
-        <v>163.63</v>
+        <v>126.6</v>
       </c>
       <c r="H169" s="3" t="n"/>
     </row>
@@ -5885,27 +5885,27 @@
       </c>
       <c r="B170" s="2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="C170" s="2" t="inlineStr">
         <is>
-          <t>19/07/2023</t>
+          <t>04/10/2023</t>
         </is>
       </c>
       <c r="D170" s="2" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E170" s="2" t="n">
-        <v>9.9</v>
+        <v>49.6</v>
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>75/116</t>
+          <t>19/115</t>
         </is>
       </c>
       <c r="G170" s="2" t="n">
-        <v>173.53</v>
+        <v>176.2</v>
       </c>
       <c r="H170" s="2" t="n"/>
     </row>
@@ -5917,27 +5917,27 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>10/07/2023</t>
+          <t>04/10/2023</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>28/07/2023</t>
+          <t>09/10/2023</t>
         </is>
       </c>
       <c r="D171" s="3" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>-13.37</v>
+        <v>-2.14</v>
       </c>
       <c r="F171" s="3" t="inlineStr">
         <is>
-          <t>75/115</t>
+          <t>113/114</t>
         </is>
       </c>
       <c r="G171" s="3" t="n">
-        <v>160.16</v>
+        <v>174.06</v>
       </c>
       <c r="H171" s="3" t="n"/>
     </row>
@@ -5949,27 +5949,27 @@
       </c>
       <c r="B172" s="2" t="inlineStr">
         <is>
-          <t>28/07/2023</t>
+          <t>09/10/2023</t>
         </is>
       </c>
       <c r="C172" s="2" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="D172" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E172" s="2" t="n">
-        <v>12.75</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F172" s="2" t="inlineStr">
         <is>
-          <t>65/116</t>
+          <t>88/115</t>
         </is>
       </c>
       <c r="G172" s="2" t="n">
-        <v>172.91</v>
+        <v>182.25</v>
       </c>
       <c r="H172" s="2" t="n"/>
     </row>
@@ -5981,27 +5981,27 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>28/09/2023</t>
+          <t>27/10/2023</t>
         </is>
       </c>
       <c r="D173" s="3" t="n">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>-62.8</v>
+        <v>-34.34</v>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>4/115</t>
+          <t>22/114</t>
         </is>
       </c>
       <c r="G173" s="3" t="n">
-        <v>110.11</v>
+        <v>147.91</v>
       </c>
       <c r="H173" s="3" t="n"/>
     </row>
@@ -6013,27 +6013,27 @@
       </c>
       <c r="B174" s="2" t="inlineStr">
         <is>
-          <t>28/09/2023</t>
+          <t>27/10/2023</t>
         </is>
       </c>
       <c r="C174" s="2" t="inlineStr">
         <is>
-          <t>04/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D174" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E174" s="2" t="n">
-        <v>49.6</v>
+        <v>15.6</v>
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>19/116</t>
+          <t>58/115</t>
         </is>
       </c>
       <c r="G174" s="2" t="n">
-        <v>159.71</v>
+        <v>163.51</v>
       </c>
       <c r="H174" s="2" t="n"/>
     </row>
@@ -6045,27 +6045,27 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>04/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>09/10/2023</t>
+          <t>27/11/2023</t>
         </is>
       </c>
       <c r="D175" s="3" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>-2.14</v>
+        <v>-44.17</v>
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>114/115</t>
+          <t>9/114</t>
         </is>
       </c>
       <c r="G175" s="3" t="n">
-        <v>157.57</v>
+        <v>119.34</v>
       </c>
       <c r="H175" s="3" t="n"/>
     </row>
@@ -6077,27 +6077,27 @@
       </c>
       <c r="B176" s="2" t="inlineStr">
         <is>
-          <t>09/10/2023</t>
+          <t>27/11/2023</t>
         </is>
       </c>
       <c r="C176" s="2" t="inlineStr">
         <is>
-          <t>11/10/2023</t>
+          <t>30/11/2023</t>
         </is>
       </c>
       <c r="D176" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E176" s="2" t="n">
-        <v>8.199999999999999</v>
+        <v>34.74</v>
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>87/116</t>
+          <t>24/115</t>
         </is>
       </c>
       <c r="G176" s="2" t="n">
-        <v>165.77</v>
+        <v>154.08</v>
       </c>
       <c r="H176" s="2" t="n"/>
     </row>
@@ -6109,27 +6109,27 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>11/10/2023</t>
+          <t>28/12/2023</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>27/10/2023</t>
+          <t>22/01/2024</t>
         </is>
       </c>
       <c r="D177" s="3" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>-34.34</v>
+        <v>-17.37</v>
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>23/115</t>
+          <t>58/114</t>
         </is>
       </c>
       <c r="G177" s="3" t="n">
-        <v>131.43</v>
+        <v>136.7</v>
       </c>
       <c r="H177" s="3" t="n"/>
     </row>
@@ -6141,27 +6141,27 @@
       </c>
       <c r="B178" s="2" t="inlineStr">
         <is>
-          <t>27/10/2023</t>
+          <t>22/01/2024</t>
         </is>
       </c>
       <c r="C178" s="2" t="inlineStr">
         <is>
-          <t>31/10/2023</t>
+          <t>25/01/2024</t>
         </is>
       </c>
       <c r="D178" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E178" s="2" t="n">
-        <v>15.6</v>
+        <v>1.87</v>
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>58/116</t>
+          <t>115/115</t>
         </is>
       </c>
       <c r="G178" s="2" t="n">
-        <v>147.03</v>
+        <v>138.57</v>
       </c>
       <c r="H178" s="2" t="n"/>
     </row>
@@ -6173,27 +6173,27 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>31/10/2023</t>
+          <t>24/01/2024</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>27/11/2023</t>
+          <t>02/02/2024</t>
         </is>
       </c>
       <c r="D179" s="3" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>-44.17</v>
+        <v>-1.83</v>
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>10/115</t>
+          <t>114/114</t>
         </is>
       </c>
       <c r="G179" s="3" t="n">
-        <v>102.86</v>
+        <v>136.74</v>
       </c>
       <c r="H179" s="3" t="n"/>
     </row>
@@ -6205,27 +6205,27 @@
       </c>
       <c r="B180" s="2" t="inlineStr">
         <is>
-          <t>27/11/2023</t>
+          <t>02/02/2024</t>
         </is>
       </c>
       <c r="C180" s="2" t="inlineStr">
         <is>
-          <t>30/11/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="D180" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E180" s="2" t="n">
-        <v>34.74</v>
+        <v>7.94</v>
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>24/116</t>
+          <t>91/115</t>
         </is>
       </c>
       <c r="G180" s="2" t="n">
-        <v>137.6</v>
+        <v>144.68</v>
       </c>
       <c r="H180" s="2" t="n"/>
     </row>
@@ -6237,27 +6237,27 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>28/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>22/01/2024</t>
+          <t>21/02/2024</t>
         </is>
       </c>
       <c r="D181" s="3" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E181" s="3" t="n">
-        <v>-17.37</v>
+        <v>-13.51</v>
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>60/115</t>
+          <t>72/114</t>
         </is>
       </c>
       <c r="G181" s="3" t="n">
-        <v>120.22</v>
+        <v>131.17</v>
       </c>
       <c r="H181" s="3" t="n"/>
     </row>
@@ -6269,27 +6269,27 @@
       </c>
       <c r="B182" s="2" t="inlineStr">
         <is>
-          <t>22/01/2024</t>
+          <t>21/02/2024</t>
         </is>
       </c>
       <c r="C182" s="2" t="inlineStr">
         <is>
-          <t>25/01/2024</t>
+          <t>26/02/2024</t>
         </is>
       </c>
       <c r="D182" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E182" s="2" t="n">
-        <v>1.87</v>
+        <v>26.13</v>
       </c>
       <c r="F182" s="2" t="inlineStr">
         <is>
-          <t>116/116</t>
+          <t>32/115</t>
         </is>
       </c>
       <c r="G182" s="2" t="n">
-        <v>122.09</v>
+        <v>157.3</v>
       </c>
       <c r="H182" s="2" t="n"/>
     </row>
@@ -6301,27 +6301,27 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>24/01/2024</t>
+          <t>26/02/2024</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>02/02/2024</t>
+          <t>07/03/2024</t>
         </is>
       </c>
       <c r="D183" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E183" s="3" t="n">
-        <v>-1.83</v>
+        <v>-16.67</v>
       </c>
       <c r="F183" s="3" t="inlineStr">
         <is>
-          <t>115/115</t>
+          <t>61/114</t>
         </is>
       </c>
       <c r="G183" s="3" t="n">
-        <v>120.26</v>
+        <v>140.63</v>
       </c>
       <c r="H183" s="3" t="n"/>
     </row>
@@ -6333,27 +6333,27 @@
       </c>
       <c r="B184" s="2" t="inlineStr">
         <is>
-          <t>02/02/2024</t>
+          <t>07/03/2024</t>
         </is>
       </c>
       <c r="C184" s="2" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="D184" s="2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E184" s="2" t="n">
-        <v>7.94</v>
+        <v>41.63</v>
       </c>
       <c r="F184" s="2" t="inlineStr">
         <is>
-          <t>90/116</t>
+          <t>21/115</t>
         </is>
       </c>
       <c r="G184" s="2" t="n">
-        <v>128.2</v>
+        <v>182.27</v>
       </c>
       <c r="H184" s="2" t="n"/>
     </row>
@@ -6365,27 +6365,27 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>21/02/2024</t>
+          <t>27/03/2024</t>
         </is>
       </c>
       <c r="D185" s="3" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>-13.51</v>
+        <v>-36.91</v>
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>74/115</t>
+          <t>18/114</t>
         </is>
       </c>
       <c r="G185" s="3" t="n">
-        <v>114.69</v>
+        <v>145.36</v>
       </c>
       <c r="H185" s="3" t="n"/>
     </row>
@@ -6397,27 +6397,27 @@
       </c>
       <c r="B186" s="2" t="inlineStr">
         <is>
-          <t>21/02/2024</t>
+          <t>27/03/2024</t>
         </is>
       </c>
       <c r="C186" s="2" t="inlineStr">
         <is>
-          <t>26/02/2024</t>
+          <t>05/04/2024</t>
         </is>
       </c>
       <c r="D186" s="2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E186" s="2" t="n">
-        <v>26.13</v>
+        <v>24.47</v>
       </c>
       <c r="F186" s="2" t="inlineStr">
         <is>
-          <t>32/116</t>
+          <t>35/115</t>
         </is>
       </c>
       <c r="G186" s="2" t="n">
-        <v>140.82</v>
+        <v>169.82</v>
       </c>
       <c r="H186" s="2" t="n"/>
     </row>
@@ -6429,27 +6429,27 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>26/02/2024</t>
+          <t>01/04/2024</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>07/03/2024</t>
+          <t>16/04/2024</t>
         </is>
       </c>
       <c r="D187" s="3" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>-16.67</v>
+        <v>-25.3</v>
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>63/115</t>
+          <t>35/114</t>
         </is>
       </c>
       <c r="G187" s="3" t="n">
-        <v>124.15</v>
+        <v>144.53</v>
       </c>
       <c r="H187" s="3" t="n"/>
     </row>
@@ -6461,27 +6461,27 @@
       </c>
       <c r="B188" s="2" t="inlineStr">
         <is>
-          <t>07/03/2024</t>
+          <t>16/04/2024</t>
         </is>
       </c>
       <c r="C188" s="2" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>29/04/2024</t>
         </is>
       </c>
       <c r="D188" s="2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E188" s="2" t="n">
-        <v>41.63</v>
+        <v>24.03</v>
       </c>
       <c r="F188" s="2" t="inlineStr">
         <is>
-          <t>21/116</t>
+          <t>36/115</t>
         </is>
       </c>
       <c r="G188" s="2" t="n">
-        <v>165.79</v>
+        <v>168.55</v>
       </c>
       <c r="H188" s="2" t="n"/>
     </row>
@@ -6493,27 +6493,27 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>23/04/2024</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>27/03/2024</t>
+          <t>03/05/2024</t>
         </is>
       </c>
       <c r="D189" s="3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E189" s="3" t="n">
-        <v>-36.91</v>
+        <v>-11.44</v>
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>19/115</t>
+          <t>82/114</t>
         </is>
       </c>
       <c r="G189" s="3" t="n">
-        <v>128.88</v>
+        <v>157.11</v>
       </c>
       <c r="H189" s="3" t="n"/>
     </row>
@@ -6525,27 +6525,27 @@
       </c>
       <c r="B190" s="2" t="inlineStr">
         <is>
-          <t>27/03/2024</t>
+          <t>03/05/2024</t>
         </is>
       </c>
       <c r="C190" s="2" t="inlineStr">
         <is>
-          <t>05/04/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="D190" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E190" s="2" t="n">
-        <v>24.47</v>
+        <v>69.79000000000001</v>
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>35/116</t>
+          <t>11/115</t>
         </is>
       </c>
       <c r="G190" s="2" t="n">
-        <v>153.34</v>
+        <v>226.91</v>
       </c>
       <c r="H190" s="2" t="n"/>
     </row>
@@ -6557,27 +6557,27 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>16/04/2024</t>
+          <t>20/05/2024</t>
         </is>
       </c>
       <c r="D191" s="3" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>-25.3</v>
+        <v>-40.61</v>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>36/115</t>
+          <t>16/114</t>
         </is>
       </c>
       <c r="G191" s="3" t="n">
-        <v>128.04</v>
+        <v>186.29</v>
       </c>
       <c r="H191" s="3" t="n"/>
     </row>
@@ -6589,27 +6589,27 @@
       </c>
       <c r="B192" s="2" t="inlineStr">
         <is>
-          <t>16/04/2024</t>
+          <t>20/05/2024</t>
         </is>
       </c>
       <c r="C192" s="2" t="inlineStr">
         <is>
-          <t>29/04/2024</t>
+          <t>30/05/2024</t>
         </is>
       </c>
       <c r="D192" s="2" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E192" s="2" t="n">
-        <v>24.03</v>
+        <v>22.93</v>
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>36/116</t>
+          <t>39/115</t>
         </is>
       </c>
       <c r="G192" s="2" t="n">
-        <v>152.07</v>
+        <v>209.23</v>
       </c>
       <c r="H192" s="2" t="n"/>
     </row>
@@ -6621,27 +6621,27 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>23/04/2024</t>
+          <t>30/05/2024</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>03/05/2024</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="D193" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E193" s="3" t="n">
-        <v>-11.44</v>
+        <v>-18.49</v>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>84/115</t>
+          <t>54/114</t>
         </is>
       </c>
       <c r="G193" s="3" t="n">
-        <v>140.63</v>
+        <v>190.74</v>
       </c>
       <c r="H193" s="3" t="n"/>
     </row>
@@ -6653,27 +6653,27 @@
       </c>
       <c r="B194" s="2" t="inlineStr">
         <is>
-          <t>03/05/2024</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="C194" s="2" t="inlineStr">
         <is>
-          <t>10/05/2024</t>
+          <t>24/06/2024</t>
         </is>
       </c>
       <c r="D194" s="2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E194" s="2" t="n">
-        <v>69.79000000000001</v>
+        <v>17.53</v>
       </c>
       <c r="F194" s="2" t="inlineStr">
         <is>
-          <t>11/116</t>
+          <t>48/115</t>
         </is>
       </c>
       <c r="G194" s="2" t="n">
-        <v>210.42</v>
+        <v>208.26</v>
       </c>
       <c r="H194" s="2" t="n"/>
     </row>
@@ -6685,27 +6685,27 @@
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>10/05/2024</t>
+          <t>24/06/2024</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>20/05/2024</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="D195" s="3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E195" s="3" t="n">
-        <v>-40.61</v>
+        <v>-15</v>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>17/115</t>
+          <t>66/114</t>
         </is>
       </c>
       <c r="G195" s="3" t="n">
-        <v>169.81</v>
+        <v>193.26</v>
       </c>
       <c r="H195" s="3" t="n"/>
     </row>
@@ -6717,27 +6717,27 @@
       </c>
       <c r="B196" s="2" t="inlineStr">
         <is>
-          <t>20/05/2024</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="C196" s="2" t="inlineStr">
         <is>
-          <t>30/05/2024</t>
+          <t>12/07/2024</t>
         </is>
       </c>
       <c r="D196" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E196" s="2" t="n">
-        <v>22.93</v>
+        <v>23.84</v>
       </c>
       <c r="F196" s="2" t="inlineStr">
         <is>
-          <t>39/116</t>
+          <t>37/115</t>
         </is>
       </c>
       <c r="G196" s="2" t="n">
-        <v>192.74</v>
+        <v>217.1</v>
       </c>
       <c r="H196" s="2" t="n"/>
     </row>
@@ -6749,27 +6749,27 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>30/05/2024</t>
+          <t>12/07/2024</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>22/07/2024</t>
         </is>
       </c>
       <c r="D197" s="3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>-18.49</v>
+        <v>-25</v>
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>55/115</t>
+          <t>36/114</t>
         </is>
       </c>
       <c r="G197" s="3" t="n">
-        <v>174.26</v>
+        <v>192.1</v>
       </c>
       <c r="H197" s="3" t="n"/>
     </row>
@@ -6781,27 +6781,27 @@
       </c>
       <c r="B198" s="2" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>22/07/2024</t>
         </is>
       </c>
       <c r="C198" s="2" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>25/07/2024</t>
         </is>
       </c>
       <c r="D198" s="2" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E198" s="2" t="n">
-        <v>17.53</v>
+        <v>6.78</v>
       </c>
       <c r="F198" s="2" t="inlineStr">
         <is>
-          <t>47/116</t>
+          <t>94/115</t>
         </is>
       </c>
       <c r="G198" s="2" t="n">
-        <v>191.78</v>
+        <v>198.88</v>
       </c>
       <c r="H198" s="2" t="n"/>
     </row>
@@ -6813,27 +6813,27 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>25/07/2024</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="D199" s="3" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>-15</v>
+        <v>-21.96</v>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>68/115</t>
+          <t>40/114</t>
         </is>
       </c>
       <c r="G199" s="3" t="n">
-        <v>176.78</v>
+        <v>176.92</v>
       </c>
       <c r="H199" s="3" t="n"/>
     </row>
@@ -6845,27 +6845,27 @@
       </c>
       <c r="B200" s="2" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="C200" s="2" t="inlineStr">
         <is>
-          <t>12/07/2024</t>
+          <t>07/08/2024</t>
         </is>
       </c>
       <c r="D200" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E200" s="2" t="n">
-        <v>23.84</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="F200" s="2" t="inlineStr">
         <is>
-          <t>37/116</t>
+          <t>77/115</t>
         </is>
       </c>
       <c r="G200" s="2" t="n">
-        <v>200.62</v>
+        <v>186.79</v>
       </c>
       <c r="H200" s="2" t="n"/>
     </row>
@@ -6877,27 +6877,27 @@
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>12/07/2024</t>
+          <t>07/08/2024</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>22/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D201" s="3" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E201" s="3" t="n">
-        <v>-25</v>
+        <v>-41.02</v>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>37/115</t>
+          <t>14/114</t>
         </is>
       </c>
       <c r="G201" s="3" t="n">
-        <v>175.62</v>
+        <v>145.77</v>
       </c>
       <c r="H201" s="3" t="n"/>
     </row>
@@ -6909,27 +6909,27 @@
       </c>
       <c r="B202" s="2" t="inlineStr">
         <is>
-          <t>22/07/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C202" s="2" t="inlineStr">
         <is>
-          <t>25/07/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="D202" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E202" s="2" t="n">
-        <v>6.78</v>
+        <v>16</v>
       </c>
       <c r="F202" s="2" t="inlineStr">
         <is>
-          <t>94/116</t>
+          <t>54/115</t>
         </is>
       </c>
       <c r="G202" s="2" t="n">
-        <v>182.4</v>
+        <v>161.77</v>
       </c>
       <c r="H202" s="2" t="n"/>
     </row>
@@ -6941,27 +6941,27 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>25/07/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="D203" s="3" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>-21.96</v>
+        <v>-13.79</v>
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>41/115</t>
+          <t>70/114</t>
         </is>
       </c>
       <c r="G203" s="3" t="n">
-        <v>160.44</v>
+        <v>147.98</v>
       </c>
       <c r="H203" s="3" t="n"/>
     </row>
@@ -6973,27 +6973,27 @@
       </c>
       <c r="B204" s="2" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C204" s="2" t="inlineStr">
         <is>
-          <t>07/08/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="D204" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E204" s="2" t="n">
-        <v>9.869999999999999</v>
+        <v>11.34</v>
       </c>
       <c r="F204" s="2" t="inlineStr">
         <is>
-          <t>76/116</t>
+          <t>72/115</t>
         </is>
       </c>
       <c r="G204" s="2" t="n">
-        <v>170.31</v>
+        <v>159.32</v>
       </c>
       <c r="H204" s="2" t="n"/>
     </row>
@@ -7005,27 +7005,27 @@
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>07/08/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="D205" s="3" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E205" s="3" t="n">
-        <v>-41.02</v>
+        <v>-19.44</v>
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>15/115</t>
+          <t>49/114</t>
         </is>
       </c>
       <c r="G205" s="3" t="n">
-        <v>129.29</v>
+        <v>139.87</v>
       </c>
       <c r="H205" s="3" t="n"/>
     </row>
@@ -7037,29 +7037,33 @@
       </c>
       <c r="B206" s="2" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="C206" s="2" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>01/01/2025</t>
         </is>
       </c>
       <c r="D206" s="2" t="n">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E206" s="2" t="n">
-        <v>16</v>
+        <v>84.48</v>
       </c>
       <c r="F206" s="2" t="inlineStr">
         <is>
-          <t>53/116</t>
+          <t>9/115</t>
         </is>
       </c>
       <c r="G206" s="2" t="n">
-        <v>145.29</v>
-      </c>
-      <c r="H206" s="2" t="n"/>
+        <v>224.36</v>
+      </c>
+      <c r="H206" s="2" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="3" t="inlineStr">
@@ -7069,27 +7073,27 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>31/12/2024</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>22/01/2025</t>
         </is>
       </c>
       <c r="D207" s="3" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E207" s="3" t="n">
-        <v>-13.79</v>
+        <v>-23.78</v>
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>72/115</t>
+          <t>38/114</t>
         </is>
       </c>
       <c r="G207" s="3" t="n">
-        <v>131.5</v>
+        <v>200.58</v>
       </c>
       <c r="H207" s="3" t="n"/>
     </row>
@@ -7101,27 +7105,27 @@
       </c>
       <c r="B208" s="2" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>22/01/2025</t>
         </is>
       </c>
       <c r="C208" s="2" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="D208" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E208" s="2" t="n">
-        <v>11.34</v>
+        <v>25</v>
       </c>
       <c r="F208" s="2" t="inlineStr">
         <is>
-          <t>70/116</t>
+          <t>34/115</t>
         </is>
       </c>
       <c r="G208" s="2" t="n">
-        <v>142.84</v>
+        <v>225.58</v>
       </c>
       <c r="H208" s="2" t="n"/>
     </row>
@@ -7133,27 +7137,27 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="D209" s="3" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E209" s="3" t="n">
-        <v>-19.44</v>
+        <v>-29.05</v>
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>50/115</t>
+          <t>26/114</t>
         </is>
       </c>
       <c r="G209" s="3" t="n">
-        <v>123.39</v>
+        <v>196.52</v>
       </c>
       <c r="H209" s="3" t="n"/>
     </row>
@@ -7165,33 +7169,29 @@
       </c>
       <c r="B210" s="2" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="C210" s="2" t="inlineStr">
         <is>
-          <t>01/01/2025</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="D210" s="2" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E210" s="2" t="n">
-        <v>84.48</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="F210" s="2" t="inlineStr">
         <is>
-          <t>8/116</t>
+          <t>81/115</t>
         </is>
       </c>
       <c r="G210" s="2" t="n">
-        <v>207.88</v>
-      </c>
-      <c r="H210" s="2" t="inlineStr">
-        <is>
-          <t>09/12/2024</t>
-        </is>
-      </c>
+        <v>205.72</v>
+      </c>
+      <c r="H210" s="2" t="n"/>
     </row>
     <row r="211">
       <c r="A211" s="3" t="inlineStr">
@@ -7201,27 +7201,27 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>31/12/2024</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>22/01/2025</t>
+          <t>14/02/2025</t>
         </is>
       </c>
       <c r="D211" s="3" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E211" s="3" t="n">
-        <v>-23.78</v>
+        <v>-12.23</v>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>39/115</t>
+          <t>77/114</t>
         </is>
       </c>
       <c r="G211" s="3" t="n">
-        <v>184.1</v>
+        <v>193.5</v>
       </c>
       <c r="H211" s="3" t="n"/>
     </row>
@@ -7233,27 +7233,27 @@
       </c>
       <c r="B212" s="2" t="inlineStr">
         <is>
-          <t>22/01/2025</t>
+          <t>14/02/2025</t>
         </is>
       </c>
       <c r="C212" s="2" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="D212" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E212" s="2" t="n">
-        <v>25</v>
+        <v>26.93</v>
       </c>
       <c r="F212" s="2" t="inlineStr">
         <is>
-          <t>34/116</t>
+          <t>29/115</t>
         </is>
       </c>
       <c r="G212" s="2" t="n">
-        <v>209.1</v>
+        <v>220.43</v>
       </c>
       <c r="H212" s="2" t="n"/>
     </row>
@@ -7265,29 +7265,33 @@
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>13/06/2025</t>
         </is>
       </c>
       <c r="D213" s="3" t="n">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E213" s="3" t="n">
-        <v>-29.05</v>
+        <v>-92.09999999999999</v>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>28/115</t>
+          <t>1/114</t>
         </is>
       </c>
       <c r="G213" s="3" t="n">
-        <v>180.04</v>
-      </c>
-      <c r="H213" s="3" t="n"/>
+        <v>128.33</v>
+      </c>
+      <c r="H213" s="3" t="inlineStr">
+        <is>
+          <t>18/03/2025, 19/03/2025, 20/03/2025, 16/04/2025, 22/04/2025, 23/04/2025, 25/04/2025, 29/04/2025, 30/04/2025, 02/05/2025, 05/05/2025, 07/05/2025, 15/05/2025, 21/05/2025, 13/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="inlineStr">
@@ -7297,27 +7301,27 @@
       </c>
       <c r="B214" s="2" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>13/06/2025</t>
         </is>
       </c>
       <c r="C214" s="2" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>30/06/2025</t>
         </is>
       </c>
       <c r="D214" s="2" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E214" s="2" t="n">
-        <v>9.199999999999999</v>
+        <v>128.4</v>
       </c>
       <c r="F214" s="2" t="inlineStr">
         <is>
-          <t>80/116</t>
+          <t>2/115</t>
         </is>
       </c>
       <c r="G214" s="2" t="n">
-        <v>189.24</v>
+        <v>256.73</v>
       </c>
       <c r="H214" s="2" t="n"/>
     </row>
@@ -7329,27 +7333,27 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>30/06/2025</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>14/07/2025</t>
         </is>
       </c>
       <c r="D215" s="3" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E215" s="3" t="n">
-        <v>-12.23</v>
+        <v>-18.92</v>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>80/115</t>
+          <t>51/114</t>
         </is>
       </c>
       <c r="G215" s="3" t="n">
-        <v>177.01</v>
+        <v>237.81</v>
       </c>
       <c r="H215" s="3" t="n"/>
     </row>
@@ -7361,27 +7365,27 @@
       </c>
       <c r="B216" s="2" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>14/07/2025</t>
         </is>
       </c>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>24/02/2025</t>
+          <t>22/07/2025</t>
         </is>
       </c>
       <c r="D216" s="2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E216" s="2" t="n">
-        <v>26.93</v>
+        <v>96.20999999999999</v>
       </c>
       <c r="F216" s="2" t="inlineStr">
         <is>
-          <t>29/116</t>
+          <t>6/115</t>
         </is>
       </c>
       <c r="G216" s="2" t="n">
-        <v>203.95</v>
+        <v>334.02</v>
       </c>
       <c r="H216" s="2" t="n"/>
     </row>
@@ -7393,33 +7397,29 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>24/02/2025</t>
+          <t>22/07/2025</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>31/07/2025</t>
         </is>
       </c>
       <c r="D217" s="3" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E217" s="3" t="n">
-        <v>-80.12</v>
+        <v>-25.87</v>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>1/115</t>
+          <t>32/114</t>
         </is>
       </c>
       <c r="G217" s="3" t="n">
-        <v>123.83</v>
-      </c>
-      <c r="H217" s="3" t="inlineStr">
-        <is>
-          <t>18/03/2025, 19/03/2025, 20/03/2025</t>
-        </is>
-      </c>
+        <v>308.15</v>
+      </c>
+      <c r="H217" s="3" t="n"/>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">
@@ -7429,27 +7429,27 @@
       </c>
       <c r="B218" s="2" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>31/07/2025</t>
         </is>
       </c>
       <c r="C218" s="2" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>04/08/2025</t>
         </is>
       </c>
       <c r="D218" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E218" s="2" t="n">
-        <v>15.95</v>
+        <v>14.58</v>
       </c>
       <c r="F218" s="2" t="inlineStr">
         <is>
-          <t>54/116</t>
+          <t>61/115</t>
         </is>
       </c>
       <c r="G218" s="2" t="n">
-        <v>139.78</v>
+        <v>322.74</v>
       </c>
       <c r="H218" s="2" t="n"/>
     </row>
@@ -7461,33 +7461,29 @@
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>03/04/2025</t>
+          <t>04/08/2025</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>13/06/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="D219" s="3" t="n">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="E219" s="3" t="n">
-        <v>-65.70999999999999</v>
+        <v>-35.91</v>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>3/115</t>
+          <t>19/114</t>
         </is>
       </c>
       <c r="G219" s="3" t="n">
-        <v>74.06</v>
-      </c>
-      <c r="H219" s="3" t="inlineStr">
-        <is>
-          <t>16/04/2025, 22/04/2025, 23/04/2025, 25/04/2025, 29/04/2025, 30/04/2025, 02/05/2025, 05/05/2025, 07/05/2025, 15/05/2025, 21/05/2025, 13/06/2025</t>
-        </is>
-      </c>
+        <v>286.83</v>
+      </c>
+      <c r="H219" s="3" t="n"/>
     </row>
     <row r="220">
       <c r="A220" s="2" t="inlineStr">
@@ -7497,27 +7493,27 @@
       </c>
       <c r="B220" s="2" t="inlineStr">
         <is>
-          <t>13/06/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="C220" s="2" t="inlineStr">
         <is>
-          <t>30/06/2025</t>
+          <t>28/08/2025</t>
         </is>
       </c>
       <c r="D220" s="2" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E220" s="2" t="n">
-        <v>128.4</v>
+        <v>17.81</v>
       </c>
       <c r="F220" s="2" t="inlineStr">
         <is>
-          <t>2/116</t>
+          <t>47/115</t>
         </is>
       </c>
       <c r="G220" s="2" t="n">
-        <v>202.46</v>
+        <v>304.63</v>
       </c>
       <c r="H220" s="2" t="n"/>
     </row>
@@ -7529,29 +7525,33 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>30/06/2025</t>
+          <t>28/08/2025</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>17/07/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
       <c r="D221" s="3" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E221" s="3" t="n">
-        <v>-18.92</v>
+        <v>-6.4</v>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>52/115</t>
+          <t>101/114</t>
         </is>
       </c>
       <c r="G221" s="3" t="n">
-        <v>183.54</v>
-      </c>
-      <c r="H221" s="3" t="n"/>
+        <v>298.24</v>
+      </c>
+      <c r="H221" s="3" t="inlineStr">
+        <is>
+          <t>03/09/2025</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="inlineStr">
@@ -7561,29 +7561,33 @@
       </c>
       <c r="B222" s="2" t="inlineStr">
         <is>
-          <t>17/07/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
       <c r="C222" s="2" t="inlineStr">
         <is>
-          <t>22/07/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="D222" s="2" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E222" s="2" t="n">
-        <v>83.69</v>
+        <v>170.19</v>
       </c>
       <c r="F222" s="2" t="inlineStr">
         <is>
-          <t>9/116</t>
+          <t>1/115</t>
         </is>
       </c>
       <c r="G222" s="2" t="n">
-        <v>267.23</v>
-      </c>
-      <c r="H222" s="2" t="n"/>
+        <v>468.43</v>
+      </c>
+      <c r="H222" s="2" t="inlineStr">
+        <is>
+          <t>25/09/2025</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="3" t="inlineStr">
@@ -7593,33 +7597,29 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>22/07/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>03/09/2025</t>
+          <t>22/10/2025</t>
         </is>
       </c>
       <c r="D223" s="3" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E223" s="3" t="n">
-        <v>-45.56</v>
+        <v>-32.18</v>
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>9/115</t>
+          <t>25/114</t>
         </is>
       </c>
       <c r="G223" s="3" t="n">
-        <v>221.67</v>
-      </c>
-      <c r="H223" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2025</t>
-        </is>
-      </c>
+        <v>436.24</v>
+      </c>
+      <c r="H223" s="3" t="n"/>
     </row>
     <row r="224">
       <c r="A224" s="2" t="inlineStr">
@@ -7629,33 +7629,29 @@
       </c>
       <c r="B224" s="2" t="inlineStr">
         <is>
-          <t>03/09/2025</t>
+          <t>22/10/2025</t>
         </is>
       </c>
       <c r="C224" s="2" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>31/10/2025</t>
         </is>
       </c>
       <c r="D224" s="2" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E224" s="2" t="n">
-        <v>170.19</v>
+        <v>11.36</v>
       </c>
       <c r="F224" s="2" t="inlineStr">
         <is>
-          <t>1/116</t>
+          <t>71/115</t>
         </is>
       </c>
       <c r="G224" s="2" t="n">
-        <v>391.85</v>
-      </c>
-      <c r="H224" s="2" t="inlineStr">
-        <is>
-          <t>25/09/2025</t>
-        </is>
-      </c>
+        <v>447.61</v>
+      </c>
+      <c r="H224" s="2" t="n"/>
     </row>
     <row r="225">
       <c r="A225" s="3" t="inlineStr">
@@ -7665,29 +7661,33 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>16/10/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="D225" s="3" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E225" s="3" t="n">
-        <v>-32.18</v>
+        <v>-56.56</v>
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>26/115</t>
+          <t>4/114</t>
         </is>
       </c>
       <c r="G225" s="3" t="n">
-        <v>359.67</v>
-      </c>
-      <c r="H225" s="3" t="n"/>
+        <v>391.05</v>
+      </c>
+      <c r="H225" s="3" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="inlineStr">
@@ -7697,29 +7697,33 @@
       </c>
       <c r="B226" s="2" t="inlineStr">
         <is>
-          <t>16/10/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="C226" s="2" t="inlineStr">
         <is>
-          <t>31/10/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="D226" s="2" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E226" s="2" t="n">
-        <v>9.94</v>
+        <v>53.69</v>
       </c>
       <c r="F226" s="2" t="inlineStr">
         <is>
-          <t>73/116</t>
+          <t>14/115</t>
         </is>
       </c>
       <c r="G226" s="2" t="n">
-        <v>369.61</v>
-      </c>
-      <c r="H226" s="2" t="n"/>
+        <v>444.74</v>
+      </c>
+      <c r="H226" s="2" t="inlineStr">
+        <is>
+          <t>26/11/2025</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="3" t="inlineStr">
@@ -7729,33 +7733,29 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="D227" s="3" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E227" s="3" t="n">
-        <v>-56.56</v>
+        <v>-17.03</v>
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>5/115</t>
+          <t>59/114</t>
         </is>
       </c>
       <c r="G227" s="3" t="n">
-        <v>313.05</v>
-      </c>
-      <c r="H227" s="3" t="inlineStr">
-        <is>
-          <t>19/11/2025</t>
-        </is>
-      </c>
+        <v>427.71</v>
+      </c>
+      <c r="H227" s="3" t="n"/>
     </row>
     <row r="228">
       <c r="A228" s="2" t="inlineStr">
@@ -7765,33 +7765,29 @@
       </c>
       <c r="B228" s="2" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="C228" s="2" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>22/12/2025</t>
         </is>
       </c>
       <c r="D228" s="2" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E228" s="2" t="n">
-        <v>53.69</v>
+        <v>10.53</v>
       </c>
       <c r="F228" s="2" t="inlineStr">
         <is>
-          <t>14/116</t>
+          <t>73/115</t>
         </is>
       </c>
       <c r="G228" s="2" t="n">
-        <v>366.74</v>
-      </c>
-      <c r="H228" s="2" t="inlineStr">
-        <is>
-          <t>26/11/2025</t>
-        </is>
-      </c>
+        <v>438.23</v>
+      </c>
+      <c r="H228" s="2" t="n"/>
     </row>
     <row r="229">
       <c r="A229" s="3" t="inlineStr">
@@ -7801,27 +7797,27 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>22/12/2025</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>17/12/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="D229" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E229" s="3" t="n">
-        <v>-17.03</v>
+        <v>-18.1</v>
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>61/115</t>
+          <t>56/114</t>
         </is>
       </c>
       <c r="G229" s="3" t="n">
-        <v>349.71</v>
+        <v>420.14</v>
       </c>
       <c r="H229" s="3" t="n"/>
     </row>
@@ -7833,93 +7829,29 @@
       </c>
       <c r="B230" s="2" t="inlineStr">
         <is>
-          <t>17/12/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="C230" s="2" t="inlineStr">
         <is>
-          <t>22/12/2025</t>
+          <t>04/02/2026</t>
         </is>
       </c>
       <c r="D230" s="2" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E230" s="2" t="n">
-        <v>10.53</v>
+        <v>108.72</v>
       </c>
       <c r="F230" s="2" t="inlineStr">
         <is>
-          <t>71/116</t>
+          <t>4/115</t>
         </is>
       </c>
       <c r="G230" s="2" t="n">
-        <v>360.23</v>
+        <v>528.86</v>
       </c>
       <c r="H230" s="2" t="n"/>
-    </row>
-    <row r="231">
-      <c r="A231" s="3" t="inlineStr">
-        <is>
-          <t>DOWN</t>
-        </is>
-      </c>
-      <c r="B231" s="3" t="inlineStr">
-        <is>
-          <t>22/12/2025</t>
-        </is>
-      </c>
-      <c r="C231" s="3" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="D231" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="E231" s="3" t="n">
-        <v>-18.1</v>
-      </c>
-      <c r="F231" s="3" t="inlineStr">
-        <is>
-          <t>57/115</t>
-        </is>
-      </c>
-      <c r="G231" s="3" t="n">
-        <v>342.14</v>
-      </c>
-      <c r="H231" s="3" t="n"/>
-    </row>
-    <row r="232">
-      <c r="A232" s="2" t="inlineStr">
-        <is>
-          <t>RISE</t>
-        </is>
-      </c>
-      <c r="B232" s="2" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="C232" s="2" t="inlineStr">
-        <is>
-          <t>04/02/2026</t>
-        </is>
-      </c>
-      <c r="D232" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="E232" s="2" t="n">
-        <v>108.72</v>
-      </c>
-      <c r="F232" s="2" t="inlineStr">
-        <is>
-          <t>4/116</t>
-        </is>
-      </c>
-      <c r="G232" s="2" t="n">
-        <v>450.86</v>
-      </c>
-      <c r="H232" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Improve code structure; fix buy and sell order logic
Refactored code for better readability and updated buy/sell order handling logic. Adjusted output data files to reflect new calculations.

- Enhanced `backtest_all_stocks_insider_conviction.py` for improved logic clarity.
- Updated `blne_rise_volatility_analysis.json` with new rise event data.
- Adjusted `blne_rise_events.xlsx` to include updated analysis results.
- Refined insider conviction results in `insider_conviction_all_stocks_results.json`.

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H230"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>23/115</t>
+          <t>23/117</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>13/114</t>
+          <t>12/117</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
@@ -585,7 +585,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>49/115</t>
+          <t>49/117</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
@@ -617,7 +617,7 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>57/114</t>
+          <t>60/117</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>27/115</t>
+          <t>27/117</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
@@ -681,7 +681,7 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>21/114</t>
+          <t>21/117</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
@@ -713,7 +713,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>12/115</t>
+          <t>12/117</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
@@ -745,7 +745,7 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>93/114</t>
+          <t>96/117</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
@@ -777,7 +777,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>67/115</t>
+          <t>68/117</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
@@ -809,7 +809,7 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>11/114</t>
+          <t>10/117</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>102/115</t>
+          <t>104/117</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
@@ -873,7 +873,7 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>79/114</t>
+          <t>83/117</t>
         </is>
       </c>
       <c r="G13" s="3" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>66/115</t>
+          <t>67/117</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
@@ -937,7 +937,7 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>105/114</t>
+          <t>108/117</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>113/115</t>
+          <t>115/117</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>111/114</t>
+          <t>114/117</t>
         </is>
       </c>
       <c r="G17" s="3" t="n">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>20/115</t>
+          <t>20/117</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>37/114</t>
+          <t>38/117</t>
         </is>
       </c>
       <c r="G19" s="3" t="n">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>103/115</t>
+          <t>105/117</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>69/114</t>
+          <t>72/117</t>
         </is>
       </c>
       <c r="G21" s="3" t="n">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>69/115</t>
+          <t>69/117</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>109/114</t>
+          <t>112/117</t>
         </is>
       </c>
       <c r="G23" s="3" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>31/115</t>
+          <t>31/117</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>99/114</t>
+          <t>102/117</t>
         </is>
       </c>
       <c r="G25" s="3" t="n">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>13/115</t>
+          <t>13/117</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>104/114</t>
+          <t>107/117</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>114/115</t>
+          <t>116/117</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>84/114</t>
+          <t>87/117</t>
         </is>
       </c>
       <c r="G29" s="3" t="n">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>100/115</t>
+          <t>101/117</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>112/114</t>
+          <t>115/117</t>
         </is>
       </c>
       <c r="G31" s="3" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>92/115</t>
+          <t>92/117</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>89/114</t>
+          <t>92/117</t>
         </is>
       </c>
       <c r="G33" s="3" t="n">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>74/115</t>
+          <t>73/117</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>65/114</t>
+          <t>68/117</t>
         </is>
       </c>
       <c r="G35" s="3" t="n">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>97/115</t>
+          <t>98/117</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>67/114</t>
+          <t>70/117</t>
         </is>
       </c>
       <c r="G37" s="3" t="n">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>42/115</t>
+          <t>42/117</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>80/114</t>
+          <t>84/117</t>
         </is>
       </c>
       <c r="G39" s="3" t="n">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>89/115</t>
+          <t>89/117</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>98/114</t>
+          <t>101/117</t>
         </is>
       </c>
       <c r="G41" s="3" t="n">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>79/115</t>
+          <t>79/117</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>28/114</t>
+          <t>29/117</t>
         </is>
       </c>
       <c r="G43" s="3" t="n">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>96/115</t>
+          <t>97/117</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>108/114</t>
+          <t>111/117</t>
         </is>
       </c>
       <c r="G45" s="3" t="n">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>106/115</t>
+          <t>108/117</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>76/114</t>
+          <t>80/117</t>
         </is>
       </c>
       <c r="G47" s="3" t="n">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>82/115</t>
+          <t>82/117</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>107/114</t>
+          <t>110/117</t>
         </is>
       </c>
       <c r="G49" s="3" t="n">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>99/115</t>
+          <t>100/117</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>103/114</t>
+          <t>106/117</t>
         </is>
       </c>
       <c r="G51" s="3" t="n">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>104/115</t>
+          <t>106/117</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>97/114</t>
+          <t>100/117</t>
         </is>
       </c>
       <c r="G53" s="3" t="n">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>110/115</t>
+          <t>112/117</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>60/114</t>
+          <t>63/117</t>
         </is>
       </c>
       <c r="G55" s="3" t="n">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>112/115</t>
+          <t>114/117</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>91/114</t>
+          <t>94/117</t>
         </is>
       </c>
       <c r="G57" s="3" t="n">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>101/115</t>
+          <t>102/117</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>74/114</t>
+          <t>77/117</t>
         </is>
       </c>
       <c r="G59" s="3" t="n">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>84/115</t>
+          <t>84/117</t>
         </is>
       </c>
       <c r="G60" s="2" t="n">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>95/114</t>
+          <t>98/117</t>
         </is>
       </c>
       <c r="G61" s="3" t="n">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>87/115</t>
+          <t>87/117</t>
         </is>
       </c>
       <c r="G62" s="2" t="n">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>50/114</t>
+          <t>52/117</t>
         </is>
       </c>
       <c r="G63" s="3" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>83/115</t>
+          <t>83/117</t>
         </is>
       </c>
       <c r="G64" s="2" t="n">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>96/114</t>
+          <t>99/117</t>
         </is>
       </c>
       <c r="G65" s="3" t="n">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>25/115</t>
+          <t>25/117</t>
         </is>
       </c>
       <c r="G66" s="2" t="n">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>75/114</t>
+          <t>79/117</t>
         </is>
       </c>
       <c r="G67" s="3" t="n">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>90/115</t>
+          <t>90/117</t>
         </is>
       </c>
       <c r="G68" s="2" t="n">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>12/114</t>
+          <t>11/117</t>
         </is>
       </c>
       <c r="G69" s="3" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>111/115</t>
+          <t>113/117</t>
         </is>
       </c>
       <c r="G70" s="2" t="n">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>48/114</t>
+          <t>50/117</t>
         </is>
       </c>
       <c r="G71" s="3" t="n">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>33/115</t>
+          <t>33/117</t>
         </is>
       </c>
       <c r="G72" s="2" t="n">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>87/114</t>
+          <t>90/117</t>
         </is>
       </c>
       <c r="G73" s="3" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>59/115</t>
+          <t>59/117</t>
         </is>
       </c>
       <c r="G74" s="2" t="n">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>85/114</t>
+          <t>88/117</t>
         </is>
       </c>
       <c r="G75" s="3" t="n">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>40/115</t>
+          <t>40/117</t>
         </is>
       </c>
       <c r="G76" s="2" t="n">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>106/114</t>
+          <t>109/117</t>
         </is>
       </c>
       <c r="G77" s="3" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>107/115</t>
+          <t>109/117</t>
         </is>
       </c>
       <c r="G78" s="2" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>2/114</t>
+          <t>2/117</t>
         </is>
       </c>
       <c r="G79" s="3" t="n">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>5/115</t>
+          <t>5/117</t>
         </is>
       </c>
       <c r="G80" s="2" t="n">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>90/114</t>
+          <t>93/117</t>
         </is>
       </c>
       <c r="G81" s="3" t="n">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>95/115</t>
+          <t>96/117</t>
         </is>
       </c>
       <c r="G82" s="2" t="n">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>29/114</t>
+          <t>30/117</t>
         </is>
       </c>
       <c r="G83" s="3" t="n">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>38/115</t>
+          <t>38/117</t>
         </is>
       </c>
       <c r="G84" s="2" t="n">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>42/114</t>
+          <t>43/117</t>
         </is>
       </c>
       <c r="G85" s="3" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>64/115</t>
+          <t>65/117</t>
         </is>
       </c>
       <c r="G86" s="2" t="n">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>53/114</t>
+          <t>55/117</t>
         </is>
       </c>
       <c r="G87" s="3" t="n">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>85/115</t>
+          <t>85/117</t>
         </is>
       </c>
       <c r="G88" s="2" t="n">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>45/114</t>
+          <t>47/117</t>
         </is>
       </c>
       <c r="G89" s="3" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>51/115</t>
+          <t>51/117</t>
         </is>
       </c>
       <c r="G90" s="2" t="n">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>86/114</t>
+          <t>89/117</t>
         </is>
       </c>
       <c r="G91" s="3" t="n">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="F92" s="2" t="inlineStr">
         <is>
-          <t>15/115</t>
+          <t>15/117</t>
         </is>
       </c>
       <c r="G92" s="2" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>17/114</t>
+          <t>16/117</t>
         </is>
       </c>
       <c r="G93" s="3" t="n">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>62/115</t>
+          <t>62/117</t>
         </is>
       </c>
       <c r="G94" s="2" t="n">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>100/114</t>
+          <t>103/117</t>
         </is>
       </c>
       <c r="G95" s="3" t="n">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>57/115</t>
+          <t>57/117</t>
         </is>
       </c>
       <c r="G96" s="2" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>102/114</t>
+          <t>105/117</t>
         </is>
       </c>
       <c r="G97" s="3" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>16/115</t>
+          <t>16/117</t>
         </is>
       </c>
       <c r="G98" s="2" t="n">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>46/114</t>
+          <t>48/117</t>
         </is>
       </c>
       <c r="G99" s="3" t="n">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>86/115</t>
+          <t>86/117</t>
         </is>
       </c>
       <c r="G100" s="2" t="n">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>33/114</t>
+          <t>34/117</t>
         </is>
       </c>
       <c r="G101" s="3" t="n">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>3/115</t>
+          <t>3/117</t>
         </is>
       </c>
       <c r="G102" s="2" t="n">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>24/114</t>
+          <t>24/117</t>
         </is>
       </c>
       <c r="G103" s="3" t="n">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>70/115</t>
+          <t>70/117</t>
         </is>
       </c>
       <c r="G104" s="2" t="n">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>71/114</t>
+          <t>74/117</t>
         </is>
       </c>
       <c r="G105" s="3" t="n">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>56/115</t>
+          <t>56/117</t>
         </is>
       </c>
       <c r="G106" s="2" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>39/114</t>
+          <t>40/117</t>
         </is>
       </c>
       <c r="G107" s="3" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>55/115</t>
+          <t>55/117</t>
         </is>
       </c>
       <c r="G108" s="2" t="n">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>92/114</t>
+          <t>95/117</t>
         </is>
       </c>
       <c r="G109" s="3" t="n">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>7/115</t>
+          <t>7/117</t>
         </is>
       </c>
       <c r="G110" s="2" t="n">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>78/114</t>
+          <t>82/117</t>
         </is>
       </c>
       <c r="G111" s="3" t="n">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>93/115</t>
+          <t>93/117</t>
         </is>
       </c>
       <c r="G112" s="2" t="n">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>94/114</t>
+          <t>97/117</t>
         </is>
       </c>
       <c r="G113" s="3" t="n">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>28/115</t>
+          <t>28/117</t>
         </is>
       </c>
       <c r="G114" s="2" t="n">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>110/114</t>
+          <t>113/117</t>
         </is>
       </c>
       <c r="G115" s="3" t="n">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t>26/115</t>
+          <t>26/117</t>
         </is>
       </c>
       <c r="G116" s="2" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>52/114</t>
+          <t>54/117</t>
         </is>
       </c>
       <c r="G117" s="3" t="n">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="F118" s="2" t="inlineStr">
         <is>
-          <t>108/115</t>
+          <t>110/117</t>
         </is>
       </c>
       <c r="G118" s="2" t="n">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>30/114</t>
+          <t>31/117</t>
         </is>
       </c>
       <c r="G119" s="3" t="n">
@@ -4297,7 +4297,7 @@
       </c>
       <c r="F120" s="2" t="inlineStr">
         <is>
-          <t>80/115</t>
+          <t>80/117</t>
         </is>
       </c>
       <c r="G120" s="2" t="n">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>43/114</t>
+          <t>44/117</t>
         </is>
       </c>
       <c r="G121" s="3" t="n">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>53/115</t>
+          <t>53/117</t>
         </is>
       </c>
       <c r="G122" s="2" t="n">
@@ -4393,7 +4393,7 @@
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>88/114</t>
+          <t>91/117</t>
         </is>
       </c>
       <c r="G123" s="3" t="n">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>75/115</t>
+          <t>75/117</t>
         </is>
       </c>
       <c r="G124" s="2" t="n">
@@ -4457,7 +4457,7 @@
       </c>
       <c r="F125" s="3" t="inlineStr">
         <is>
-          <t>23/114</t>
+          <t>23/117</t>
         </is>
       </c>
       <c r="G125" s="3" t="n">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>98/115</t>
+          <t>99/117</t>
         </is>
       </c>
       <c r="G126" s="2" t="n">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>63/114</t>
+          <t>66/117</t>
         </is>
       </c>
       <c r="G127" s="3" t="n">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="F128" s="2" t="inlineStr">
         <is>
-          <t>43/115</t>
+          <t>43/117</t>
         </is>
       </c>
       <c r="G128" s="2" t="n">
@@ -4585,7 +4585,7 @@
       </c>
       <c r="F129" s="3" t="inlineStr">
         <is>
-          <t>6/114</t>
+          <t>5/117</t>
         </is>
       </c>
       <c r="G129" s="3" t="n">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="F130" s="2" t="inlineStr">
         <is>
-          <t>41/115</t>
+          <t>41/117</t>
         </is>
       </c>
       <c r="G130" s="2" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="F131" s="3" t="inlineStr">
         <is>
-          <t>44/114</t>
+          <t>45/117</t>
         </is>
       </c>
       <c r="G131" s="3" t="n">
@@ -4681,7 +4681,7 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>63/115</t>
+          <t>63/117</t>
         </is>
       </c>
       <c r="G132" s="2" t="n">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="F133" s="3" t="inlineStr">
         <is>
-          <t>55/114</t>
+          <t>57/117</t>
         </is>
       </c>
       <c r="G133" s="3" t="n">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>18/115</t>
+          <t>18/117</t>
         </is>
       </c>
       <c r="G134" s="2" t="n">
@@ -4770,22 +4770,22 @@
       </c>
       <c r="C135" s="3" t="inlineStr">
         <is>
-          <t>21/06/2022</t>
+          <t>28/04/2022</t>
         </is>
       </c>
       <c r="D135" s="3" t="n">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="E135" s="3" t="n">
-        <v>-55.56</v>
+        <v>-35.56</v>
       </c>
       <c r="F135" s="3" t="inlineStr">
         <is>
-          <t>5/114</t>
+          <t>20/117</t>
         </is>
       </c>
       <c r="G135" s="3" t="n">
-        <v>171.92</v>
+        <v>191.92</v>
       </c>
       <c r="H135" s="3" t="n"/>
     </row>
@@ -4797,27 +4797,27 @@
       </c>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>21/06/2022</t>
+          <t>28/04/2022</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>24/06/2022</t>
+          <t>02/05/2022</t>
         </is>
       </c>
       <c r="D136" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E136" s="2" t="n">
-        <v>19.16</v>
+        <v>5.13</v>
       </c>
       <c r="F136" s="2" t="inlineStr">
         <is>
-          <t>44/115</t>
+          <t>103/117</t>
         </is>
       </c>
       <c r="G136" s="2" t="n">
-        <v>191.09</v>
+        <v>197.06</v>
       </c>
       <c r="H136" s="2" t="n"/>
     </row>
@@ -4829,27 +4829,27 @@
       </c>
       <c r="B137" s="3" t="inlineStr">
         <is>
-          <t>24/06/2022</t>
+          <t>02/05/2022</t>
         </is>
       </c>
       <c r="C137" s="3" t="inlineStr">
         <is>
-          <t>13/07/2022</t>
+          <t>31/05/2022</t>
         </is>
       </c>
       <c r="D137" s="3" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E137" s="3" t="n">
-        <v>-16.49</v>
+        <v>-31.46</v>
       </c>
       <c r="F137" s="3" t="inlineStr">
         <is>
-          <t>62/114</t>
+          <t>26/117</t>
         </is>
       </c>
       <c r="G137" s="3" t="n">
-        <v>174.6</v>
+        <v>165.59</v>
       </c>
       <c r="H137" s="3" t="n"/>
     </row>
@@ -4861,27 +4861,27 @@
       </c>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>13/07/2022</t>
+          <t>31/05/2022</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr">
         <is>
-          <t>28/07/2022</t>
+          <t>09/06/2022</t>
         </is>
       </c>
       <c r="D138" s="2" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E138" s="2" t="n">
-        <v>11.65</v>
+        <v>7.35</v>
       </c>
       <c r="F138" s="2" t="inlineStr">
         <is>
-          <t>68/115</t>
+          <t>94/117</t>
         </is>
       </c>
       <c r="G138" s="2" t="n">
-        <v>186.25</v>
+        <v>172.94</v>
       </c>
       <c r="H138" s="2" t="n"/>
     </row>
@@ -4893,27 +4893,27 @@
       </c>
       <c r="B139" s="3" t="inlineStr">
         <is>
-          <t>28/07/2022</t>
+          <t>06/06/2022</t>
         </is>
       </c>
       <c r="C139" s="3" t="inlineStr">
         <is>
-          <t>03/08/2022</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="D139" s="3" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>-11.59</v>
+        <v>-17.81</v>
       </c>
       <c r="F139" s="3" t="inlineStr">
         <is>
-          <t>81/114</t>
+          <t>59/117</t>
         </is>
       </c>
       <c r="G139" s="3" t="n">
-        <v>174.66</v>
+        <v>155.14</v>
       </c>
       <c r="H139" s="3" t="n"/>
     </row>
@@ -4925,27 +4925,27 @@
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>03/08/2022</t>
+          <t>21/06/2022</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr">
         <is>
-          <t>05/08/2022</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E140" s="2" t="n">
-        <v>18.03</v>
+        <v>19.16</v>
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>46/115</t>
+          <t>44/117</t>
         </is>
       </c>
       <c r="G140" s="2" t="n">
-        <v>192.69</v>
+        <v>174.3</v>
       </c>
       <c r="H140" s="2" t="n"/>
     </row>
@@ -4957,27 +4957,27 @@
       </c>
       <c r="B141" s="3" t="inlineStr">
         <is>
-          <t>05/08/2022</t>
+          <t>24/06/2022</t>
         </is>
       </c>
       <c r="C141" s="3" t="inlineStr">
         <is>
-          <t>12/09/2022</t>
+          <t>06/07/2022</t>
         </is>
       </c>
       <c r="D141" s="3" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>-47.64</v>
+        <v>-16.35</v>
       </c>
       <c r="F141" s="3" t="inlineStr">
         <is>
-          <t>8/114</t>
+          <t>65/117</t>
         </is>
       </c>
       <c r="G141" s="3" t="n">
-        <v>145.05</v>
+        <v>157.95</v>
       </c>
       <c r="H141" s="3" t="n"/>
     </row>
@@ -4989,27 +4989,27 @@
       </c>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>12/09/2022</t>
+          <t>06/07/2022</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>15/09/2022</t>
+          <t>20/07/2022</t>
         </is>
       </c>
       <c r="D142" s="2" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E142" s="2" t="n">
-        <v>16.88</v>
+        <v>13.09</v>
       </c>
       <c r="F142" s="2" t="inlineStr">
         <is>
-          <t>52/115</t>
+          <t>64/117</t>
         </is>
       </c>
       <c r="G142" s="2" t="n">
-        <v>161.93</v>
+        <v>171.03</v>
       </c>
       <c r="H142" s="2" t="n"/>
     </row>
@@ -5021,27 +5021,27 @@
       </c>
       <c r="B143" s="3" t="inlineStr">
         <is>
-          <t>14/09/2022</t>
+          <t>08/07/2022</t>
         </is>
       </c>
       <c r="C143" s="3" t="inlineStr">
         <is>
-          <t>04/10/2022</t>
+          <t>03/08/2022</t>
         </is>
       </c>
       <c r="D143" s="3" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>-40.89</v>
+        <v>-12.86</v>
       </c>
       <c r="F143" s="3" t="inlineStr">
         <is>
-          <t>15/114</t>
+          <t>78/117</t>
         </is>
       </c>
       <c r="G143" s="3" t="n">
-        <v>121.05</v>
+        <v>158.18</v>
       </c>
       <c r="H143" s="3" t="n"/>
     </row>
@@ -5053,27 +5053,27 @@
       </c>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>04/10/2022</t>
+          <t>03/08/2022</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr">
         <is>
-          <t>06/10/2022</t>
+          <t>05/08/2022</t>
         </is>
       </c>
       <c r="D144" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E144" s="2" t="n">
-        <v>17.18</v>
+        <v>18.03</v>
       </c>
       <c r="F144" s="2" t="inlineStr">
         <is>
-          <t>50/115</t>
+          <t>46/117</t>
         </is>
       </c>
       <c r="G144" s="2" t="n">
-        <v>138.23</v>
+        <v>176.21</v>
       </c>
       <c r="H144" s="2" t="n"/>
     </row>
@@ -5085,27 +5085,27 @@
       </c>
       <c r="B145" s="3" t="inlineStr">
         <is>
-          <t>06/10/2022</t>
+          <t>05/08/2022</t>
         </is>
       </c>
       <c r="C145" s="3" t="inlineStr">
         <is>
-          <t>28/10/2022</t>
+          <t>12/09/2022</t>
         </is>
       </c>
       <c r="D145" s="3" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>-14.96</v>
+        <v>-47.64</v>
       </c>
       <c r="F145" s="3" t="inlineStr">
         <is>
-          <t>68/114</t>
+          <t>7/117</t>
         </is>
       </c>
       <c r="G145" s="3" t="n">
-        <v>123.27</v>
+        <v>128.57</v>
       </c>
       <c r="H145" s="3" t="n"/>
     </row>
@@ -5117,27 +5117,27 @@
       </c>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>28/10/2022</t>
+          <t>12/09/2022</t>
         </is>
       </c>
       <c r="C146" s="2" t="inlineStr">
         <is>
-          <t>01/11/2022</t>
+          <t>15/09/2022</t>
         </is>
       </c>
       <c r="D146" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E146" s="2" t="n">
-        <v>3.96</v>
+        <v>16.88</v>
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>109/115</t>
+          <t>52/117</t>
         </is>
       </c>
       <c r="G146" s="2" t="n">
-        <v>127.23</v>
+        <v>145.45</v>
       </c>
       <c r="H146" s="2" t="n"/>
     </row>
@@ -5149,27 +5149,27 @@
       </c>
       <c r="B147" s="3" t="inlineStr">
         <is>
-          <t>01/11/2022</t>
+          <t>14/09/2022</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>29/12/2022</t>
+          <t>04/10/2022</t>
         </is>
       </c>
       <c r="D147" s="3" t="n">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>-28.57</v>
+        <v>-40.89</v>
       </c>
       <c r="F147" s="3" t="inlineStr">
         <is>
-          <t>27/114</t>
+          <t>14/117</t>
         </is>
       </c>
       <c r="G147" s="3" t="n">
-        <v>98.66</v>
+        <v>104.56</v>
       </c>
       <c r="H147" s="3" t="n"/>
     </row>
@@ -5181,27 +5181,27 @@
       </c>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>29/12/2022</t>
+          <t>04/10/2022</t>
         </is>
       </c>
       <c r="C148" s="2" t="inlineStr">
         <is>
-          <t>11/01/2023</t>
+          <t>06/10/2022</t>
         </is>
       </c>
       <c r="D148" s="2" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E148" s="2" t="n">
-        <v>26.67</v>
+        <v>17.18</v>
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>30/115</t>
+          <t>50/117</t>
         </is>
       </c>
       <c r="G148" s="2" t="n">
-        <v>125.33</v>
+        <v>121.75</v>
       </c>
       <c r="H148" s="2" t="n"/>
     </row>
@@ -5213,27 +5213,27 @@
       </c>
       <c r="B149" s="3" t="inlineStr">
         <is>
-          <t>11/01/2023</t>
+          <t>06/10/2022</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>27/01/2023</t>
+          <t>28/10/2022</t>
         </is>
       </c>
       <c r="D149" s="3" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E149" s="3" t="n">
-        <v>-11.23</v>
+        <v>-14.96</v>
       </c>
       <c r="F149" s="3" t="inlineStr">
         <is>
-          <t>83/114</t>
+          <t>71/117</t>
         </is>
       </c>
       <c r="G149" s="3" t="n">
-        <v>114.1</v>
+        <v>106.79</v>
       </c>
       <c r="H149" s="3" t="n"/>
     </row>
@@ -5245,27 +5245,27 @@
       </c>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>27/01/2023</t>
+          <t>28/10/2022</t>
         </is>
       </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>03/02/2023</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="D150" s="2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E150" s="2" t="n">
-        <v>78.73999999999999</v>
+        <v>3.96</v>
       </c>
       <c r="F150" s="2" t="inlineStr">
         <is>
-          <t>10/115</t>
+          <t>111/117</t>
         </is>
       </c>
       <c r="G150" s="2" t="n">
-        <v>192.84</v>
+        <v>110.75</v>
       </c>
       <c r="H150" s="2" t="n"/>
     </row>
@@ -5277,27 +5277,27 @@
       </c>
       <c r="B151" s="3" t="inlineStr">
         <is>
-          <t>03/02/2023</t>
+          <t>01/11/2022</t>
         </is>
       </c>
       <c r="C151" s="3" t="inlineStr">
         <is>
-          <t>13/02/2023</t>
+          <t>29/12/2022</t>
         </is>
       </c>
       <c r="D151" s="3" t="n">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>-35.9</v>
+        <v>-28.57</v>
       </c>
       <c r="F151" s="3" t="inlineStr">
         <is>
-          <t>20/114</t>
+          <t>28/117</t>
         </is>
       </c>
       <c r="G151" s="3" t="n">
-        <v>156.94</v>
+        <v>82.18000000000001</v>
       </c>
       <c r="H151" s="3" t="n"/>
     </row>
@@ -5309,27 +5309,27 @@
       </c>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>13/02/2023</t>
+          <t>29/12/2022</t>
         </is>
       </c>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>15/02/2023</t>
+          <t>11/01/2023</t>
         </is>
       </c>
       <c r="D152" s="2" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E152" s="2" t="n">
-        <v>14.78</v>
+        <v>26.67</v>
       </c>
       <c r="F152" s="2" t="inlineStr">
         <is>
-          <t>60/115</t>
+          <t>30/117</t>
         </is>
       </c>
       <c r="G152" s="2" t="n">
-        <v>171.71</v>
+        <v>108.85</v>
       </c>
       <c r="H152" s="2" t="n"/>
     </row>
@@ -5341,27 +5341,27 @@
       </c>
       <c r="B153" s="3" t="inlineStr">
         <is>
-          <t>15/02/2023</t>
+          <t>11/01/2023</t>
         </is>
       </c>
       <c r="C153" s="3" t="inlineStr">
         <is>
-          <t>24/02/2023</t>
+          <t>27/01/2023</t>
         </is>
       </c>
       <c r="D153" s="3" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>-20.36</v>
+        <v>-11.23</v>
       </c>
       <c r="F153" s="3" t="inlineStr">
         <is>
-          <t>47/114</t>
+          <t>86/117</t>
         </is>
       </c>
       <c r="G153" s="3" t="n">
-        <v>151.35</v>
+        <v>97.62</v>
       </c>
       <c r="H153" s="3" t="n"/>
     </row>
@@ -5373,27 +5373,27 @@
       </c>
       <c r="B154" s="2" t="inlineStr">
         <is>
-          <t>24/02/2023</t>
+          <t>27/01/2023</t>
         </is>
       </c>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>06/03/2023</t>
+          <t>03/02/2023</t>
         </is>
       </c>
       <c r="D154" s="2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E154" s="2" t="n">
-        <v>9.77</v>
+        <v>78.73999999999999</v>
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>78/115</t>
+          <t>10/117</t>
         </is>
       </c>
       <c r="G154" s="2" t="n">
-        <v>161.13</v>
+        <v>176.36</v>
       </c>
       <c r="H154" s="2" t="n"/>
     </row>
@@ -5405,27 +5405,27 @@
       </c>
       <c r="B155" s="3" t="inlineStr">
         <is>
-          <t>03/03/2023</t>
+          <t>03/02/2023</t>
         </is>
       </c>
       <c r="C155" s="3" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>13/02/2023</t>
         </is>
       </c>
       <c r="D155" s="3" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>-21.58</v>
+        <v>-35.9</v>
       </c>
       <c r="F155" s="3" t="inlineStr">
         <is>
-          <t>41/114</t>
+          <t>19/117</t>
         </is>
       </c>
       <c r="G155" s="3" t="n">
-        <v>139.55</v>
+        <v>140.45</v>
       </c>
       <c r="H155" s="3" t="n"/>
     </row>
@@ -5437,27 +5437,27 @@
       </c>
       <c r="B156" s="2" t="inlineStr">
         <is>
-          <t>20/03/2023</t>
+          <t>13/02/2023</t>
         </is>
       </c>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>31/03/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="D156" s="2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E156" s="2" t="n">
-        <v>52.84</v>
+        <v>14.78</v>
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>17/115</t>
+          <t>60/117</t>
         </is>
       </c>
       <c r="G156" s="2" t="n">
-        <v>192.39</v>
+        <v>155.23</v>
       </c>
       <c r="H156" s="2" t="n"/>
     </row>
@@ -5469,27 +5469,27 @@
       </c>
       <c r="B157" s="3" t="inlineStr">
         <is>
-          <t>31/03/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="C157" s="3" t="inlineStr">
         <is>
-          <t>19/04/2023</t>
+          <t>24/02/2023</t>
         </is>
       </c>
       <c r="D157" s="3" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E157" s="3" t="n">
-        <v>-44</v>
+        <v>-20.36</v>
       </c>
       <c r="F157" s="3" t="inlineStr">
         <is>
-          <t>10/114</t>
+          <t>49/117</t>
         </is>
       </c>
       <c r="G157" s="3" t="n">
-        <v>148.39</v>
+        <v>134.87</v>
       </c>
       <c r="H157" s="3" t="n"/>
     </row>
@@ -5501,27 +5501,27 @@
       </c>
       <c r="B158" s="2" t="inlineStr">
         <is>
-          <t>19/04/2023</t>
+          <t>24/02/2023</t>
         </is>
       </c>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>21/04/2023</t>
+          <t>06/03/2023</t>
         </is>
       </c>
       <c r="D158" s="2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E158" s="2" t="n">
-        <v>4.59</v>
+        <v>9.77</v>
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>105/115</t>
+          <t>78/117</t>
         </is>
       </c>
       <c r="G158" s="2" t="n">
-        <v>152.98</v>
+        <v>144.65</v>
       </c>
       <c r="H158" s="2" t="n"/>
     </row>
@@ -5533,27 +5533,27 @@
       </c>
       <c r="B159" s="3" t="inlineStr">
         <is>
-          <t>21/04/2023</t>
+          <t>03/03/2023</t>
         </is>
       </c>
       <c r="C159" s="3" t="inlineStr">
         <is>
-          <t>05/05/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="D159" s="3" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>-15.61</v>
+        <v>-21.58</v>
       </c>
       <c r="F159" s="3" t="inlineStr">
         <is>
-          <t>64/114</t>
+          <t>42/117</t>
         </is>
       </c>
       <c r="G159" s="3" t="n">
-        <v>137.37</v>
+        <v>123.07</v>
       </c>
       <c r="H159" s="3" t="n"/>
     </row>
@@ -5565,27 +5565,27 @@
       </c>
       <c r="B160" s="2" t="inlineStr">
         <is>
-          <t>05/05/2023</t>
+          <t>20/03/2023</t>
         </is>
       </c>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>15/05/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="D160" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E160" s="2" t="n">
-        <v>38.29</v>
+        <v>52.84</v>
       </c>
       <c r="F160" s="2" t="inlineStr">
         <is>
-          <t>22/115</t>
+          <t>17/117</t>
         </is>
       </c>
       <c r="G160" s="2" t="n">
-        <v>175.66</v>
+        <v>175.91</v>
       </c>
       <c r="H160" s="2" t="n"/>
     </row>
@@ -5597,27 +5597,27 @@
       </c>
       <c r="B161" s="3" t="inlineStr">
         <is>
-          <t>15/05/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="C161" s="3" t="inlineStr">
         <is>
-          <t>18/05/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="D161" s="3" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E161" s="3" t="n">
-        <v>-25.43</v>
+        <v>-44</v>
       </c>
       <c r="F161" s="3" t="inlineStr">
         <is>
-          <t>34/114</t>
+          <t>9/117</t>
         </is>
       </c>
       <c r="G161" s="3" t="n">
-        <v>150.22</v>
+        <v>131.91</v>
       </c>
       <c r="H161" s="3" t="n"/>
     </row>
@@ -5629,27 +5629,27 @@
       </c>
       <c r="B162" s="2" t="inlineStr">
         <is>
-          <t>18/05/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>23/05/2023</t>
+          <t>21/04/2023</t>
         </is>
       </c>
       <c r="D162" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E162" s="2" t="n">
-        <v>19.15</v>
+        <v>4.59</v>
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>45/115</t>
+          <t>107/117</t>
         </is>
       </c>
       <c r="G162" s="2" t="n">
-        <v>169.37</v>
+        <v>136.5</v>
       </c>
       <c r="H162" s="2" t="n"/>
     </row>
@@ -5661,27 +5661,27 @@
       </c>
       <c r="B163" s="3" t="inlineStr">
         <is>
-          <t>23/05/2023</t>
+          <t>21/04/2023</t>
         </is>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
-          <t>08/06/2023</t>
+          <t>05/05/2023</t>
         </is>
       </c>
       <c r="D163" s="3" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>-26.51</v>
+        <v>-15.61</v>
       </c>
       <c r="F163" s="3" t="inlineStr">
         <is>
-          <t>31/114</t>
+          <t>67/117</t>
         </is>
       </c>
       <c r="G163" s="3" t="n">
-        <v>142.86</v>
+        <v>120.89</v>
       </c>
       <c r="H163" s="3" t="n"/>
     </row>
@@ -5693,27 +5693,27 @@
       </c>
       <c r="B164" s="2" t="inlineStr">
         <is>
-          <t>08/06/2023</t>
+          <t>05/05/2023</t>
         </is>
       </c>
       <c r="C164" s="2" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>15/05/2023</t>
         </is>
       </c>
       <c r="D164" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E164" s="2" t="n">
-        <v>87.65000000000001</v>
+        <v>38.29</v>
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>8/115</t>
+          <t>22/117</t>
         </is>
       </c>
       <c r="G164" s="2" t="n">
-        <v>230.51</v>
+        <v>159.18</v>
       </c>
       <c r="H164" s="2" t="n"/>
     </row>
@@ -5725,27 +5725,27 @@
       </c>
       <c r="B165" s="3" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>15/05/2023</t>
         </is>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>18/05/2023</t>
         </is>
       </c>
       <c r="D165" s="3" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>-50.4</v>
+        <v>-25.43</v>
       </c>
       <c r="F165" s="3" t="inlineStr">
         <is>
-          <t>7/114</t>
+          <t>35/117</t>
         </is>
       </c>
       <c r="G165" s="3" t="n">
-        <v>180.11</v>
+        <v>133.74</v>
       </c>
       <c r="H165" s="3" t="n"/>
     </row>
@@ -5757,27 +5757,27 @@
       </c>
       <c r="B166" s="2" t="inlineStr">
         <is>
-          <t>27/06/2023</t>
+          <t>18/05/2023</t>
         </is>
       </c>
       <c r="C166" s="2" t="inlineStr">
         <is>
-          <t>19/07/2023</t>
+          <t>23/05/2023</t>
         </is>
       </c>
       <c r="D166" s="2" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E166" s="2" t="n">
-        <v>9.9</v>
+        <v>19.15</v>
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>76/115</t>
+          <t>45/117</t>
         </is>
       </c>
       <c r="G166" s="2" t="n">
-        <v>190.01</v>
+        <v>152.89</v>
       </c>
       <c r="H166" s="2" t="n"/>
     </row>
@@ -5789,27 +5789,27 @@
       </c>
       <c r="B167" s="3" t="inlineStr">
         <is>
-          <t>10/07/2023</t>
+          <t>23/05/2023</t>
         </is>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
-          <t>28/07/2023</t>
+          <t>08/06/2023</t>
         </is>
       </c>
       <c r="D167" s="3" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E167" s="3" t="n">
-        <v>-13.37</v>
+        <v>-26.51</v>
       </c>
       <c r="F167" s="3" t="inlineStr">
         <is>
-          <t>73/114</t>
+          <t>32/117</t>
         </is>
       </c>
       <c r="G167" s="3" t="n">
-        <v>176.64</v>
+        <v>126.38</v>
       </c>
       <c r="H167" s="3" t="n"/>
     </row>
@@ -5821,27 +5821,27 @@
       </c>
       <c r="B168" s="2" t="inlineStr">
         <is>
-          <t>28/07/2023</t>
+          <t>08/06/2023</t>
         </is>
       </c>
       <c r="C168" s="2" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="D168" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E168" s="2" t="n">
-        <v>12.75</v>
+        <v>87.65000000000001</v>
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>65/115</t>
+          <t>8/117</t>
         </is>
       </c>
       <c r="G168" s="2" t="n">
-        <v>189.39</v>
+        <v>214.03</v>
       </c>
       <c r="H168" s="2" t="n"/>
     </row>
@@ -5853,27 +5853,27 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
-          <t>28/09/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="D169" s="3" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>-62.8</v>
+        <v>-50.4</v>
       </c>
       <c r="F169" s="3" t="inlineStr">
         <is>
-          <t>3/114</t>
+          <t>6/117</t>
         </is>
       </c>
       <c r="G169" s="3" t="n">
-        <v>126.6</v>
+        <v>163.63</v>
       </c>
       <c r="H169" s="3" t="n"/>
     </row>
@@ -5885,27 +5885,27 @@
       </c>
       <c r="B170" s="2" t="inlineStr">
         <is>
-          <t>28/09/2023</t>
+          <t>27/06/2023</t>
         </is>
       </c>
       <c r="C170" s="2" t="inlineStr">
         <is>
-          <t>04/10/2023</t>
+          <t>19/07/2023</t>
         </is>
       </c>
       <c r="D170" s="2" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E170" s="2" t="n">
-        <v>49.6</v>
+        <v>9.9</v>
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>19/115</t>
+          <t>76/117</t>
         </is>
       </c>
       <c r="G170" s="2" t="n">
-        <v>176.2</v>
+        <v>173.53</v>
       </c>
       <c r="H170" s="2" t="n"/>
     </row>
@@ -5917,27 +5917,27 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>04/10/2023</t>
+          <t>10/07/2023</t>
         </is>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
-          <t>09/10/2023</t>
+          <t>28/07/2023</t>
         </is>
       </c>
       <c r="D171" s="3" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>-2.14</v>
+        <v>-13.37</v>
       </c>
       <c r="F171" s="3" t="inlineStr">
         <is>
-          <t>113/114</t>
+          <t>76/117</t>
         </is>
       </c>
       <c r="G171" s="3" t="n">
-        <v>174.06</v>
+        <v>160.16</v>
       </c>
       <c r="H171" s="3" t="n"/>
     </row>
@@ -5949,27 +5949,27 @@
       </c>
       <c r="B172" s="2" t="inlineStr">
         <is>
-          <t>09/10/2023</t>
+          <t>28/07/2023</t>
         </is>
       </c>
       <c r="C172" s="2" t="inlineStr">
         <is>
-          <t>11/10/2023</t>
+          <t>02/08/2023</t>
         </is>
       </c>
       <c r="D172" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E172" s="2" t="n">
-        <v>8.199999999999999</v>
+        <v>12.75</v>
       </c>
       <c r="F172" s="2" t="inlineStr">
         <is>
-          <t>88/115</t>
+          <t>66/117</t>
         </is>
       </c>
       <c r="G172" s="2" t="n">
-        <v>182.25</v>
+        <v>172.91</v>
       </c>
       <c r="H172" s="2" t="n"/>
     </row>
@@ -5981,27 +5981,27 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>11/10/2023</t>
+          <t>02/08/2023</t>
         </is>
       </c>
       <c r="C173" s="3" t="inlineStr">
         <is>
-          <t>27/10/2023</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="D173" s="3" t="n">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>-34.34</v>
+        <v>-62.8</v>
       </c>
       <c r="F173" s="3" t="inlineStr">
         <is>
-          <t>22/114</t>
+          <t>3/117</t>
         </is>
       </c>
       <c r="G173" s="3" t="n">
-        <v>147.91</v>
+        <v>110.11</v>
       </c>
       <c r="H173" s="3" t="n"/>
     </row>
@@ -6013,27 +6013,27 @@
       </c>
       <c r="B174" s="2" t="inlineStr">
         <is>
-          <t>27/10/2023</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="C174" s="2" t="inlineStr">
         <is>
-          <t>31/10/2023</t>
+          <t>04/10/2023</t>
         </is>
       </c>
       <c r="D174" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E174" s="2" t="n">
-        <v>15.6</v>
+        <v>49.6</v>
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>58/115</t>
+          <t>19/117</t>
         </is>
       </c>
       <c r="G174" s="2" t="n">
-        <v>163.51</v>
+        <v>159.71</v>
       </c>
       <c r="H174" s="2" t="n"/>
     </row>
@@ -6045,27 +6045,27 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>31/10/2023</t>
+          <t>04/10/2023</t>
         </is>
       </c>
       <c r="C175" s="3" t="inlineStr">
         <is>
-          <t>27/11/2023</t>
+          <t>09/10/2023</t>
         </is>
       </c>
       <c r="D175" s="3" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>-44.17</v>
+        <v>-2.14</v>
       </c>
       <c r="F175" s="3" t="inlineStr">
         <is>
-          <t>9/114</t>
+          <t>116/117</t>
         </is>
       </c>
       <c r="G175" s="3" t="n">
-        <v>119.34</v>
+        <v>157.57</v>
       </c>
       <c r="H175" s="3" t="n"/>
     </row>
@@ -6077,27 +6077,27 @@
       </c>
       <c r="B176" s="2" t="inlineStr">
         <is>
-          <t>27/11/2023</t>
+          <t>09/10/2023</t>
         </is>
       </c>
       <c r="C176" s="2" t="inlineStr">
         <is>
-          <t>30/11/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="D176" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E176" s="2" t="n">
-        <v>34.74</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>24/115</t>
+          <t>88/117</t>
         </is>
       </c>
       <c r="G176" s="2" t="n">
-        <v>154.08</v>
+        <v>165.77</v>
       </c>
       <c r="H176" s="2" t="n"/>
     </row>
@@ -6109,27 +6109,27 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>28/12/2023</t>
+          <t>11/10/2023</t>
         </is>
       </c>
       <c r="C177" s="3" t="inlineStr">
         <is>
-          <t>22/01/2024</t>
+          <t>27/10/2023</t>
         </is>
       </c>
       <c r="D177" s="3" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>-17.37</v>
+        <v>-34.34</v>
       </c>
       <c r="F177" s="3" t="inlineStr">
         <is>
-          <t>58/114</t>
+          <t>22/117</t>
         </is>
       </c>
       <c r="G177" s="3" t="n">
-        <v>136.7</v>
+        <v>131.43</v>
       </c>
       <c r="H177" s="3" t="n"/>
     </row>
@@ -6141,27 +6141,27 @@
       </c>
       <c r="B178" s="2" t="inlineStr">
         <is>
-          <t>22/01/2024</t>
+          <t>27/10/2023</t>
         </is>
       </c>
       <c r="C178" s="2" t="inlineStr">
         <is>
-          <t>25/01/2024</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D178" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E178" s="2" t="n">
-        <v>1.87</v>
+        <v>15.6</v>
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>115/115</t>
+          <t>58/117</t>
         </is>
       </c>
       <c r="G178" s="2" t="n">
-        <v>138.57</v>
+        <v>147.03</v>
       </c>
       <c r="H178" s="2" t="n"/>
     </row>
@@ -6173,27 +6173,27 @@
       </c>
       <c r="B179" s="3" t="inlineStr">
         <is>
-          <t>24/01/2024</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="C179" s="3" t="inlineStr">
         <is>
-          <t>02/02/2024</t>
+          <t>27/11/2023</t>
         </is>
       </c>
       <c r="D179" s="3" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>-1.83</v>
+        <v>-44.17</v>
       </c>
       <c r="F179" s="3" t="inlineStr">
         <is>
-          <t>114/114</t>
+          <t>8/117</t>
         </is>
       </c>
       <c r="G179" s="3" t="n">
-        <v>136.74</v>
+        <v>102.86</v>
       </c>
       <c r="H179" s="3" t="n"/>
     </row>
@@ -6205,27 +6205,27 @@
       </c>
       <c r="B180" s="2" t="inlineStr">
         <is>
-          <t>02/02/2024</t>
+          <t>27/11/2023</t>
         </is>
       </c>
       <c r="C180" s="2" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>30/11/2023</t>
         </is>
       </c>
       <c r="D180" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E180" s="2" t="n">
-        <v>7.94</v>
+        <v>34.74</v>
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>91/115</t>
+          <t>24/117</t>
         </is>
       </c>
       <c r="G180" s="2" t="n">
-        <v>144.68</v>
+        <v>137.6</v>
       </c>
       <c r="H180" s="2" t="n"/>
     </row>
@@ -6237,27 +6237,27 @@
       </c>
       <c r="B181" s="3" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>28/12/2023</t>
         </is>
       </c>
       <c r="C181" s="3" t="inlineStr">
         <is>
-          <t>21/02/2024</t>
+          <t>22/01/2024</t>
         </is>
       </c>
       <c r="D181" s="3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E181" s="3" t="n">
-        <v>-13.51</v>
+        <v>-17.37</v>
       </c>
       <c r="F181" s="3" t="inlineStr">
         <is>
-          <t>72/114</t>
+          <t>61/117</t>
         </is>
       </c>
       <c r="G181" s="3" t="n">
-        <v>131.17</v>
+        <v>120.22</v>
       </c>
       <c r="H181" s="3" t="n"/>
     </row>
@@ -6269,27 +6269,27 @@
       </c>
       <c r="B182" s="2" t="inlineStr">
         <is>
-          <t>21/02/2024</t>
+          <t>22/01/2024</t>
         </is>
       </c>
       <c r="C182" s="2" t="inlineStr">
         <is>
-          <t>26/02/2024</t>
+          <t>25/01/2024</t>
         </is>
       </c>
       <c r="D182" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E182" s="2" t="n">
-        <v>26.13</v>
+        <v>1.87</v>
       </c>
       <c r="F182" s="2" t="inlineStr">
         <is>
-          <t>32/115</t>
+          <t>117/117</t>
         </is>
       </c>
       <c r="G182" s="2" t="n">
-        <v>157.3</v>
+        <v>122.09</v>
       </c>
       <c r="H182" s="2" t="n"/>
     </row>
@@ -6301,27 +6301,27 @@
       </c>
       <c r="B183" s="3" t="inlineStr">
         <is>
-          <t>26/02/2024</t>
+          <t>24/01/2024</t>
         </is>
       </c>
       <c r="C183" s="3" t="inlineStr">
         <is>
-          <t>07/03/2024</t>
+          <t>02/02/2024</t>
         </is>
       </c>
       <c r="D183" s="3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E183" s="3" t="n">
-        <v>-16.67</v>
+        <v>-1.83</v>
       </c>
       <c r="F183" s="3" t="inlineStr">
         <is>
-          <t>61/114</t>
+          <t>117/117</t>
         </is>
       </c>
       <c r="G183" s="3" t="n">
-        <v>140.63</v>
+        <v>120.26</v>
       </c>
       <c r="H183" s="3" t="n"/>
     </row>
@@ -6333,27 +6333,27 @@
       </c>
       <c r="B184" s="2" t="inlineStr">
         <is>
-          <t>07/03/2024</t>
+          <t>02/02/2024</t>
         </is>
       </c>
       <c r="C184" s="2" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="D184" s="2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E184" s="2" t="n">
-        <v>41.63</v>
+        <v>7.94</v>
       </c>
       <c r="F184" s="2" t="inlineStr">
         <is>
-          <t>21/115</t>
+          <t>91/117</t>
         </is>
       </c>
       <c r="G184" s="2" t="n">
-        <v>182.27</v>
+        <v>128.2</v>
       </c>
       <c r="H184" s="2" t="n"/>
     </row>
@@ -6365,27 +6365,27 @@
       </c>
       <c r="B185" s="3" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="C185" s="3" t="inlineStr">
         <is>
-          <t>27/03/2024</t>
+          <t>21/02/2024</t>
         </is>
       </c>
       <c r="D185" s="3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>-36.91</v>
+        <v>-13.51</v>
       </c>
       <c r="F185" s="3" t="inlineStr">
         <is>
-          <t>18/114</t>
+          <t>75/117</t>
         </is>
       </c>
       <c r="G185" s="3" t="n">
-        <v>145.36</v>
+        <v>114.69</v>
       </c>
       <c r="H185" s="3" t="n"/>
     </row>
@@ -6397,27 +6397,27 @@
       </c>
       <c r="B186" s="2" t="inlineStr">
         <is>
-          <t>27/03/2024</t>
+          <t>21/02/2024</t>
         </is>
       </c>
       <c r="C186" s="2" t="inlineStr">
         <is>
-          <t>05/04/2024</t>
+          <t>26/02/2024</t>
         </is>
       </c>
       <c r="D186" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E186" s="2" t="n">
-        <v>24.47</v>
+        <v>26.13</v>
       </c>
       <c r="F186" s="2" t="inlineStr">
         <is>
-          <t>35/115</t>
+          <t>32/117</t>
         </is>
       </c>
       <c r="G186" s="2" t="n">
-        <v>169.82</v>
+        <v>140.82</v>
       </c>
       <c r="H186" s="2" t="n"/>
     </row>
@@ -6429,27 +6429,27 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
+          <t>26/02/2024</t>
         </is>
       </c>
       <c r="C187" s="3" t="inlineStr">
         <is>
-          <t>16/04/2024</t>
+          <t>07/03/2024</t>
         </is>
       </c>
       <c r="D187" s="3" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>-25.3</v>
+        <v>-16.67</v>
       </c>
       <c r="F187" s="3" t="inlineStr">
         <is>
-          <t>35/114</t>
+          <t>64/117</t>
         </is>
       </c>
       <c r="G187" s="3" t="n">
-        <v>144.53</v>
+        <v>124.15</v>
       </c>
       <c r="H187" s="3" t="n"/>
     </row>
@@ -6461,27 +6461,27 @@
       </c>
       <c r="B188" s="2" t="inlineStr">
         <is>
-          <t>16/04/2024</t>
+          <t>07/03/2024</t>
         </is>
       </c>
       <c r="C188" s="2" t="inlineStr">
         <is>
-          <t>29/04/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="D188" s="2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E188" s="2" t="n">
-        <v>24.03</v>
+        <v>41.63</v>
       </c>
       <c r="F188" s="2" t="inlineStr">
         <is>
-          <t>36/115</t>
+          <t>21/117</t>
         </is>
       </c>
       <c r="G188" s="2" t="n">
-        <v>168.55</v>
+        <v>165.79</v>
       </c>
       <c r="H188" s="2" t="n"/>
     </row>
@@ -6493,27 +6493,27 @@
       </c>
       <c r="B189" s="3" t="inlineStr">
         <is>
-          <t>23/04/2024</t>
+          <t>19/03/2024</t>
         </is>
       </c>
       <c r="C189" s="3" t="inlineStr">
         <is>
-          <t>03/05/2024</t>
+          <t>27/03/2024</t>
         </is>
       </c>
       <c r="D189" s="3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E189" s="3" t="n">
-        <v>-11.44</v>
+        <v>-36.91</v>
       </c>
       <c r="F189" s="3" t="inlineStr">
         <is>
-          <t>82/114</t>
+          <t>17/117</t>
         </is>
       </c>
       <c r="G189" s="3" t="n">
-        <v>157.11</v>
+        <v>128.88</v>
       </c>
       <c r="H189" s="3" t="n"/>
     </row>
@@ -6525,27 +6525,27 @@
       </c>
       <c r="B190" s="2" t="inlineStr">
         <is>
-          <t>03/05/2024</t>
+          <t>27/03/2024</t>
         </is>
       </c>
       <c r="C190" s="2" t="inlineStr">
         <is>
-          <t>10/05/2024</t>
+          <t>05/04/2024</t>
         </is>
       </c>
       <c r="D190" s="2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E190" s="2" t="n">
-        <v>69.79000000000001</v>
+        <v>24.47</v>
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>11/115</t>
+          <t>35/117</t>
         </is>
       </c>
       <c r="G190" s="2" t="n">
-        <v>226.91</v>
+        <v>153.34</v>
       </c>
       <c r="H190" s="2" t="n"/>
     </row>
@@ -6557,27 +6557,27 @@
       </c>
       <c r="B191" s="3" t="inlineStr">
         <is>
-          <t>10/05/2024</t>
+          <t>01/04/2024</t>
         </is>
       </c>
       <c r="C191" s="3" t="inlineStr">
         <is>
-          <t>20/05/2024</t>
+          <t>16/04/2024</t>
         </is>
       </c>
       <c r="D191" s="3" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>-40.61</v>
+        <v>-25.3</v>
       </c>
       <c r="F191" s="3" t="inlineStr">
         <is>
-          <t>16/114</t>
+          <t>36/117</t>
         </is>
       </c>
       <c r="G191" s="3" t="n">
-        <v>186.29</v>
+        <v>128.04</v>
       </c>
       <c r="H191" s="3" t="n"/>
     </row>
@@ -6589,27 +6589,27 @@
       </c>
       <c r="B192" s="2" t="inlineStr">
         <is>
-          <t>20/05/2024</t>
+          <t>16/04/2024</t>
         </is>
       </c>
       <c r="C192" s="2" t="inlineStr">
         <is>
-          <t>30/05/2024</t>
+          <t>29/04/2024</t>
         </is>
       </c>
       <c r="D192" s="2" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E192" s="2" t="n">
-        <v>22.93</v>
+        <v>24.03</v>
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>39/115</t>
+          <t>36/117</t>
         </is>
       </c>
       <c r="G192" s="2" t="n">
-        <v>209.23</v>
+        <v>152.07</v>
       </c>
       <c r="H192" s="2" t="n"/>
     </row>
@@ -6621,27 +6621,27 @@
       </c>
       <c r="B193" s="3" t="inlineStr">
         <is>
-          <t>30/05/2024</t>
+          <t>23/04/2024</t>
         </is>
       </c>
       <c r="C193" s="3" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>03/05/2024</t>
         </is>
       </c>
       <c r="D193" s="3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E193" s="3" t="n">
-        <v>-18.49</v>
+        <v>-11.44</v>
       </c>
       <c r="F193" s="3" t="inlineStr">
         <is>
-          <t>54/114</t>
+          <t>85/117</t>
         </is>
       </c>
       <c r="G193" s="3" t="n">
-        <v>190.74</v>
+        <v>140.63</v>
       </c>
       <c r="H193" s="3" t="n"/>
     </row>
@@ -6653,27 +6653,27 @@
       </c>
       <c r="B194" s="2" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>03/05/2024</t>
         </is>
       </c>
       <c r="C194" s="2" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="D194" s="2" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E194" s="2" t="n">
-        <v>17.53</v>
+        <v>69.79000000000001</v>
       </c>
       <c r="F194" s="2" t="inlineStr">
         <is>
-          <t>48/115</t>
+          <t>11/117</t>
         </is>
       </c>
       <c r="G194" s="2" t="n">
-        <v>208.26</v>
+        <v>210.42</v>
       </c>
       <c r="H194" s="2" t="n"/>
     </row>
@@ -6685,27 +6685,27 @@
       </c>
       <c r="B195" s="3" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="C195" s="3" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>20/05/2024</t>
         </is>
       </c>
       <c r="D195" s="3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E195" s="3" t="n">
-        <v>-15</v>
+        <v>-40.61</v>
       </c>
       <c r="F195" s="3" t="inlineStr">
         <is>
-          <t>66/114</t>
+          <t>15/117</t>
         </is>
       </c>
       <c r="G195" s="3" t="n">
-        <v>193.26</v>
+        <v>169.81</v>
       </c>
       <c r="H195" s="3" t="n"/>
     </row>
@@ -6717,27 +6717,27 @@
       </c>
       <c r="B196" s="2" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>20/05/2024</t>
         </is>
       </c>
       <c r="C196" s="2" t="inlineStr">
         <is>
-          <t>12/07/2024</t>
+          <t>30/05/2024</t>
         </is>
       </c>
       <c r="D196" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E196" s="2" t="n">
-        <v>23.84</v>
+        <v>22.93</v>
       </c>
       <c r="F196" s="2" t="inlineStr">
         <is>
-          <t>37/115</t>
+          <t>39/117</t>
         </is>
       </c>
       <c r="G196" s="2" t="n">
-        <v>217.1</v>
+        <v>192.74</v>
       </c>
       <c r="H196" s="2" t="n"/>
     </row>
@@ -6749,27 +6749,27 @@
       </c>
       <c r="B197" s="3" t="inlineStr">
         <is>
-          <t>12/07/2024</t>
+          <t>30/05/2024</t>
         </is>
       </c>
       <c r="C197" s="3" t="inlineStr">
         <is>
-          <t>22/07/2024</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="D197" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>-25</v>
+        <v>-18.49</v>
       </c>
       <c r="F197" s="3" t="inlineStr">
         <is>
-          <t>36/114</t>
+          <t>56/117</t>
         </is>
       </c>
       <c r="G197" s="3" t="n">
-        <v>192.1</v>
+        <v>174.26</v>
       </c>
       <c r="H197" s="3" t="n"/>
     </row>
@@ -6781,27 +6781,27 @@
       </c>
       <c r="B198" s="2" t="inlineStr">
         <is>
-          <t>22/07/2024</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="C198" s="2" t="inlineStr">
         <is>
-          <t>25/07/2024</t>
+          <t>24/06/2024</t>
         </is>
       </c>
       <c r="D198" s="2" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E198" s="2" t="n">
-        <v>6.78</v>
+        <v>17.53</v>
       </c>
       <c r="F198" s="2" t="inlineStr">
         <is>
-          <t>94/115</t>
+          <t>48/117</t>
         </is>
       </c>
       <c r="G198" s="2" t="n">
-        <v>198.88</v>
+        <v>191.78</v>
       </c>
       <c r="H198" s="2" t="n"/>
     </row>
@@ -6813,27 +6813,27 @@
       </c>
       <c r="B199" s="3" t="inlineStr">
         <is>
-          <t>25/07/2024</t>
+          <t>24/06/2024</t>
         </is>
       </c>
       <c r="C199" s="3" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="D199" s="3" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>-21.96</v>
+        <v>-15</v>
       </c>
       <c r="F199" s="3" t="inlineStr">
         <is>
-          <t>40/114</t>
+          <t>69/117</t>
         </is>
       </c>
       <c r="G199" s="3" t="n">
-        <v>176.92</v>
+        <v>176.78</v>
       </c>
       <c r="H199" s="3" t="n"/>
     </row>
@@ -6845,27 +6845,27 @@
       </c>
       <c r="B200" s="2" t="inlineStr">
         <is>
-          <t>05/08/2024</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="C200" s="2" t="inlineStr">
         <is>
-          <t>07/08/2024</t>
+          <t>12/07/2024</t>
         </is>
       </c>
       <c r="D200" s="2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E200" s="2" t="n">
-        <v>9.869999999999999</v>
+        <v>23.84</v>
       </c>
       <c r="F200" s="2" t="inlineStr">
         <is>
-          <t>77/115</t>
+          <t>37/117</t>
         </is>
       </c>
       <c r="G200" s="2" t="n">
-        <v>186.79</v>
+        <v>200.62</v>
       </c>
       <c r="H200" s="2" t="n"/>
     </row>
@@ -6877,27 +6877,27 @@
       </c>
       <c r="B201" s="3" t="inlineStr">
         <is>
-          <t>07/08/2024</t>
+          <t>12/07/2024</t>
         </is>
       </c>
       <c r="C201" s="3" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>22/07/2024</t>
         </is>
       </c>
       <c r="D201" s="3" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E201" s="3" t="n">
-        <v>-41.02</v>
+        <v>-25</v>
       </c>
       <c r="F201" s="3" t="inlineStr">
         <is>
-          <t>14/114</t>
+          <t>37/117</t>
         </is>
       </c>
       <c r="G201" s="3" t="n">
-        <v>145.77</v>
+        <v>175.62</v>
       </c>
       <c r="H201" s="3" t="n"/>
     </row>
@@ -6909,27 +6909,27 @@
       </c>
       <c r="B202" s="2" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>22/07/2024</t>
         </is>
       </c>
       <c r="C202" s="2" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>25/07/2024</t>
         </is>
       </c>
       <c r="D202" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E202" s="2" t="n">
-        <v>16</v>
+        <v>6.78</v>
       </c>
       <c r="F202" s="2" t="inlineStr">
         <is>
-          <t>54/115</t>
+          <t>95/117</t>
         </is>
       </c>
       <c r="G202" s="2" t="n">
-        <v>161.77</v>
+        <v>182.4</v>
       </c>
       <c r="H202" s="2" t="n"/>
     </row>
@@ -6941,27 +6941,27 @@
       </c>
       <c r="B203" s="3" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>25/07/2024</t>
         </is>
       </c>
       <c r="C203" s="3" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="D203" s="3" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>-13.79</v>
+        <v>-21.96</v>
       </c>
       <c r="F203" s="3" t="inlineStr">
         <is>
-          <t>70/114</t>
+          <t>41/117</t>
         </is>
       </c>
       <c r="G203" s="3" t="n">
-        <v>147.98</v>
+        <v>160.44</v>
       </c>
       <c r="H203" s="3" t="n"/>
     </row>
@@ -6973,27 +6973,27 @@
       </c>
       <c r="B204" s="2" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>05/08/2024</t>
         </is>
       </c>
       <c r="C204" s="2" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>07/08/2024</t>
         </is>
       </c>
       <c r="D204" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E204" s="2" t="n">
-        <v>11.34</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="F204" s="2" t="inlineStr">
         <is>
-          <t>72/115</t>
+          <t>77/117</t>
         </is>
       </c>
       <c r="G204" s="2" t="n">
-        <v>159.32</v>
+        <v>170.31</v>
       </c>
       <c r="H204" s="2" t="n"/>
     </row>
@@ -7005,27 +7005,27 @@
       </c>
       <c r="B205" s="3" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>07/08/2024</t>
         </is>
       </c>
       <c r="C205" s="3" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="D205" s="3" t="n">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E205" s="3" t="n">
-        <v>-19.44</v>
+        <v>-41.02</v>
       </c>
       <c r="F205" s="3" t="inlineStr">
         <is>
-          <t>49/114</t>
+          <t>13/117</t>
         </is>
       </c>
       <c r="G205" s="3" t="n">
-        <v>139.87</v>
+        <v>129.29</v>
       </c>
       <c r="H205" s="3" t="n"/>
     </row>
@@ -7037,33 +7037,29 @@
       </c>
       <c r="B206" s="2" t="inlineStr">
         <is>
-          <t>05/11/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C206" s="2" t="inlineStr">
         <is>
-          <t>01/01/2025</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="D206" s="2" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E206" s="2" t="n">
-        <v>84.48</v>
+        <v>16</v>
       </c>
       <c r="F206" s="2" t="inlineStr">
         <is>
-          <t>9/115</t>
+          <t>54/117</t>
         </is>
       </c>
       <c r="G206" s="2" t="n">
-        <v>224.36</v>
-      </c>
-      <c r="H206" s="2" t="inlineStr">
-        <is>
-          <t>09/12/2024</t>
-        </is>
-      </c>
+        <v>145.29</v>
+      </c>
+      <c r="H206" s="2" t="n"/>
     </row>
     <row r="207">
       <c r="A207" s="3" t="inlineStr">
@@ -7073,27 +7069,27 @@
       </c>
       <c r="B207" s="3" t="inlineStr">
         <is>
-          <t>31/12/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C207" s="3" t="inlineStr">
         <is>
-          <t>22/01/2025</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="D207" s="3" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E207" s="3" t="n">
-        <v>-23.78</v>
+        <v>-13.79</v>
       </c>
       <c r="F207" s="3" t="inlineStr">
         <is>
-          <t>38/114</t>
+          <t>73/117</t>
         </is>
       </c>
       <c r="G207" s="3" t="n">
-        <v>200.58</v>
+        <v>131.5</v>
       </c>
       <c r="H207" s="3" t="n"/>
     </row>
@@ -7105,27 +7101,27 @@
       </c>
       <c r="B208" s="2" t="inlineStr">
         <is>
-          <t>22/01/2025</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C208" s="2" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="D208" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E208" s="2" t="n">
-        <v>25</v>
+        <v>11.34</v>
       </c>
       <c r="F208" s="2" t="inlineStr">
         <is>
-          <t>34/115</t>
+          <t>71/117</t>
         </is>
       </c>
       <c r="G208" s="2" t="n">
-        <v>225.58</v>
+        <v>142.84</v>
       </c>
       <c r="H208" s="2" t="n"/>
     </row>
@@ -7137,27 +7133,27 @@
       </c>
       <c r="B209" s="3" t="inlineStr">
         <is>
-          <t>27/01/2025</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C209" s="3" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="D209" s="3" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E209" s="3" t="n">
-        <v>-29.05</v>
+        <v>-19.44</v>
       </c>
       <c r="F209" s="3" t="inlineStr">
         <is>
-          <t>26/114</t>
+          <t>51/117</t>
         </is>
       </c>
       <c r="G209" s="3" t="n">
-        <v>196.52</v>
+        <v>123.39</v>
       </c>
       <c r="H209" s="3" t="n"/>
     </row>
@@ -7169,29 +7165,33 @@
       </c>
       <c r="B210" s="2" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>05/11/2024</t>
         </is>
       </c>
       <c r="C210" s="2" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>01/01/2025</t>
         </is>
       </c>
       <c r="D210" s="2" t="n">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E210" s="2" t="n">
-        <v>9.199999999999999</v>
+        <v>84.48</v>
       </c>
       <c r="F210" s="2" t="inlineStr">
         <is>
-          <t>81/115</t>
+          <t>9/117</t>
         </is>
       </c>
       <c r="G210" s="2" t="n">
-        <v>205.72</v>
-      </c>
-      <c r="H210" s="2" t="n"/>
+        <v>207.88</v>
+      </c>
+      <c r="H210" s="2" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="3" t="inlineStr">
@@ -7201,27 +7201,27 @@
       </c>
       <c r="B211" s="3" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>31/12/2024</t>
         </is>
       </c>
       <c r="C211" s="3" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>22/01/2025</t>
         </is>
       </c>
       <c r="D211" s="3" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E211" s="3" t="n">
-        <v>-12.23</v>
+        <v>-23.78</v>
       </c>
       <c r="F211" s="3" t="inlineStr">
         <is>
-          <t>77/114</t>
+          <t>39/117</t>
         </is>
       </c>
       <c r="G211" s="3" t="n">
-        <v>193.5</v>
+        <v>184.1</v>
       </c>
       <c r="H211" s="3" t="n"/>
     </row>
@@ -7233,27 +7233,27 @@
       </c>
       <c r="B212" s="2" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>22/01/2025</t>
         </is>
       </c>
       <c r="C212" s="2" t="inlineStr">
         <is>
-          <t>24/02/2025</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="D212" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E212" s="2" t="n">
-        <v>26.93</v>
+        <v>25</v>
       </c>
       <c r="F212" s="2" t="inlineStr">
         <is>
-          <t>29/115</t>
+          <t>34/117</t>
         </is>
       </c>
       <c r="G212" s="2" t="n">
-        <v>220.43</v>
+        <v>209.1</v>
       </c>
       <c r="H212" s="2" t="n"/>
     </row>
@@ -7265,33 +7265,29 @@
       </c>
       <c r="B213" s="3" t="inlineStr">
         <is>
-          <t>24/02/2025</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="C213" s="3" t="inlineStr">
         <is>
-          <t>13/06/2025</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="D213" s="3" t="n">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="E213" s="3" t="n">
-        <v>-92.09999999999999</v>
+        <v>-29.05</v>
       </c>
       <c r="F213" s="3" t="inlineStr">
         <is>
-          <t>1/114</t>
+          <t>27/117</t>
         </is>
       </c>
       <c r="G213" s="3" t="n">
-        <v>128.33</v>
-      </c>
-      <c r="H213" s="3" t="inlineStr">
-        <is>
-          <t>18/03/2025, 19/03/2025, 20/03/2025, 16/04/2025, 22/04/2025, 23/04/2025, 25/04/2025, 29/04/2025, 30/04/2025, 02/05/2025, 05/05/2025, 07/05/2025, 15/05/2025, 21/05/2025, 13/06/2025</t>
-        </is>
-      </c>
+        <v>180.04</v>
+      </c>
+      <c r="H213" s="3" t="n"/>
     </row>
     <row r="214">
       <c r="A214" s="2" t="inlineStr">
@@ -7301,27 +7297,27 @@
       </c>
       <c r="B214" s="2" t="inlineStr">
         <is>
-          <t>13/06/2025</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="C214" s="2" t="inlineStr">
         <is>
-          <t>30/06/2025</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="D214" s="2" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E214" s="2" t="n">
-        <v>128.4</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="F214" s="2" t="inlineStr">
         <is>
-          <t>2/115</t>
+          <t>81/117</t>
         </is>
       </c>
       <c r="G214" s="2" t="n">
-        <v>256.73</v>
+        <v>189.24</v>
       </c>
       <c r="H214" s="2" t="n"/>
     </row>
@@ -7333,27 +7329,27 @@
       </c>
       <c r="B215" s="3" t="inlineStr">
         <is>
-          <t>30/06/2025</t>
+          <t>06/02/2025</t>
         </is>
       </c>
       <c r="C215" s="3" t="inlineStr">
         <is>
-          <t>14/07/2025</t>
+          <t>14/02/2025</t>
         </is>
       </c>
       <c r="D215" s="3" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E215" s="3" t="n">
-        <v>-18.92</v>
+        <v>-12.23</v>
       </c>
       <c r="F215" s="3" t="inlineStr">
         <is>
-          <t>51/114</t>
+          <t>81/117</t>
         </is>
       </c>
       <c r="G215" s="3" t="n">
-        <v>237.81</v>
+        <v>177.01</v>
       </c>
       <c r="H215" s="3" t="n"/>
     </row>
@@ -7365,27 +7361,27 @@
       </c>
       <c r="B216" s="2" t="inlineStr">
         <is>
-          <t>14/07/2025</t>
+          <t>14/02/2025</t>
         </is>
       </c>
       <c r="C216" s="2" t="inlineStr">
         <is>
-          <t>22/07/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="D216" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E216" s="2" t="n">
-        <v>96.20999999999999</v>
+        <v>26.93</v>
       </c>
       <c r="F216" s="2" t="inlineStr">
         <is>
-          <t>6/115</t>
+          <t>29/117</t>
         </is>
       </c>
       <c r="G216" s="2" t="n">
-        <v>334.02</v>
+        <v>203.95</v>
       </c>
       <c r="H216" s="2" t="n"/>
     </row>
@@ -7397,29 +7393,33 @@
       </c>
       <c r="B217" s="3" t="inlineStr">
         <is>
-          <t>22/07/2025</t>
+          <t>24/02/2025</t>
         </is>
       </c>
       <c r="C217" s="3" t="inlineStr">
         <is>
-          <t>31/07/2025</t>
+          <t>13/06/2025</t>
         </is>
       </c>
       <c r="D217" s="3" t="n">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="E217" s="3" t="n">
-        <v>-25.87</v>
+        <v>-92.09999999999999</v>
       </c>
       <c r="F217" s="3" t="inlineStr">
         <is>
-          <t>32/114</t>
+          <t>1/117</t>
         </is>
       </c>
       <c r="G217" s="3" t="n">
-        <v>308.15</v>
-      </c>
-      <c r="H217" s="3" t="n"/>
+        <v>111.85</v>
+      </c>
+      <c r="H217" s="3" t="inlineStr">
+        <is>
+          <t>18/03/2025, 19/03/2025, 20/03/2025, 16/04/2025, 22/04/2025, 23/04/2025, 25/04/2025, 29/04/2025, 30/04/2025, 02/05/2025, 05/05/2025, 07/05/2025, 15/05/2025, 21/05/2025, 13/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">
@@ -7429,27 +7429,27 @@
       </c>
       <c r="B218" s="2" t="inlineStr">
         <is>
-          <t>31/07/2025</t>
+          <t>13/06/2025</t>
         </is>
       </c>
       <c r="C218" s="2" t="inlineStr">
         <is>
-          <t>04/08/2025</t>
+          <t>30/06/2025</t>
         </is>
       </c>
       <c r="D218" s="2" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E218" s="2" t="n">
-        <v>14.58</v>
+        <v>128.4</v>
       </c>
       <c r="F218" s="2" t="inlineStr">
         <is>
-          <t>61/115</t>
+          <t>2/117</t>
         </is>
       </c>
       <c r="G218" s="2" t="n">
-        <v>322.74</v>
+        <v>240.25</v>
       </c>
       <c r="H218" s="2" t="n"/>
     </row>
@@ -7461,27 +7461,27 @@
       </c>
       <c r="B219" s="3" t="inlineStr">
         <is>
-          <t>04/08/2025</t>
+          <t>30/06/2025</t>
         </is>
       </c>
       <c r="C219" s="3" t="inlineStr">
         <is>
-          <t>26/08/2025</t>
+          <t>14/07/2025</t>
         </is>
       </c>
       <c r="D219" s="3" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E219" s="3" t="n">
-        <v>-35.91</v>
+        <v>-18.92</v>
       </c>
       <c r="F219" s="3" t="inlineStr">
         <is>
-          <t>19/114</t>
+          <t>53/117</t>
         </is>
       </c>
       <c r="G219" s="3" t="n">
-        <v>286.83</v>
+        <v>221.33</v>
       </c>
       <c r="H219" s="3" t="n"/>
     </row>
@@ -7493,27 +7493,27 @@
       </c>
       <c r="B220" s="2" t="inlineStr">
         <is>
-          <t>26/08/2025</t>
+          <t>14/07/2025</t>
         </is>
       </c>
       <c r="C220" s="2" t="inlineStr">
         <is>
-          <t>28/08/2025</t>
+          <t>22/07/2025</t>
         </is>
       </c>
       <c r="D220" s="2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E220" s="2" t="n">
-        <v>17.81</v>
+        <v>96.20999999999999</v>
       </c>
       <c r="F220" s="2" t="inlineStr">
         <is>
-          <t>47/115</t>
+          <t>6/117</t>
         </is>
       </c>
       <c r="G220" s="2" t="n">
-        <v>304.63</v>
+        <v>317.54</v>
       </c>
       <c r="H220" s="2" t="n"/>
     </row>
@@ -7525,33 +7525,29 @@
       </c>
       <c r="B221" s="3" t="inlineStr">
         <is>
-          <t>28/08/2025</t>
+          <t>22/07/2025</t>
         </is>
       </c>
       <c r="C221" s="3" t="inlineStr">
         <is>
-          <t>03/09/2025</t>
+          <t>31/07/2025</t>
         </is>
       </c>
       <c r="D221" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E221" s="3" t="n">
-        <v>-6.4</v>
+        <v>-25.87</v>
       </c>
       <c r="F221" s="3" t="inlineStr">
         <is>
-          <t>101/114</t>
+          <t>33/117</t>
         </is>
       </c>
       <c r="G221" s="3" t="n">
-        <v>298.24</v>
-      </c>
-      <c r="H221" s="3" t="inlineStr">
-        <is>
-          <t>03/09/2025</t>
-        </is>
-      </c>
+        <v>291.67</v>
+      </c>
+      <c r="H221" s="3" t="n"/>
     </row>
     <row r="222">
       <c r="A222" s="2" t="inlineStr">
@@ -7561,33 +7557,29 @@
       </c>
       <c r="B222" s="2" t="inlineStr">
         <is>
-          <t>03/09/2025</t>
+          <t>31/07/2025</t>
         </is>
       </c>
       <c r="C222" s="2" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>04/08/2025</t>
         </is>
       </c>
       <c r="D222" s="2" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E222" s="2" t="n">
-        <v>170.19</v>
+        <v>14.58</v>
       </c>
       <c r="F222" s="2" t="inlineStr">
         <is>
-          <t>1/115</t>
+          <t>61/117</t>
         </is>
       </c>
       <c r="G222" s="2" t="n">
-        <v>468.43</v>
-      </c>
-      <c r="H222" s="2" t="inlineStr">
-        <is>
-          <t>25/09/2025</t>
-        </is>
-      </c>
+        <v>306.25</v>
+      </c>
+      <c r="H222" s="2" t="n"/>
     </row>
     <row r="223">
       <c r="A223" s="3" t="inlineStr">
@@ -7597,27 +7589,27 @@
       </c>
       <c r="B223" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>04/08/2025</t>
         </is>
       </c>
       <c r="C223" s="3" t="inlineStr">
         <is>
-          <t>22/10/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="D223" s="3" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E223" s="3" t="n">
-        <v>-32.18</v>
+        <v>-35.91</v>
       </c>
       <c r="F223" s="3" t="inlineStr">
         <is>
-          <t>25/114</t>
+          <t>18/117</t>
         </is>
       </c>
       <c r="G223" s="3" t="n">
-        <v>436.24</v>
+        <v>270.35</v>
       </c>
       <c r="H223" s="3" t="n"/>
     </row>
@@ -7629,27 +7621,27 @@
       </c>
       <c r="B224" s="2" t="inlineStr">
         <is>
-          <t>22/10/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="C224" s="2" t="inlineStr">
         <is>
-          <t>31/10/2025</t>
+          <t>28/08/2025</t>
         </is>
       </c>
       <c r="D224" s="2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E224" s="2" t="n">
-        <v>11.36</v>
+        <v>17.81</v>
       </c>
       <c r="F224" s="2" t="inlineStr">
         <is>
-          <t>71/115</t>
+          <t>47/117</t>
         </is>
       </c>
       <c r="G224" s="2" t="n">
-        <v>447.61</v>
+        <v>288.15</v>
       </c>
       <c r="H224" s="2" t="n"/>
     </row>
@@ -7661,31 +7653,31 @@
       </c>
       <c r="B225" s="3" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>28/08/2025</t>
         </is>
       </c>
       <c r="C225" s="3" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
       <c r="D225" s="3" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E225" s="3" t="n">
-        <v>-56.56</v>
+        <v>-6.4</v>
       </c>
       <c r="F225" s="3" t="inlineStr">
         <is>
-          <t>4/114</t>
+          <t>104/117</t>
         </is>
       </c>
       <c r="G225" s="3" t="n">
-        <v>391.05</v>
+        <v>281.76</v>
       </c>
       <c r="H225" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
     </row>
@@ -7697,31 +7689,31 @@
       </c>
       <c r="B226" s="2" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
       <c r="C226" s="2" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="D226" s="2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E226" s="2" t="n">
-        <v>53.69</v>
+        <v>170.19</v>
       </c>
       <c r="F226" s="2" t="inlineStr">
         <is>
-          <t>14/115</t>
+          <t>1/117</t>
         </is>
       </c>
       <c r="G226" s="2" t="n">
-        <v>444.74</v>
+        <v>451.94</v>
       </c>
       <c r="H226" s="2" t="inlineStr">
         <is>
-          <t>26/11/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
     </row>
@@ -7733,27 +7725,27 @@
       </c>
       <c r="B227" s="3" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="C227" s="3" t="inlineStr">
         <is>
-          <t>17/12/2025</t>
+          <t>16/10/2025</t>
         </is>
       </c>
       <c r="D227" s="3" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E227" s="3" t="n">
-        <v>-17.03</v>
+        <v>-32.18</v>
       </c>
       <c r="F227" s="3" t="inlineStr">
         <is>
-          <t>59/114</t>
+          <t>25/117</t>
         </is>
       </c>
       <c r="G227" s="3" t="n">
-        <v>427.71</v>
+        <v>419.76</v>
       </c>
       <c r="H227" s="3" t="n"/>
     </row>
@@ -7765,27 +7757,27 @@
       </c>
       <c r="B228" s="2" t="inlineStr">
         <is>
-          <t>17/12/2025</t>
+          <t>16/10/2025</t>
         </is>
       </c>
       <c r="C228" s="2" t="inlineStr">
         <is>
-          <t>22/12/2025</t>
+          <t>31/10/2025</t>
         </is>
       </c>
       <c r="D228" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E228" s="2" t="n">
-        <v>10.53</v>
+        <v>9.94</v>
       </c>
       <c r="F228" s="2" t="inlineStr">
         <is>
-          <t>73/115</t>
+          <t>74/117</t>
         </is>
       </c>
       <c r="G228" s="2" t="n">
-        <v>438.23</v>
+        <v>429.7</v>
       </c>
       <c r="H228" s="2" t="n"/>
     </row>
@@ -7797,29 +7789,33 @@
       </c>
       <c r="B229" s="3" t="inlineStr">
         <is>
-          <t>22/12/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="C229" s="3" t="inlineStr">
         <is>
-          <t>31/12/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="D229" s="3" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E229" s="3" t="n">
-        <v>-18.1</v>
+        <v>-56.56</v>
       </c>
       <c r="F229" s="3" t="inlineStr">
         <is>
-          <t>56/114</t>
+          <t>4/117</t>
         </is>
       </c>
       <c r="G229" s="3" t="n">
-        <v>420.14</v>
-      </c>
-      <c r="H229" s="3" t="n"/>
+        <v>373.14</v>
+      </c>
+      <c r="H229" s="3" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="inlineStr">
@@ -7829,29 +7825,189 @@
       </c>
       <c r="B230" s="2" t="inlineStr">
         <is>
+          <t>20/11/2025</t>
+        </is>
+      </c>
+      <c r="C230" s="2" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="D230" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E230" s="2" t="n">
+        <v>53.69</v>
+      </c>
+      <c r="F230" s="2" t="inlineStr">
+        <is>
+          <t>14/117</t>
+        </is>
+      </c>
+      <c r="G230" s="2" t="n">
+        <v>426.83</v>
+      </c>
+      <c r="H230" s="2" t="n"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B231" s="3" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="C231" s="3" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="D231" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E231" s="3" t="n">
+        <v>-17.03</v>
+      </c>
+      <c r="F231" s="3" t="inlineStr">
+        <is>
+          <t>62/117</t>
+        </is>
+      </c>
+      <c r="G231" s="3" t="n">
+        <v>409.8</v>
+      </c>
+      <c r="H231" s="3" t="n"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B232" s="2" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="C232" s="2" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="D232" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E232" s="2" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="F232" s="2" t="inlineStr">
+        <is>
+          <t>72/117</t>
+        </is>
+      </c>
+      <c r="G232" s="2" t="n">
+        <v>420.32</v>
+      </c>
+      <c r="H232" s="2" t="n"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B233" s="3" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="C233" s="3" t="inlineStr">
+        <is>
           <t>31/12/2025</t>
         </is>
       </c>
-      <c r="C230" s="2" t="inlineStr">
+      <c r="D233" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E233" s="3" t="n">
+        <v>-18.1</v>
+      </c>
+      <c r="F233" s="3" t="inlineStr">
+        <is>
+          <t>58/117</t>
+        </is>
+      </c>
+      <c r="G233" s="3" t="n">
+        <v>402.23</v>
+      </c>
+      <c r="H233" s="3" t="n"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="2" t="inlineStr">
+        <is>
+          <t>RISE</t>
+        </is>
+      </c>
+      <c r="B234" s="2" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="C234" s="2" t="inlineStr">
         <is>
           <t>04/02/2026</t>
         </is>
       </c>
-      <c r="D230" s="2" t="n">
+      <c r="D234" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="E230" s="2" t="n">
+      <c r="E234" s="2" t="n">
         <v>108.72</v>
       </c>
-      <c r="F230" s="2" t="inlineStr">
-        <is>
-          <t>4/115</t>
-        </is>
-      </c>
-      <c r="G230" s="2" t="n">
-        <v>528.86</v>
-      </c>
-      <c r="H230" s="2" t="n"/>
+      <c r="F234" s="2" t="inlineStr">
+        <is>
+          <t>4/117</t>
+        </is>
+      </c>
+      <c r="G234" s="2" t="n">
+        <v>510.95</v>
+      </c>
+      <c r="H234" s="2" t="n"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="3" t="inlineStr">
+        <is>
+          <t>DOWN</t>
+        </is>
+      </c>
+      <c r="B235" s="3" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="C235" s="3" t="inlineStr">
+        <is>
+          <t>11/02/2026</t>
+        </is>
+      </c>
+      <c r="D235" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E235" s="3" t="n">
+        <v>-20.61</v>
+      </c>
+      <c r="F235" s="3" t="inlineStr">
+        <is>
+          <t>46/117</t>
+        </is>
+      </c>
+      <c r="G235" s="3" t="n">
+        <v>490.34</v>
+      </c>
+      <c r="H235" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Test confirmed working for single stock, data updated
Updated output files and backtest script to reflect new results for single stock analysis. Adjustments made to data and logic for improved accuracy.

- Updated `blne_rise_events.xlsx` with latest rise event data
- Modified `blne_rise_volatility_analysis.json` to include insider details
- Adjusted `insider_conviction_all_stocks_results.json` with updated trade stats
- Deleted temporary file `~$blne_rise_events.xlsx`
- Refined `backtest_all_stocks_insider_conviction.py` for single stock testing

============================================================
  FEATURE LABELS
============================================================

# POC_tests
</commit_message>
<xml_diff>
--- a/output CSVs/blne_rise_events.xlsx
+++ b/output CSVs/blne_rise_events.xlsx
@@ -7847,7 +7847,11 @@
       <c r="G230" s="2" t="n">
         <v>426.83</v>
       </c>
-      <c r="H230" s="2" t="n"/>
+      <c r="H230" s="2" t="inlineStr">
+        <is>
+          <t>26/11/2025</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="3" t="inlineStr">

</xml_diff>